<commit_message>
Added RFE results for Logistic Regression with MinMaxScaler and Original Data & LASSO/RIDGE with OR+Stand and OHE+MinMax
</commit_message>
<xml_diff>
--- a/ML_Excel_ReportResults.xlsx
+++ b/ML_Excel_ReportResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveeduisegiunl-my.sharepoint.com/personal/20240502_novaims_unl_pt/Documents/MDSAA-DS_1ºAno/1º Semestre/2_Machine Learning_[ML]/[ML]_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1061" documentId="8_{617E8CF7-4F71-4121-97E1-8CD89EF3D5D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{122EF5B8-9229-451D-8860-F5CEFC7E2D56}"/>
+  <xr:revisionPtr revIDLastSave="1157" documentId="8_{617E8CF7-4F71-4121-97E1-8CD89EF3D5D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{938F1076-8701-4486-AB8C-AEFCECFA3E8F}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B50C4AD8-7853-4F6B-84A1-47D583CD2B87}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="233">
   <si>
     <t>Wrapper Methods | RFE</t>
   </si>
@@ -1135,6 +1135,9 @@
   <si>
     <t>JUSTIFICATION</t>
   </si>
+  <si>
+    <t>100 iterations</t>
+  </si>
 </sst>
 </file>
 
@@ -1143,7 +1146,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1245,6 +1248,12 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="15">
@@ -1622,7 +1631,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1751,6 +1760,29 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1775,6 +1807,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1783,6 +1824,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -1817,54 +1861,6 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1966,23 +1962,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>6350</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>73585</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>57872</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>107</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>2070</xdr:rowOff>
+      <xdr:colOff>2734834</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>21123</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55CA3FF3-156C-F804-68F8-FF3E446D2EDB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CEE7689-E1ED-19CF-2453-8386274F9749}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1998,95 +1994,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6358792" y="7018215"/>
-          <a:ext cx="2748680" cy="728413"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>48522</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>122763</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>2637040</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>8401</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD6451FF-E5B3-77B1-A979-F70487EDA1C6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:srcRect/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6400964" y="8600013"/>
-          <a:ext cx="2588518" cy="1534196"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>171451</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>2619376</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>83798</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F71D94C4-0741-88CB-B2C4-201716B2FF8F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6496050" y="7839076"/>
-          <a:ext cx="2476501" cy="455272"/>
+          <a:off x="9180950" y="7252910"/>
+          <a:ext cx="2658074" cy="695944"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2098,59 +2007,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>73585</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>5604</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>2734834</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>142503</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CEE7689-E1ED-19CF-2453-8386274F9749}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9178364" y="6897222"/>
-          <a:ext cx="2661249" cy="681131"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>28762</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>128868</xdr:rowOff>
+      <xdr:colOff>25587</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>4313</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2736664</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>56919</xdr:rowOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>140937</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2166,15 +2031,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9133541" y="7737662"/>
-          <a:ext cx="2707902" cy="465933"/>
+          <a:off x="9132952" y="8115217"/>
+          <a:ext cx="2707902" cy="499795"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2187,14 +2052,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>40719</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>71901</xdr:rowOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>136869</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2697285</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>4600</xdr:rowOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>50518</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2210,14 +2075,273 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:srcRect/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9148084" y="8797292"/>
+          <a:ext cx="2653391" cy="1559032"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>63012</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>2304</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2620642</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>88897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31EE4208-818F-2655-4D97-541FE18F5F70}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:srcRect/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6416747" y="8507569"/>
+          <a:ext cx="2560805" cy="1517771"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>83828</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>10735</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2705855</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>153280</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98E33750-8CB5-4B94-A735-5FDF82E9928D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:srcRect/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6437563" y="7081647"/>
+          <a:ext cx="2622027" cy="680427"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>132736</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>142820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2629828</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>96975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9967D9D5-8BBB-447E-A540-437D5A877628}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
         <a:srcRect/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9148084" y="8549151"/>
-          <a:ext cx="2656566" cy="1581257"/>
+          <a:off x="6486471" y="7930908"/>
+          <a:ext cx="2497092" cy="492038"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>83829</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>1533</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2702681</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>124009</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{968BED48-A83A-A592-1404-4B5ABDEDD9DB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:srcRect/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3680917" y="7072445"/>
+          <a:ext cx="2618852" cy="657183"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>108885</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>60886</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2583704</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>159335</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C75145EF-40CB-106F-2037-D5CE0E6ED42C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3705973" y="7848974"/>
+          <a:ext cx="2471644" cy="460212"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>53301</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>21094</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2601406</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>86166</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6737415E-9414-591F-8F0F-D75E03A78148}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:srcRect/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3650389" y="8347065"/>
+          <a:ext cx="2551280" cy="1502600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2227,10 +2351,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2617,10 +2737,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.89999084444715716"/>
   </sheetPr>
-  <dimension ref="B3:F36"/>
+  <dimension ref="B3:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2631,29 +2751,29 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
+      <c r="B3" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
     </row>
     <row r="4" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
     </row>
     <row r="5" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="27"/>
-      <c r="C5" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
+      <c r="C5" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
     </row>
     <row r="6" spans="2:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="3" t="s">
@@ -2676,8 +2796,11 @@
       <c r="B7" t="s">
         <v>7</v>
       </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
       <c r="D7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
@@ -2687,6 +2810,9 @@
       <c r="B8" t="s">
         <v>8</v>
       </c>
+      <c r="C8" t="b">
+        <v>1</v>
+      </c>
       <c r="D8" t="b">
         <v>0</v>
       </c>
@@ -2698,8 +2824,11 @@
       <c r="B9" t="s">
         <v>9</v>
       </c>
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
       <c r="D9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" t="b">
         <v>1</v>
@@ -2709,6 +2838,9 @@
       <c r="B10" t="s">
         <v>10</v>
       </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
       <c r="D10" t="b">
         <v>1</v>
       </c>
@@ -2720,6 +2852,9 @@
       <c r="B11" t="s">
         <v>11</v>
       </c>
+      <c r="C11" t="b">
+        <v>1</v>
+      </c>
       <c r="D11" t="b">
         <v>1</v>
       </c>
@@ -2731,6 +2866,9 @@
       <c r="B12" t="s">
         <v>12</v>
       </c>
+      <c r="C12" t="b">
+        <v>0</v>
+      </c>
       <c r="D12" t="b">
         <v>1</v>
       </c>
@@ -2742,6 +2880,9 @@
       <c r="B13" t="s">
         <v>13</v>
       </c>
+      <c r="C13" t="b">
+        <v>0</v>
+      </c>
       <c r="D13" t="b">
         <v>0</v>
       </c>
@@ -2753,8 +2894,11 @@
       <c r="B14" t="s">
         <v>14</v>
       </c>
+      <c r="C14" t="b">
+        <v>1</v>
+      </c>
       <c r="D14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" t="b">
         <v>1</v>
@@ -2764,10 +2908,13 @@
       <c r="B15" t="s">
         <v>15</v>
       </c>
+      <c r="C15" t="b">
+        <v>0</v>
+      </c>
       <c r="D15" t="b">
         <v>0</v>
       </c>
-      <c r="E15" s="89" t="b">
+      <c r="E15" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2775,6 +2922,9 @@
       <c r="B16" t="s">
         <v>16</v>
       </c>
+      <c r="C16" t="b">
+        <v>0</v>
+      </c>
       <c r="D16" t="b">
         <v>1</v>
       </c>
@@ -2786,6 +2936,9 @@
       <c r="B17" t="s">
         <v>17</v>
       </c>
+      <c r="C17" t="b">
+        <v>1</v>
+      </c>
       <c r="D17" t="b">
         <v>1</v>
       </c>
@@ -2797,7 +2950,10 @@
       <c r="B18" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="88" t="b">
+      <c r="C18" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="57" t="b">
         <v>0</v>
       </c>
       <c r="E18" t="b">
@@ -2808,6 +2964,9 @@
       <c r="B19" t="s">
         <v>19</v>
       </c>
+      <c r="C19" t="b">
+        <v>1</v>
+      </c>
       <c r="D19" t="b">
         <v>0</v>
       </c>
@@ -2819,6 +2978,9 @@
       <c r="B20" t="s">
         <v>20</v>
       </c>
+      <c r="C20" t="b">
+        <v>0</v>
+      </c>
       <c r="D20" t="b">
         <v>0</v>
       </c>
@@ -2830,6 +2992,9 @@
       <c r="B21" t="s">
         <v>21</v>
       </c>
+      <c r="C21" t="b">
+        <v>0</v>
+      </c>
       <c r="D21" t="b">
         <v>1</v>
       </c>
@@ -2841,6 +3006,9 @@
       <c r="B22" t="s">
         <v>22</v>
       </c>
+      <c r="C22" t="b">
+        <v>1</v>
+      </c>
       <c r="D22" t="b">
         <v>1</v>
       </c>
@@ -2852,6 +3020,9 @@
       <c r="B23" t="s">
         <v>23</v>
       </c>
+      <c r="C23" t="b">
+        <v>0</v>
+      </c>
       <c r="D23" t="b">
         <v>1</v>
       </c>
@@ -2863,8 +3034,11 @@
       <c r="B24" t="s">
         <v>24</v>
       </c>
+      <c r="C24" t="b">
+        <v>0</v>
+      </c>
       <c r="D24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24" t="b">
         <v>1</v>
@@ -2874,8 +3048,11 @@
       <c r="B25" t="s">
         <v>25</v>
       </c>
+      <c r="C25" t="b">
+        <v>1</v>
+      </c>
       <c r="D25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25" t="b">
         <v>1</v>
@@ -2885,8 +3062,11 @@
       <c r="B26" t="s">
         <v>26</v>
       </c>
+      <c r="C26" t="b">
+        <v>0</v>
+      </c>
       <c r="D26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26" t="b">
         <v>1</v>
@@ -2896,6 +3076,9 @@
       <c r="B27" t="s">
         <v>27</v>
       </c>
+      <c r="C27" t="b">
+        <v>1</v>
+      </c>
       <c r="D27" t="b">
         <v>1</v>
       </c>
@@ -2907,6 +3090,9 @@
       <c r="B28" t="s">
         <v>28</v>
       </c>
+      <c r="C28" t="b">
+        <v>0</v>
+      </c>
       <c r="D28" t="b">
         <v>1</v>
       </c>
@@ -2918,6 +3104,9 @@
       <c r="B29" t="s">
         <v>29</v>
       </c>
+      <c r="C29" t="b">
+        <v>1</v>
+      </c>
       <c r="D29" t="b">
         <v>1</v>
       </c>
@@ -2929,6 +3118,9 @@
       <c r="B30" t="s">
         <v>30</v>
       </c>
+      <c r="C30" t="b">
+        <v>1</v>
+      </c>
       <c r="D30" t="b">
         <v>1</v>
       </c>
@@ -2940,6 +3132,9 @@
       <c r="B31" t="s">
         <v>31</v>
       </c>
+      <c r="C31" t="b">
+        <v>1</v>
+      </c>
       <c r="D31" t="b">
         <v>1</v>
       </c>
@@ -2951,8 +3146,11 @@
       <c r="B32" t="s">
         <v>32</v>
       </c>
+      <c r="C32" t="b">
+        <v>0</v>
+      </c>
       <c r="D32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E32" t="b">
         <v>1</v>
@@ -2962,6 +3160,9 @@
       <c r="B33" t="s">
         <v>33</v>
       </c>
+      <c r="C33" t="b">
+        <v>1</v>
+      </c>
       <c r="D33" t="b">
         <v>1</v>
       </c>
@@ -2973,6 +3174,9 @@
       <c r="B34" t="s">
         <v>34</v>
       </c>
+      <c r="C34" t="b">
+        <v>0</v>
+      </c>
       <c r="D34" t="b">
         <v>1</v>
       </c>
@@ -2984,6 +3188,9 @@
       <c r="B35" t="s">
         <v>35</v>
       </c>
+      <c r="C35" t="b">
+        <v>1</v>
+      </c>
       <c r="D35" t="b">
         <v>1</v>
       </c>
@@ -2995,7 +3202,9 @@
       <c r="B36" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="28"/>
+      <c r="C36" s="28" t="b">
+        <v>1</v>
+      </c>
       <c r="D36" s="28" t="b">
         <v>1</v>
       </c>
@@ -3003,6 +3212,23 @@
         <v>1</v>
       </c>
       <c r="F36" s="2"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C38" s="60" t="s">
+        <v>232</v>
+      </c>
+      <c r="D38" s="60" t="s">
+        <v>232</v>
+      </c>
+      <c r="E38" s="60" t="s">
+        <v>232</v>
+      </c>
+      <c r="F38" s="60" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="59" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D59" s="60"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B7:C36">
@@ -3012,6 +3238,7 @@
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="B3:F4"/>
   </mergeCells>
+  <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="C7:F36">
     <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C7)))</formula>
@@ -3033,7 +3260,7 @@
   <dimension ref="B3:O128"/>
   <sheetViews>
     <sheetView zoomScale="83" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:G35"/>
+      <selection activeCell="J3" sqref="J3:O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3050,67 +3277,67 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="54" t="s">
+      <c r="J3" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="54"/>
+      <c r="K3" s="67"/>
+      <c r="L3" s="67"/>
+      <c r="M3" s="67"/>
+      <c r="N3" s="67"/>
+      <c r="O3" s="67"/>
     </row>
     <row r="4" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="55"/>
-      <c r="M4" s="55"/>
-      <c r="N4" s="55"/>
-      <c r="O4" s="55"/>
+      <c r="J4" s="68"/>
+      <c r="K4" s="68"/>
+      <c r="L4" s="68"/>
+      <c r="M4" s="68"/>
+      <c r="N4" s="68"/>
+      <c r="O4" s="68"/>
     </row>
     <row r="5" spans="2:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="52" t="s">
+      <c r="C5" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="53"/>
-      <c r="E5" s="52" t="s">
+      <c r="D5" s="66"/>
+      <c r="E5" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="53"/>
+      <c r="F5" s="66"/>
       <c r="G5" s="45" t="s">
         <v>41</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="52" t="s">
+      <c r="K5" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="L5" s="53"/>
-      <c r="M5" s="52" t="s">
+      <c r="L5" s="66"/>
+      <c r="M5" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="N5" s="53"/>
+      <c r="N5" s="66"/>
       <c r="O5" s="3" t="s">
         <v>41</v>
       </c>
@@ -8839,24 +9066,24 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="72" t="s">
         <v>154</v>
       </c>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
     </row>
     <row r="4" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
     </row>
     <row r="5" spans="2:9" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="18"/>
@@ -8889,7 +9116,7 @@
       <c r="C6" s="13">
         <v>1</v>
       </c>
-      <c r="D6" s="70">
+      <c r="D6" s="48">
         <v>0</v>
       </c>
       <c r="E6" s="13"/>
@@ -8907,7 +9134,7 @@
       <c r="C7" s="13">
         <v>1</v>
       </c>
-      <c r="D7" s="70">
+      <c r="D7" s="48">
         <v>0</v>
       </c>
       <c r="E7" s="13"/>
@@ -8925,7 +9152,7 @@
       <c r="C8" s="13">
         <v>1</v>
       </c>
-      <c r="D8" s="70">
+      <c r="D8" s="48">
         <v>0</v>
       </c>
       <c r="E8" s="13"/>
@@ -8943,7 +9170,7 @@
       <c r="C9" s="13">
         <v>1</v>
       </c>
-      <c r="D9" s="70">
+      <c r="D9" s="48">
         <v>1</v>
       </c>
       <c r="E9" s="13"/>
@@ -8959,7 +9186,7 @@
       <c r="C10" s="13">
         <v>1</v>
       </c>
-      <c r="D10" s="70">
+      <c r="D10" s="48">
         <v>0</v>
       </c>
       <c r="E10" s="13"/>
@@ -8975,7 +9202,7 @@
       <c r="C11" s="13">
         <v>1</v>
       </c>
-      <c r="D11" s="70">
+      <c r="D11" s="48">
         <v>1</v>
       </c>
       <c r="E11" s="13"/>
@@ -8991,7 +9218,7 @@
       <c r="C12" s="13">
         <v>1</v>
       </c>
-      <c r="D12" s="70">
+      <c r="D12" s="48">
         <v>0</v>
       </c>
       <c r="E12" s="13"/>
@@ -9007,7 +9234,7 @@
       <c r="C13" s="13">
         <v>1</v>
       </c>
-      <c r="D13" s="70">
+      <c r="D13" s="48">
         <v>0</v>
       </c>
       <c r="E13" s="13"/>
@@ -9023,7 +9250,7 @@
       <c r="C14" s="13">
         <v>1</v>
       </c>
-      <c r="D14" s="70">
+      <c r="D14" s="48">
         <v>0</v>
       </c>
       <c r="E14" s="13"/>
@@ -9039,7 +9266,7 @@
       <c r="C15" s="13">
         <v>1</v>
       </c>
-      <c r="D15" s="70">
+      <c r="D15" s="48">
         <v>0</v>
       </c>
       <c r="E15" s="13"/>
@@ -9055,7 +9282,7 @@
       <c r="C16" s="13">
         <v>1</v>
       </c>
-      <c r="D16" s="70">
+      <c r="D16" s="48">
         <v>0</v>
       </c>
       <c r="E16" s="13"/>
@@ -9071,7 +9298,7 @@
       <c r="C17" s="13">
         <v>1</v>
       </c>
-      <c r="D17" s="70">
+      <c r="D17" s="48">
         <v>0</v>
       </c>
       <c r="E17" s="13"/>
@@ -9087,7 +9314,7 @@
       <c r="C18" s="13">
         <v>1</v>
       </c>
-      <c r="D18" s="70">
+      <c r="D18" s="48">
         <v>0</v>
       </c>
       <c r="E18" s="13"/>
@@ -9103,7 +9330,7 @@
       <c r="C19" s="13">
         <v>1</v>
       </c>
-      <c r="D19" s="70">
+      <c r="D19" s="48">
         <v>0</v>
       </c>
       <c r="E19" s="13"/>
@@ -9119,7 +9346,7 @@
       <c r="C20" s="13">
         <v>1</v>
       </c>
-      <c r="D20" s="70">
+      <c r="D20" s="48">
         <v>0</v>
       </c>
       <c r="E20" s="13"/>
@@ -9135,7 +9362,7 @@
       <c r="C21" s="13">
         <v>1</v>
       </c>
-      <c r="D21" s="70">
+      <c r="D21" s="48">
         <v>0</v>
       </c>
       <c r="E21" s="13"/>
@@ -9151,7 +9378,7 @@
       <c r="C22" s="13">
         <v>1</v>
       </c>
-      <c r="D22" s="70">
+      <c r="D22" s="48">
         <v>0</v>
       </c>
       <c r="E22" s="13"/>
@@ -9167,7 +9394,7 @@
       <c r="C23" s="13">
         <v>1</v>
       </c>
-      <c r="D23" s="70">
+      <c r="D23" s="48">
         <v>0</v>
       </c>
       <c r="E23" s="13"/>
@@ -9183,7 +9410,7 @@
       <c r="C24" s="13">
         <v>1</v>
       </c>
-      <c r="D24" s="70">
+      <c r="D24" s="48">
         <v>1</v>
       </c>
       <c r="E24" s="13"/>
@@ -9199,7 +9426,7 @@
       <c r="C25" s="13">
         <v>1</v>
       </c>
-      <c r="D25" s="70">
+      <c r="D25" s="48">
         <v>0</v>
       </c>
       <c r="E25" s="13"/>
@@ -9215,7 +9442,7 @@
       <c r="C26" s="13">
         <v>1</v>
       </c>
-      <c r="D26" s="70">
+      <c r="D26" s="48">
         <v>1</v>
       </c>
       <c r="E26" s="13"/>
@@ -9231,7 +9458,7 @@
       <c r="C27" s="13">
         <v>1</v>
       </c>
-      <c r="D27" s="70">
+      <c r="D27" s="48">
         <v>0</v>
       </c>
       <c r="E27" s="13"/>
@@ -9247,7 +9474,7 @@
       <c r="C28" s="13">
         <v>1</v>
       </c>
-      <c r="D28" s="70">
+      <c r="D28" s="48">
         <v>1</v>
       </c>
       <c r="E28" s="13"/>
@@ -9263,7 +9490,7 @@
       <c r="C29" s="13">
         <v>1</v>
       </c>
-      <c r="D29" s="70">
+      <c r="D29" s="48">
         <v>0</v>
       </c>
       <c r="E29" s="13"/>
@@ -9279,7 +9506,7 @@
       <c r="C30" s="13">
         <v>1</v>
       </c>
-      <c r="D30" s="70">
+      <c r="D30" s="48">
         <v>1</v>
       </c>
       <c r="E30" s="13"/>
@@ -9295,7 +9522,7 @@
       <c r="C31" s="13">
         <v>1</v>
       </c>
-      <c r="D31" s="70">
+      <c r="D31" s="48">
         <v>0</v>
       </c>
       <c r="E31" s="13"/>
@@ -9311,7 +9538,7 @@
       <c r="C32" s="13">
         <v>1</v>
       </c>
-      <c r="D32" s="70">
+      <c r="D32" s="48">
         <v>1</v>
       </c>
       <c r="E32" s="13"/>
@@ -9327,7 +9554,7 @@
       <c r="C33" s="13">
         <v>1</v>
       </c>
-      <c r="D33" s="70">
+      <c r="D33" s="48">
         <v>0</v>
       </c>
       <c r="E33" s="13"/>
@@ -9343,7 +9570,7 @@
       <c r="C34" s="13">
         <v>1</v>
       </c>
-      <c r="D34" s="70">
+      <c r="D34" s="48">
         <v>1</v>
       </c>
       <c r="E34" s="13"/>
@@ -9359,7 +9586,7 @@
       <c r="C35" s="15">
         <v>1</v>
       </c>
-      <c r="D35" s="71">
+      <c r="D35" s="49">
         <v>1</v>
       </c>
       <c r="E35" s="15"/>
@@ -9369,790 +9596,788 @@
       <c r="I35" s="16"/>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="C36" s="58" t="s">
+      <c r="C36" s="74" t="s">
         <v>162</v>
       </c>
-      <c r="D36" s="58"/>
-      <c r="E36" s="58"/>
-      <c r="F36" s="58"/>
-      <c r="G36" s="58"/>
-      <c r="H36" s="58"/>
+      <c r="D36" s="74"/>
+      <c r="E36" s="74"/>
+      <c r="F36" s="74"/>
+      <c r="G36" s="74"/>
+      <c r="H36" s="74"/>
     </row>
     <row r="41" spans="2:18" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B41" s="90"/>
-      <c r="C41" s="76" t="s">
+      <c r="B41" s="58"/>
+      <c r="C41" s="71" t="s">
         <v>231</v>
       </c>
-      <c r="D41" s="76"/>
-      <c r="E41" s="76"/>
-      <c r="F41" s="76"/>
-      <c r="G41" s="76"/>
-      <c r="H41" s="76"/>
-      <c r="I41" s="76"/>
-      <c r="J41" s="76"/>
-      <c r="K41" s="76"/>
-      <c r="L41" s="76"/>
-      <c r="M41" s="76"/>
-      <c r="N41" s="76"/>
+      <c r="D41" s="71"/>
+      <c r="E41" s="71"/>
+      <c r="F41" s="71"/>
+      <c r="G41" s="71"/>
+      <c r="H41" s="71"/>
+      <c r="I41" s="71"/>
+      <c r="J41" s="71"/>
+      <c r="K41" s="71"/>
+      <c r="L41" s="71"/>
+      <c r="M41" s="71"/>
+      <c r="N41" s="71"/>
     </row>
     <row r="42" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="B42" s="91"/>
-      <c r="C42" s="86" t="s">
+      <c r="B42" s="59"/>
+      <c r="C42" s="69" t="s">
         <v>155</v>
       </c>
-      <c r="D42" s="83"/>
-      <c r="E42" s="86" t="s">
+      <c r="D42" s="75"/>
+      <c r="E42" s="69" t="s">
         <v>156</v>
       </c>
-      <c r="F42" s="75"/>
-      <c r="G42" s="77" t="s">
+      <c r="F42" s="70"/>
+      <c r="G42" s="70" t="s">
         <v>157</v>
       </c>
-      <c r="H42" s="77"/>
-      <c r="I42" s="77" t="s">
+      <c r="H42" s="70"/>
+      <c r="I42" s="70" t="s">
         <v>158</v>
       </c>
-      <c r="J42" s="77"/>
-      <c r="K42" s="86" t="s">
+      <c r="J42" s="70"/>
+      <c r="K42" s="69" t="s">
         <v>159</v>
       </c>
-      <c r="L42" s="77"/>
-      <c r="M42" s="86" t="s">
+      <c r="L42" s="70"/>
+      <c r="M42" s="69" t="s">
         <v>160</v>
       </c>
-      <c r="N42" s="77"/>
-      <c r="O42" s="93"/>
-      <c r="P42" s="94"/>
-      <c r="Q42" s="94"/>
-      <c r="R42" s="93"/>
+      <c r="N42" s="70"/>
+      <c r="O42" s="18"/>
+      <c r="R42" s="18"/>
     </row>
     <row r="43" spans="2:18" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B43" s="92"/>
-      <c r="C43" s="84" t="s">
+      <c r="B43" s="53"/>
+      <c r="C43" s="50" t="s">
         <v>203</v>
       </c>
-      <c r="D43" s="81" t="s">
+      <c r="D43" s="54" t="s">
         <v>204</v>
       </c>
-      <c r="E43" s="72" t="s">
+      <c r="E43" s="50" t="s">
         <v>203</v>
       </c>
-      <c r="F43" s="81" t="s">
+      <c r="F43" s="54" t="s">
         <v>204</v>
       </c>
-      <c r="G43" s="72" t="s">
+      <c r="G43" s="50" t="s">
         <v>203</v>
       </c>
-      <c r="H43" s="81" t="s">
+      <c r="H43" s="54" t="s">
         <v>204</v>
       </c>
-      <c r="I43" s="72" t="s">
+      <c r="I43" s="50" t="s">
         <v>203</v>
       </c>
-      <c r="J43" s="81" t="s">
+      <c r="J43" s="54" t="s">
         <v>204</v>
       </c>
-      <c r="K43" s="72" t="s">
+      <c r="K43" s="50" t="s">
         <v>203</v>
       </c>
-      <c r="L43" s="81" t="s">
+      <c r="L43" s="54" t="s">
         <v>204</v>
       </c>
-      <c r="M43" s="72" t="s">
+      <c r="M43" s="50" t="s">
         <v>203</v>
       </c>
-      <c r="N43" s="81" t="s">
+      <c r="N43" s="54" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="44" spans="2:18" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B44" s="92" t="s">
+      <c r="B44" s="53" t="s">
         <v>202</v>
       </c>
-      <c r="C44" s="84" t="s">
+      <c r="C44" s="50" t="s">
         <v>202</v>
       </c>
-      <c r="D44" s="81" t="s">
+      <c r="D44" s="54" t="s">
         <v>202</v>
       </c>
-      <c r="E44" s="72" t="s">
+      <c r="E44" s="50" t="s">
         <v>202</v>
       </c>
-      <c r="F44" s="81" t="s">
+      <c r="F44" s="54" t="s">
         <v>202</v>
       </c>
-      <c r="G44" s="72" t="s">
+      <c r="G44" s="50" t="s">
         <v>202</v>
       </c>
-      <c r="H44" s="81" t="s">
+      <c r="H44" s="54" t="s">
         <v>202</v>
       </c>
-      <c r="I44" s="72" t="s">
+      <c r="I44" s="50" t="s">
         <v>202</v>
       </c>
-      <c r="J44" s="81" t="s">
+      <c r="J44" s="54" t="s">
         <v>202</v>
       </c>
-      <c r="K44" s="72" t="s">
+      <c r="K44" s="50" t="s">
         <v>202</v>
       </c>
-      <c r="L44" s="81" t="s">
+      <c r="L44" s="54" t="s">
         <v>202</v>
       </c>
-      <c r="M44" s="72" t="s">
+      <c r="M44" s="50" t="s">
         <v>202</v>
       </c>
-      <c r="N44" s="81" t="s">
+      <c r="N44" s="54" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="45" spans="2:18" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="B45" s="70" t="s">
+      <c r="B45" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="C45" s="80"/>
-      <c r="D45" s="82"/>
-      <c r="E45" s="70" t="s">
+      <c r="C45" s="53"/>
+      <c r="D45" s="55"/>
+      <c r="E45" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="F45" s="87" t="s">
+      <c r="F45" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="G45" s="85"/>
-      <c r="H45" s="82"/>
-      <c r="I45" s="85"/>
-      <c r="J45" s="82"/>
-      <c r="K45" s="85"/>
-      <c r="L45" s="82"/>
-      <c r="M45" s="85"/>
-      <c r="N45" s="82"/>
+      <c r="G45" s="53"/>
+      <c r="H45" s="55"/>
+      <c r="I45" s="53"/>
+      <c r="J45" s="55"/>
+      <c r="K45" s="53"/>
+      <c r="L45" s="55"/>
+      <c r="M45" s="53"/>
+      <c r="N45" s="55"/>
     </row>
     <row r="46" spans="2:18" ht="87" x14ac:dyDescent="0.35">
-      <c r="B46" s="78" t="s">
+      <c r="B46" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="C46" s="79"/>
-      <c r="D46" s="82"/>
-      <c r="E46" s="70" t="s">
+      <c r="C46" s="51"/>
+      <c r="D46" s="55"/>
+      <c r="E46" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="F46" s="87" t="s">
+      <c r="F46" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="G46" s="73"/>
-      <c r="H46" s="82"/>
-      <c r="I46" s="73"/>
-      <c r="J46" s="82"/>
-      <c r="K46" s="73"/>
-      <c r="L46" s="82"/>
-      <c r="M46" s="73"/>
-      <c r="N46" s="82"/>
+      <c r="G46" s="51"/>
+      <c r="H46" s="55"/>
+      <c r="I46" s="51"/>
+      <c r="J46" s="55"/>
+      <c r="K46" s="51"/>
+      <c r="L46" s="55"/>
+      <c r="M46" s="51"/>
+      <c r="N46" s="55"/>
     </row>
     <row r="47" spans="2:18" ht="145" x14ac:dyDescent="0.35">
-      <c r="B47" s="78" t="s">
+      <c r="B47" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="C47" s="79"/>
-      <c r="D47" s="82"/>
-      <c r="E47" s="70" t="s">
+      <c r="C47" s="51"/>
+      <c r="D47" s="55"/>
+      <c r="E47" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="F47" s="87" t="s">
+      <c r="F47" s="56" t="s">
         <v>208</v>
       </c>
-      <c r="G47" s="73"/>
-      <c r="H47" s="82"/>
-      <c r="I47" s="73"/>
-      <c r="J47" s="82"/>
-      <c r="K47" s="73"/>
-      <c r="L47" s="82"/>
-      <c r="M47" s="73"/>
-      <c r="N47" s="82"/>
+      <c r="G47" s="51"/>
+      <c r="H47" s="55"/>
+      <c r="I47" s="51"/>
+      <c r="J47" s="55"/>
+      <c r="K47" s="51"/>
+      <c r="L47" s="55"/>
+      <c r="M47" s="51"/>
+      <c r="N47" s="55"/>
     </row>
     <row r="48" spans="2:18" ht="58" x14ac:dyDescent="0.35">
-      <c r="B48" s="78" t="s">
+      <c r="B48" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C48" s="79"/>
-      <c r="D48" s="82"/>
-      <c r="E48" s="74" t="s">
+      <c r="C48" s="51"/>
+      <c r="D48" s="55"/>
+      <c r="E48" s="52" t="s">
         <v>209</v>
       </c>
-      <c r="F48" s="87" t="s">
+      <c r="F48" s="56" t="s">
         <v>210</v>
       </c>
-      <c r="G48" s="73"/>
-      <c r="H48" s="82"/>
-      <c r="I48" s="73"/>
-      <c r="J48" s="82"/>
-      <c r="K48" s="73"/>
-      <c r="L48" s="82"/>
-      <c r="M48" s="73"/>
-      <c r="N48" s="82"/>
+      <c r="G48" s="51"/>
+      <c r="H48" s="55"/>
+      <c r="I48" s="51"/>
+      <c r="J48" s="55"/>
+      <c r="K48" s="51"/>
+      <c r="L48" s="55"/>
+      <c r="M48" s="51"/>
+      <c r="N48" s="55"/>
     </row>
     <row r="49" spans="2:14" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B49" s="78" t="s">
+      <c r="B49" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="C49" s="79"/>
-      <c r="D49" s="82"/>
-      <c r="E49" s="70" t="s">
+      <c r="C49" s="51"/>
+      <c r="D49" s="55"/>
+      <c r="E49" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="F49" s="87" t="s">
+      <c r="F49" s="56" t="s">
         <v>211</v>
       </c>
-      <c r="G49" s="73"/>
-      <c r="H49" s="82"/>
-      <c r="I49" s="73"/>
-      <c r="J49" s="82"/>
-      <c r="K49" s="73"/>
-      <c r="L49" s="82"/>
-      <c r="M49" s="73"/>
-      <c r="N49" s="82"/>
+      <c r="G49" s="51"/>
+      <c r="H49" s="55"/>
+      <c r="I49" s="51"/>
+      <c r="J49" s="55"/>
+      <c r="K49" s="51"/>
+      <c r="L49" s="55"/>
+      <c r="M49" s="51"/>
+      <c r="N49" s="55"/>
     </row>
     <row r="50" spans="2:14" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="B50" s="78" t="s">
+      <c r="B50" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="C50" s="79"/>
-      <c r="D50" s="82"/>
-      <c r="E50" s="74" t="s">
+      <c r="C50" s="51"/>
+      <c r="D50" s="55"/>
+      <c r="E50" s="52" t="s">
         <v>209</v>
       </c>
-      <c r="F50" s="87" t="s">
+      <c r="F50" s="56" t="s">
         <v>212</v>
       </c>
-      <c r="G50" s="73"/>
-      <c r="H50" s="82"/>
-      <c r="I50" s="73"/>
-      <c r="J50" s="82"/>
-      <c r="K50" s="73"/>
-      <c r="L50" s="82"/>
-      <c r="M50" s="73"/>
-      <c r="N50" s="82"/>
+      <c r="G50" s="51"/>
+      <c r="H50" s="55"/>
+      <c r="I50" s="51"/>
+      <c r="J50" s="55"/>
+      <c r="K50" s="51"/>
+      <c r="L50" s="55"/>
+      <c r="M50" s="51"/>
+      <c r="N50" s="55"/>
     </row>
     <row r="51" spans="2:14" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="B51" s="78" t="s">
+      <c r="B51" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C51" s="79"/>
-      <c r="D51" s="82"/>
-      <c r="E51" s="70"/>
-      <c r="F51" s="87" t="s">
+      <c r="C51" s="51"/>
+      <c r="D51" s="55"/>
+      <c r="E51" s="48"/>
+      <c r="F51" s="56" t="s">
         <v>206</v>
       </c>
-      <c r="G51" s="73"/>
-      <c r="H51" s="82"/>
-      <c r="I51" s="73"/>
-      <c r="J51" s="82"/>
-      <c r="K51" s="73"/>
-      <c r="L51" s="82"/>
-      <c r="M51" s="73"/>
-      <c r="N51" s="82"/>
+      <c r="G51" s="51"/>
+      <c r="H51" s="55"/>
+      <c r="I51" s="51"/>
+      <c r="J51" s="55"/>
+      <c r="K51" s="51"/>
+      <c r="L51" s="55"/>
+      <c r="M51" s="51"/>
+      <c r="N51" s="55"/>
     </row>
     <row r="52" spans="2:14" ht="87" x14ac:dyDescent="0.35">
-      <c r="B52" s="78" t="s">
+      <c r="B52" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="C52" s="79"/>
-      <c r="D52" s="82"/>
-      <c r="E52" s="70" t="s">
+      <c r="C52" s="51"/>
+      <c r="D52" s="55"/>
+      <c r="E52" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="F52" s="87" t="s">
+      <c r="F52" s="56" t="s">
         <v>213</v>
       </c>
-      <c r="G52" s="73"/>
-      <c r="H52" s="82"/>
-      <c r="I52" s="73"/>
-      <c r="J52" s="82"/>
-      <c r="K52" s="73"/>
-      <c r="L52" s="82"/>
-      <c r="M52" s="73"/>
-      <c r="N52" s="82"/>
+      <c r="G52" s="51"/>
+      <c r="H52" s="55"/>
+      <c r="I52" s="51"/>
+      <c r="J52" s="55"/>
+      <c r="K52" s="51"/>
+      <c r="L52" s="55"/>
+      <c r="M52" s="51"/>
+      <c r="N52" s="55"/>
     </row>
     <row r="53" spans="2:14" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="B53" s="78" t="s">
+      <c r="B53" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="C53" s="79"/>
-      <c r="D53" s="82"/>
-      <c r="E53" s="70" t="s">
+      <c r="C53" s="51"/>
+      <c r="D53" s="55"/>
+      <c r="E53" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="F53" s="87" t="s">
+      <c r="F53" s="56" t="s">
         <v>214</v>
       </c>
-      <c r="G53" s="73"/>
-      <c r="H53" s="82"/>
-      <c r="I53" s="73"/>
-      <c r="J53" s="82"/>
-      <c r="K53" s="73"/>
-      <c r="L53" s="82"/>
-      <c r="M53" s="73"/>
-      <c r="N53" s="82"/>
+      <c r="G53" s="51"/>
+      <c r="H53" s="55"/>
+      <c r="I53" s="51"/>
+      <c r="J53" s="55"/>
+      <c r="K53" s="51"/>
+      <c r="L53" s="55"/>
+      <c r="M53" s="51"/>
+      <c r="N53" s="55"/>
     </row>
     <row r="54" spans="2:14" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="B54" s="78" t="s">
+      <c r="B54" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="C54" s="79"/>
-      <c r="D54" s="82"/>
-      <c r="E54" s="70" t="s">
+      <c r="C54" s="51"/>
+      <c r="D54" s="55"/>
+      <c r="E54" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="F54" s="87" t="s">
+      <c r="F54" s="56" t="s">
         <v>214</v>
       </c>
-      <c r="G54" s="73"/>
-      <c r="H54" s="82"/>
-      <c r="I54" s="73"/>
-      <c r="J54" s="82"/>
-      <c r="K54" s="73"/>
-      <c r="L54" s="82"/>
-      <c r="M54" s="73"/>
-      <c r="N54" s="82"/>
+      <c r="G54" s="51"/>
+      <c r="H54" s="55"/>
+      <c r="I54" s="51"/>
+      <c r="J54" s="55"/>
+      <c r="K54" s="51"/>
+      <c r="L54" s="55"/>
+      <c r="M54" s="51"/>
+      <c r="N54" s="55"/>
     </row>
     <row r="55" spans="2:14" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B55" s="78" t="s">
+      <c r="B55" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="C55" s="79"/>
-      <c r="D55" s="82"/>
-      <c r="E55" s="70" t="s">
+      <c r="C55" s="51"/>
+      <c r="D55" s="55"/>
+      <c r="E55" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="F55" s="87" t="s">
+      <c r="F55" s="56" t="s">
         <v>215</v>
       </c>
-      <c r="G55" s="73"/>
-      <c r="H55" s="82"/>
-      <c r="I55" s="73"/>
-      <c r="J55" s="82"/>
-      <c r="K55" s="73"/>
-      <c r="L55" s="82"/>
-      <c r="M55" s="73"/>
-      <c r="N55" s="82"/>
+      <c r="G55" s="51"/>
+      <c r="H55" s="55"/>
+      <c r="I55" s="51"/>
+      <c r="J55" s="55"/>
+      <c r="K55" s="51"/>
+      <c r="L55" s="55"/>
+      <c r="M55" s="51"/>
+      <c r="N55" s="55"/>
     </row>
     <row r="56" spans="2:14" ht="116" x14ac:dyDescent="0.35">
-      <c r="B56" s="78" t="s">
+      <c r="B56" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="C56" s="79"/>
-      <c r="D56" s="82"/>
-      <c r="E56" s="70" t="s">
+      <c r="C56" s="51"/>
+      <c r="D56" s="55"/>
+      <c r="E56" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="F56" s="87" t="s">
+      <c r="F56" s="56" t="s">
         <v>216</v>
       </c>
-      <c r="G56" s="73"/>
-      <c r="H56" s="82"/>
-      <c r="I56" s="73"/>
-      <c r="J56" s="82"/>
-      <c r="K56" s="73"/>
-      <c r="L56" s="82"/>
-      <c r="M56" s="73"/>
-      <c r="N56" s="82"/>
+      <c r="G56" s="51"/>
+      <c r="H56" s="55"/>
+      <c r="I56" s="51"/>
+      <c r="J56" s="55"/>
+      <c r="K56" s="51"/>
+      <c r="L56" s="55"/>
+      <c r="M56" s="51"/>
+      <c r="N56" s="55"/>
     </row>
     <row r="57" spans="2:14" ht="87" x14ac:dyDescent="0.35">
-      <c r="B57" s="78" t="s">
+      <c r="B57" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="C57" s="79"/>
-      <c r="D57" s="82"/>
-      <c r="E57" s="70" t="s">
+      <c r="C57" s="51"/>
+      <c r="D57" s="55"/>
+      <c r="E57" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="F57" s="87" t="s">
+      <c r="F57" s="56" t="s">
         <v>217</v>
       </c>
-      <c r="G57" s="73"/>
-      <c r="H57" s="82"/>
-      <c r="I57" s="73"/>
-      <c r="J57" s="82"/>
-      <c r="K57" s="73"/>
-      <c r="L57" s="82"/>
-      <c r="M57" s="73"/>
-      <c r="N57" s="82"/>
+      <c r="G57" s="51"/>
+      <c r="H57" s="55"/>
+      <c r="I57" s="51"/>
+      <c r="J57" s="55"/>
+      <c r="K57" s="51"/>
+      <c r="L57" s="55"/>
+      <c r="M57" s="51"/>
+      <c r="N57" s="55"/>
     </row>
     <row r="58" spans="2:14" ht="145" x14ac:dyDescent="0.35">
-      <c r="B58" s="78" t="s">
+      <c r="B58" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="C58" s="79"/>
-      <c r="D58" s="82"/>
-      <c r="E58" s="70" t="s">
+      <c r="C58" s="51"/>
+      <c r="D58" s="55"/>
+      <c r="E58" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="F58" s="87" t="s">
+      <c r="F58" s="56" t="s">
         <v>208</v>
       </c>
-      <c r="G58" s="73"/>
-      <c r="H58" s="82"/>
-      <c r="I58" s="73"/>
-      <c r="J58" s="82"/>
-      <c r="K58" s="73"/>
-      <c r="L58" s="82"/>
-      <c r="M58" s="73"/>
-      <c r="N58" s="82"/>
+      <c r="G58" s="51"/>
+      <c r="H58" s="55"/>
+      <c r="I58" s="51"/>
+      <c r="J58" s="55"/>
+      <c r="K58" s="51"/>
+      <c r="L58" s="55"/>
+      <c r="M58" s="51"/>
+      <c r="N58" s="55"/>
     </row>
     <row r="59" spans="2:14" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="B59" s="78" t="s">
+      <c r="B59" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="C59" s="79"/>
-      <c r="D59" s="82"/>
-      <c r="E59" s="70" t="s">
+      <c r="C59" s="51"/>
+      <c r="D59" s="55"/>
+      <c r="E59" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="F59" s="87" t="s">
+      <c r="F59" s="56" t="s">
         <v>218</v>
       </c>
-      <c r="G59" s="73"/>
-      <c r="H59" s="82"/>
-      <c r="I59" s="73"/>
-      <c r="J59" s="82"/>
-      <c r="K59" s="73"/>
-      <c r="L59" s="82"/>
-      <c r="M59" s="73"/>
-      <c r="N59" s="82"/>
+      <c r="G59" s="51"/>
+      <c r="H59" s="55"/>
+      <c r="I59" s="51"/>
+      <c r="J59" s="55"/>
+      <c r="K59" s="51"/>
+      <c r="L59" s="55"/>
+      <c r="M59" s="51"/>
+      <c r="N59" s="55"/>
     </row>
     <row r="60" spans="2:14" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="B60" s="78" t="s">
+      <c r="B60" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="C60" s="79"/>
-      <c r="D60" s="82"/>
-      <c r="E60" s="70" t="s">
+      <c r="C60" s="51"/>
+      <c r="D60" s="55"/>
+      <c r="E60" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="F60" s="87" t="s">
+      <c r="F60" s="56" t="s">
         <v>219</v>
       </c>
-      <c r="G60" s="73"/>
-      <c r="H60" s="82"/>
-      <c r="I60" s="73"/>
-      <c r="J60" s="82"/>
-      <c r="K60" s="73"/>
-      <c r="L60" s="82"/>
-      <c r="M60" s="73"/>
-      <c r="N60" s="82"/>
+      <c r="G60" s="51"/>
+      <c r="H60" s="55"/>
+      <c r="I60" s="51"/>
+      <c r="J60" s="55"/>
+      <c r="K60" s="51"/>
+      <c r="L60" s="55"/>
+      <c r="M60" s="51"/>
+      <c r="N60" s="55"/>
     </row>
     <row r="61" spans="2:14" ht="58" x14ac:dyDescent="0.35">
-      <c r="B61" s="78" t="s">
+      <c r="B61" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="C61" s="79"/>
-      <c r="D61" s="82"/>
-      <c r="E61" s="70" t="s">
+      <c r="C61" s="51"/>
+      <c r="D61" s="55"/>
+      <c r="E61" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="F61" s="87" t="s">
+      <c r="F61" s="56" t="s">
         <v>220</v>
       </c>
-      <c r="G61" s="73"/>
-      <c r="H61" s="82"/>
-      <c r="I61" s="73"/>
-      <c r="J61" s="82"/>
-      <c r="K61" s="73"/>
-      <c r="L61" s="82"/>
-      <c r="M61" s="73"/>
-      <c r="N61" s="82"/>
+      <c r="G61" s="51"/>
+      <c r="H61" s="55"/>
+      <c r="I61" s="51"/>
+      <c r="J61" s="55"/>
+      <c r="K61" s="51"/>
+      <c r="L61" s="55"/>
+      <c r="M61" s="51"/>
+      <c r="N61" s="55"/>
     </row>
     <row r="62" spans="2:14" ht="58" x14ac:dyDescent="0.35">
-      <c r="B62" s="78" t="s">
+      <c r="B62" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="C62" s="79"/>
-      <c r="D62" s="82"/>
-      <c r="E62" s="70" t="s">
+      <c r="C62" s="51"/>
+      <c r="D62" s="55"/>
+      <c r="E62" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="F62" s="87" t="s">
+      <c r="F62" s="56" t="s">
         <v>220</v>
       </c>
-      <c r="G62" s="73"/>
-      <c r="H62" s="82"/>
-      <c r="I62" s="73"/>
-      <c r="J62" s="82"/>
-      <c r="K62" s="73"/>
-      <c r="L62" s="82"/>
-      <c r="M62" s="73"/>
-      <c r="N62" s="82"/>
+      <c r="G62" s="51"/>
+      <c r="H62" s="55"/>
+      <c r="I62" s="51"/>
+      <c r="J62" s="55"/>
+      <c r="K62" s="51"/>
+      <c r="L62" s="55"/>
+      <c r="M62" s="51"/>
+      <c r="N62" s="55"/>
     </row>
     <row r="63" spans="2:14" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B63" s="78" t="s">
+      <c r="B63" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="C63" s="79"/>
-      <c r="D63" s="82"/>
-      <c r="E63" s="74" t="s">
+      <c r="C63" s="51"/>
+      <c r="D63" s="55"/>
+      <c r="E63" s="52" t="s">
         <v>209</v>
       </c>
-      <c r="F63" s="87" t="s">
+      <c r="F63" s="56" t="s">
         <v>221</v>
       </c>
-      <c r="G63" s="73"/>
-      <c r="H63" s="82"/>
-      <c r="I63" s="73"/>
-      <c r="J63" s="82"/>
-      <c r="K63" s="73"/>
-      <c r="L63" s="82"/>
-      <c r="M63" s="73"/>
-      <c r="N63" s="82"/>
+      <c r="G63" s="51"/>
+      <c r="H63" s="55"/>
+      <c r="I63" s="51"/>
+      <c r="J63" s="55"/>
+      <c r="K63" s="51"/>
+      <c r="L63" s="55"/>
+      <c r="M63" s="51"/>
+      <c r="N63" s="55"/>
     </row>
     <row r="64" spans="2:14" ht="145" x14ac:dyDescent="0.35">
-      <c r="B64" s="78" t="s">
+      <c r="B64" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="C64" s="79"/>
-      <c r="D64" s="82"/>
-      <c r="E64" s="70" t="s">
+      <c r="C64" s="51"/>
+      <c r="D64" s="55"/>
+      <c r="E64" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="F64" s="87" t="s">
+      <c r="F64" s="56" t="s">
         <v>208</v>
       </c>
-      <c r="G64" s="73"/>
-      <c r="H64" s="82"/>
-      <c r="I64" s="73"/>
-      <c r="J64" s="82"/>
-      <c r="K64" s="73"/>
-      <c r="L64" s="82"/>
-      <c r="M64" s="73"/>
-      <c r="N64" s="82"/>
+      <c r="G64" s="51"/>
+      <c r="H64" s="55"/>
+      <c r="I64" s="51"/>
+      <c r="J64" s="55"/>
+      <c r="K64" s="51"/>
+      <c r="L64" s="55"/>
+      <c r="M64" s="51"/>
+      <c r="N64" s="55"/>
     </row>
     <row r="65" spans="2:14" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="B65" s="78" t="s">
+      <c r="B65" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="C65" s="79"/>
-      <c r="D65" s="82"/>
-      <c r="E65" s="74" t="s">
+      <c r="C65" s="51"/>
+      <c r="D65" s="55"/>
+      <c r="E65" s="52" t="s">
         <v>209</v>
       </c>
-      <c r="F65" s="87" t="s">
+      <c r="F65" s="56" t="s">
         <v>222</v>
       </c>
-      <c r="G65" s="73"/>
-      <c r="H65" s="82"/>
-      <c r="I65" s="73"/>
-      <c r="J65" s="82"/>
-      <c r="K65" s="73"/>
-      <c r="L65" s="82"/>
-      <c r="M65" s="73"/>
-      <c r="N65" s="82"/>
+      <c r="G65" s="51"/>
+      <c r="H65" s="55"/>
+      <c r="I65" s="51"/>
+      <c r="J65" s="55"/>
+      <c r="K65" s="51"/>
+      <c r="L65" s="55"/>
+      <c r="M65" s="51"/>
+      <c r="N65" s="55"/>
     </row>
     <row r="66" spans="2:14" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="B66" s="78" t="s">
+      <c r="B66" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="C66" s="79"/>
-      <c r="D66" s="82"/>
-      <c r="E66" s="70" t="s">
+      <c r="C66" s="51"/>
+      <c r="D66" s="55"/>
+      <c r="E66" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="F66" s="87" t="s">
+      <c r="F66" s="56" t="s">
         <v>223</v>
       </c>
-      <c r="G66" s="73"/>
-      <c r="H66" s="82"/>
-      <c r="I66" s="73"/>
-      <c r="J66" s="82"/>
-      <c r="K66" s="73"/>
-      <c r="L66" s="82"/>
-      <c r="M66" s="73"/>
-      <c r="N66" s="82"/>
+      <c r="G66" s="51"/>
+      <c r="H66" s="55"/>
+      <c r="I66" s="51"/>
+      <c r="J66" s="55"/>
+      <c r="K66" s="51"/>
+      <c r="L66" s="55"/>
+      <c r="M66" s="51"/>
+      <c r="N66" s="55"/>
     </row>
     <row r="67" spans="2:14" ht="58" x14ac:dyDescent="0.35">
-      <c r="B67" s="78" t="s">
+      <c r="B67" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="C67" s="79"/>
-      <c r="D67" s="82"/>
-      <c r="E67" s="74" t="s">
+      <c r="C67" s="51"/>
+      <c r="D67" s="55"/>
+      <c r="E67" s="52" t="s">
         <v>209</v>
       </c>
-      <c r="F67" s="87" t="s">
+      <c r="F67" s="56" t="s">
         <v>224</v>
       </c>
-      <c r="G67" s="73"/>
-      <c r="H67" s="82"/>
-      <c r="I67" s="73"/>
-      <c r="J67" s="82"/>
-      <c r="K67" s="73"/>
-      <c r="L67" s="82"/>
-      <c r="M67" s="73"/>
-      <c r="N67" s="82"/>
+      <c r="G67" s="51"/>
+      <c r="H67" s="55"/>
+      <c r="I67" s="51"/>
+      <c r="J67" s="55"/>
+      <c r="K67" s="51"/>
+      <c r="L67" s="55"/>
+      <c r="M67" s="51"/>
+      <c r="N67" s="55"/>
     </row>
     <row r="68" spans="2:14" ht="58" x14ac:dyDescent="0.35">
-      <c r="B68" s="78" t="s">
+      <c r="B68" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="C68" s="79"/>
-      <c r="D68" s="82"/>
-      <c r="E68" s="70" t="s">
+      <c r="C68" s="51"/>
+      <c r="D68" s="55"/>
+      <c r="E68" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="F68" s="87" t="s">
+      <c r="F68" s="56" t="s">
         <v>225</v>
       </c>
-      <c r="G68" s="73"/>
-      <c r="H68" s="82"/>
-      <c r="I68" s="73"/>
-      <c r="J68" s="82"/>
-      <c r="K68" s="73"/>
-      <c r="L68" s="82"/>
-      <c r="M68" s="73"/>
-      <c r="N68" s="82"/>
+      <c r="G68" s="51"/>
+      <c r="H68" s="55"/>
+      <c r="I68" s="51"/>
+      <c r="J68" s="55"/>
+      <c r="K68" s="51"/>
+      <c r="L68" s="55"/>
+      <c r="M68" s="51"/>
+      <c r="N68" s="55"/>
     </row>
     <row r="69" spans="2:14" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="B69" s="78" t="s">
+      <c r="B69" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="C69" s="79"/>
-      <c r="D69" s="82"/>
-      <c r="E69" s="74" t="s">
+      <c r="C69" s="51"/>
+      <c r="D69" s="55"/>
+      <c r="E69" s="52" t="s">
         <v>209</v>
       </c>
-      <c r="F69" s="87" t="s">
+      <c r="F69" s="56" t="s">
         <v>226</v>
       </c>
-      <c r="G69" s="73"/>
-      <c r="H69" s="82"/>
-      <c r="I69" s="73"/>
-      <c r="J69" s="82"/>
-      <c r="K69" s="73"/>
-      <c r="L69" s="82"/>
-      <c r="M69" s="73"/>
-      <c r="N69" s="82"/>
+      <c r="G69" s="51"/>
+      <c r="H69" s="55"/>
+      <c r="I69" s="51"/>
+      <c r="J69" s="55"/>
+      <c r="K69" s="51"/>
+      <c r="L69" s="55"/>
+      <c r="M69" s="51"/>
+      <c r="N69" s="55"/>
     </row>
     <row r="70" spans="2:14" ht="58" x14ac:dyDescent="0.35">
-      <c r="B70" s="78" t="s">
+      <c r="B70" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="C70" s="79"/>
-      <c r="D70" s="82"/>
-      <c r="E70" s="70" t="s">
+      <c r="C70" s="51"/>
+      <c r="D70" s="55"/>
+      <c r="E70" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="F70" s="87" t="s">
+      <c r="F70" s="56" t="s">
         <v>227</v>
       </c>
-      <c r="G70" s="73"/>
-      <c r="H70" s="82"/>
-      <c r="I70" s="73"/>
-      <c r="J70" s="82"/>
-      <c r="K70" s="73"/>
-      <c r="L70" s="82"/>
-      <c r="M70" s="73"/>
-      <c r="N70" s="82"/>
+      <c r="G70" s="51"/>
+      <c r="H70" s="55"/>
+      <c r="I70" s="51"/>
+      <c r="J70" s="55"/>
+      <c r="K70" s="51"/>
+      <c r="L70" s="55"/>
+      <c r="M70" s="51"/>
+      <c r="N70" s="55"/>
     </row>
     <row r="71" spans="2:14" ht="29" x14ac:dyDescent="0.35">
-      <c r="B71" s="78" t="s">
+      <c r="B71" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="C71" s="79"/>
-      <c r="D71" s="82"/>
-      <c r="E71" s="74" t="s">
+      <c r="C71" s="51"/>
+      <c r="D71" s="55"/>
+      <c r="E71" s="52" t="s">
         <v>209</v>
       </c>
-      <c r="F71" s="87" t="s">
+      <c r="F71" s="56" t="s">
         <v>228</v>
       </c>
-      <c r="G71" s="73"/>
-      <c r="H71" s="82"/>
-      <c r="I71" s="73"/>
-      <c r="J71" s="82"/>
-      <c r="K71" s="73"/>
-      <c r="L71" s="82"/>
-      <c r="M71" s="73"/>
-      <c r="N71" s="82"/>
+      <c r="G71" s="51"/>
+      <c r="H71" s="55"/>
+      <c r="I71" s="51"/>
+      <c r="J71" s="55"/>
+      <c r="K71" s="51"/>
+      <c r="L71" s="55"/>
+      <c r="M71" s="51"/>
+      <c r="N71" s="55"/>
     </row>
     <row r="72" spans="2:14" ht="58" x14ac:dyDescent="0.35">
-      <c r="B72" s="78" t="s">
+      <c r="B72" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="C72" s="79"/>
-      <c r="D72" s="82"/>
-      <c r="E72" s="70" t="s">
+      <c r="C72" s="51"/>
+      <c r="D72" s="55"/>
+      <c r="E72" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="F72" s="87" t="s">
+      <c r="F72" s="56" t="s">
         <v>229</v>
       </c>
-      <c r="G72" s="73"/>
-      <c r="H72" s="82"/>
-      <c r="I72" s="73"/>
-      <c r="J72" s="82"/>
-      <c r="K72" s="73"/>
-      <c r="L72" s="82"/>
-      <c r="M72" s="73"/>
-      <c r="N72" s="82"/>
+      <c r="G72" s="51"/>
+      <c r="H72" s="55"/>
+      <c r="I72" s="51"/>
+      <c r="J72" s="55"/>
+      <c r="K72" s="51"/>
+      <c r="L72" s="55"/>
+      <c r="M72" s="51"/>
+      <c r="N72" s="55"/>
     </row>
     <row r="73" spans="2:14" ht="87" x14ac:dyDescent="0.35">
-      <c r="B73" s="78" t="s">
+      <c r="B73" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="C73" s="79"/>
-      <c r="D73" s="82"/>
-      <c r="E73" s="74" t="s">
+      <c r="C73" s="51"/>
+      <c r="D73" s="55"/>
+      <c r="E73" s="52" t="s">
         <v>209</v>
       </c>
-      <c r="F73" s="87" t="s">
+      <c r="F73" s="56" t="s">
         <v>230</v>
       </c>
-      <c r="G73" s="73"/>
-      <c r="H73" s="82"/>
-      <c r="I73" s="73"/>
-      <c r="J73" s="82"/>
-      <c r="K73" s="73"/>
-      <c r="L73" s="82"/>
-      <c r="M73" s="73"/>
-      <c r="N73" s="82"/>
+      <c r="G73" s="51"/>
+      <c r="H73" s="55"/>
+      <c r="I73" s="51"/>
+      <c r="J73" s="55"/>
+      <c r="K73" s="51"/>
+      <c r="L73" s="55"/>
+      <c r="M73" s="51"/>
+      <c r="N73" s="55"/>
     </row>
     <row r="74" spans="2:14" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B74" s="71" t="s">
+      <c r="B74" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="C74" s="79"/>
-      <c r="D74" s="82"/>
-      <c r="E74" s="74" t="s">
+      <c r="C74" s="51"/>
+      <c r="D74" s="55"/>
+      <c r="E74" s="52" t="s">
         <v>209</v>
       </c>
-      <c r="F74" s="87" t="s">
+      <c r="F74" s="56" t="s">
         <v>224</v>
       </c>
-      <c r="G74" s="73"/>
-      <c r="H74" s="82"/>
-      <c r="I74" s="73"/>
-      <c r="J74" s="82"/>
-      <c r="K74" s="73"/>
-      <c r="L74" s="82"/>
-      <c r="M74" s="73"/>
-      <c r="N74" s="82"/>
+      <c r="G74" s="51"/>
+      <c r="H74" s="55"/>
+      <c r="I74" s="51"/>
+      <c r="J74" s="55"/>
+      <c r="K74" s="51"/>
+      <c r="L74" s="55"/>
+      <c r="M74" s="51"/>
+      <c r="N74" s="55"/>
     </row>
     <row r="75" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B75" s="95"/>
-      <c r="C75" s="78"/>
-      <c r="D75" s="79"/>
+      <c r="B75" s="48"/>
+      <c r="C75" s="48"/>
+      <c r="D75" s="51"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B6:B35">
     <sortCondition ref="B6:B35"/>
   </sortState>
   <mergeCells count="9">
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="C41:N41"/>
+    <mergeCell ref="C3:I4"/>
+    <mergeCell ref="C36:H36"/>
     <mergeCell ref="C42:D42"/>
     <mergeCell ref="E42:F42"/>
     <mergeCell ref="G42:H42"/>
     <mergeCell ref="I42:J42"/>
     <mergeCell ref="K42:L42"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="C41:N41"/>
-    <mergeCell ref="C3:I4"/>
-    <mergeCell ref="C36:H36"/>
   </mergeCells>
   <conditionalFormatting sqref="C6:C35 E6:H35">
     <cfRule type="iconSet" priority="2">
@@ -10199,53 +10424,53 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="80" t="s">
         <v>163</v>
       </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
-      <c r="L3" s="63"/>
-      <c r="M3" s="63"/>
-      <c r="N3" s="63"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="80"/>
+      <c r="L3" s="80"/>
+      <c r="M3" s="80"/>
+      <c r="N3" s="80"/>
     </row>
     <row r="4" spans="2:14" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="63"/>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63"/>
-      <c r="I4" s="63"/>
-      <c r="J4" s="63"/>
-      <c r="K4" s="63"/>
-      <c r="L4" s="63"/>
-      <c r="M4" s="63"/>
-      <c r="N4" s="63"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="80"/>
+      <c r="K4" s="80"/>
+      <c r="L4" s="80"/>
+      <c r="M4" s="80"/>
+      <c r="N4" s="80"/>
     </row>
     <row r="5" spans="2:14" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D5" s="64" t="s">
+      <c r="D5" s="81" t="s">
         <v>164</v>
       </c>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="67" t="s">
+      <c r="E5" s="82"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="82"/>
+      <c r="H5" s="82"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="84" t="s">
         <v>165</v>
       </c>
-      <c r="K5" s="67"/>
-      <c r="L5" s="67"/>
-      <c r="M5" s="67"/>
-      <c r="N5" s="67"/>
+      <c r="K5" s="84"/>
+      <c r="L5" s="84"/>
+      <c r="M5" s="84"/>
+      <c r="N5" s="84"/>
     </row>
     <row r="6" spans="2:14" s="29" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C6" s="36" t="s">
@@ -10286,7 +10511,7 @@
       </c>
     </row>
     <row r="7" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="68" t="s">
+      <c r="B7" s="85" t="s">
         <v>155</v>
       </c>
       <c r="C7" s="39" t="s">
@@ -10305,7 +10530,7 @@
       <c r="N7" s="30"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B8" s="60"/>
+      <c r="B8" s="77"/>
       <c r="C8" s="39" t="s">
         <v>174</v>
       </c>
@@ -10322,7 +10547,7 @@
       <c r="N8" s="30"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B9" s="60"/>
+      <c r="B9" s="77"/>
       <c r="C9" s="39" t="s">
         <v>175</v>
       </c>
@@ -10339,7 +10564,7 @@
       <c r="N9" s="30"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B10" s="60"/>
+      <c r="B10" s="77"/>
       <c r="C10" s="39" t="s">
         <v>176</v>
       </c>
@@ -10356,7 +10581,7 @@
       <c r="N10" s="30"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B11" s="60"/>
+      <c r="B11" s="77"/>
       <c r="C11" s="39" t="s">
         <v>177</v>
       </c>
@@ -10373,7 +10598,7 @@
       <c r="N11" s="30"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B12" s="60"/>
+      <c r="B12" s="77"/>
       <c r="C12" s="39" t="s">
         <v>178</v>
       </c>
@@ -10390,7 +10615,7 @@
       <c r="N12" s="30"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B13" s="60"/>
+      <c r="B13" s="77"/>
       <c r="C13" s="39" t="s">
         <v>179</v>
       </c>
@@ -10407,7 +10632,7 @@
       <c r="N13" s="30"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B14" s="60"/>
+      <c r="B14" s="77"/>
       <c r="C14" s="39" t="s">
         <v>180</v>
       </c>
@@ -10424,7 +10649,7 @@
       <c r="N14" s="30"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B15" s="60"/>
+      <c r="B15" s="77"/>
       <c r="C15" s="39" t="s">
         <v>181</v>
       </c>
@@ -10441,7 +10666,7 @@
       <c r="N15" s="30"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B16" s="60"/>
+      <c r="B16" s="77"/>
       <c r="C16" s="39" t="s">
         <v>182</v>
       </c>
@@ -10458,7 +10683,7 @@
       <c r="N16" s="30"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B17" s="60"/>
+      <c r="B17" s="77"/>
       <c r="C17" s="39" t="s">
         <v>183</v>
       </c>
@@ -10475,7 +10700,7 @@
       <c r="N17" s="30"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B18" s="60"/>
+      <c r="B18" s="77"/>
       <c r="C18" s="39" t="s">
         <v>184</v>
       </c>
@@ -10492,7 +10717,7 @@
       <c r="N18" s="30"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B19" s="60"/>
+      <c r="B19" s="77"/>
       <c r="C19" s="39" t="s">
         <v>185</v>
       </c>
@@ -10509,7 +10734,7 @@
       <c r="N19" s="30"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B20" s="60"/>
+      <c r="B20" s="77"/>
       <c r="C20" s="39" t="s">
         <v>186</v>
       </c>
@@ -10526,7 +10751,7 @@
       <c r="N20" s="30"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B21" s="60"/>
+      <c r="B21" s="77"/>
       <c r="C21" s="39" t="s">
         <v>187</v>
       </c>
@@ -10543,7 +10768,7 @@
       <c r="N21" s="30"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B22" s="60"/>
+      <c r="B22" s="77"/>
       <c r="C22" s="39" t="s">
         <v>188</v>
       </c>
@@ -10560,7 +10785,7 @@
       <c r="N22" s="30"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B23" s="60"/>
+      <c r="B23" s="77"/>
       <c r="C23" s="39" t="s">
         <v>189</v>
       </c>
@@ -10577,7 +10802,7 @@
       <c r="N23" s="30"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B24" s="60"/>
+      <c r="B24" s="77"/>
       <c r="C24" s="39" t="s">
         <v>190</v>
       </c>
@@ -10594,7 +10819,7 @@
       <c r="N24" s="30"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B25" s="60"/>
+      <c r="B25" s="77"/>
       <c r="C25" s="39" t="s">
         <v>191</v>
       </c>
@@ -10611,7 +10836,7 @@
       <c r="N25" s="30"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B26" s="60"/>
+      <c r="B26" s="77"/>
       <c r="C26" s="39" t="s">
         <v>192</v>
       </c>
@@ -10628,7 +10853,7 @@
       <c r="N26" s="30"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B27" s="60"/>
+      <c r="B27" s="77"/>
       <c r="C27" s="39" t="s">
         <v>193</v>
       </c>
@@ -10645,7 +10870,7 @@
       <c r="N27" s="30"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B28" s="60"/>
+      <c r="B28" s="77"/>
       <c r="C28" s="39" t="s">
         <v>194</v>
       </c>
@@ -10662,7 +10887,7 @@
       <c r="N28" s="30"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B29" s="60"/>
+      <c r="B29" s="77"/>
       <c r="C29" s="39" t="s">
         <v>195</v>
       </c>
@@ -10679,7 +10904,7 @@
       <c r="N29" s="30"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B30" s="60"/>
+      <c r="B30" s="77"/>
       <c r="C30" s="39" t="s">
         <v>196</v>
       </c>
@@ -10696,7 +10921,7 @@
       <c r="N30" s="30"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B31" s="60"/>
+      <c r="B31" s="77"/>
       <c r="C31" s="39" t="s">
         <v>197</v>
       </c>
@@ -10713,7 +10938,7 @@
       <c r="N31" s="30"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B32" s="60"/>
+      <c r="B32" s="77"/>
       <c r="C32" s="39" t="s">
         <v>198</v>
       </c>
@@ -10730,7 +10955,7 @@
       <c r="N32" s="30"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B33" s="60"/>
+      <c r="B33" s="77"/>
       <c r="C33" s="39" t="s">
         <v>198</v>
       </c>
@@ -10747,7 +10972,7 @@
       <c r="N33" s="30"/>
     </row>
     <row r="34" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B34" s="61"/>
+      <c r="B34" s="78"/>
       <c r="C34" s="40" t="s">
         <v>198</v>
       </c>
@@ -10764,7 +10989,7 @@
       <c r="N34" s="31"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B35" s="59" t="s">
+      <c r="B35" s="76" t="s">
         <v>156</v>
       </c>
       <c r="C35" s="39" t="s">
@@ -10783,7 +11008,7 @@
       <c r="N35" s="30"/>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B36" s="60"/>
+      <c r="B36" s="77"/>
       <c r="C36" s="39" t="s">
         <v>174</v>
       </c>
@@ -10800,7 +11025,7 @@
       <c r="N36" s="30"/>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B37" s="60"/>
+      <c r="B37" s="77"/>
       <c r="C37" s="39" t="s">
         <v>175</v>
       </c>
@@ -10817,7 +11042,7 @@
       <c r="N37" s="30"/>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B38" s="60"/>
+      <c r="B38" s="77"/>
       <c r="C38" s="39" t="s">
         <v>176</v>
       </c>
@@ -10834,7 +11059,7 @@
       <c r="N38" s="30"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B39" s="60"/>
+      <c r="B39" s="77"/>
       <c r="C39" s="39" t="s">
         <v>177</v>
       </c>
@@ -10851,7 +11076,7 @@
       <c r="N39" s="30"/>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B40" s="60"/>
+      <c r="B40" s="77"/>
       <c r="C40" s="39" t="s">
         <v>178</v>
       </c>
@@ -10868,7 +11093,7 @@
       <c r="N40" s="30"/>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B41" s="60"/>
+      <c r="B41" s="77"/>
       <c r="C41" s="39" t="s">
         <v>179</v>
       </c>
@@ -10885,7 +11110,7 @@
       <c r="N41" s="30"/>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B42" s="60"/>
+      <c r="B42" s="77"/>
       <c r="C42" s="39" t="s">
         <v>180</v>
       </c>
@@ -10902,7 +11127,7 @@
       <c r="N42" s="30"/>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B43" s="60"/>
+      <c r="B43" s="77"/>
       <c r="C43" s="39" t="s">
         <v>181</v>
       </c>
@@ -10919,7 +11144,7 @@
       <c r="N43" s="30"/>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B44" s="60"/>
+      <c r="B44" s="77"/>
       <c r="C44" s="39" t="s">
         <v>182</v>
       </c>
@@ -10936,7 +11161,7 @@
       <c r="N44" s="30"/>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B45" s="60"/>
+      <c r="B45" s="77"/>
       <c r="C45" s="39" t="s">
         <v>183</v>
       </c>
@@ -10953,7 +11178,7 @@
       <c r="N45" s="30"/>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B46" s="60"/>
+      <c r="B46" s="77"/>
       <c r="C46" s="39" t="s">
         <v>184</v>
       </c>
@@ -10970,7 +11195,7 @@
       <c r="N46" s="30"/>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B47" s="60"/>
+      <c r="B47" s="77"/>
       <c r="C47" s="39" t="s">
         <v>185</v>
       </c>
@@ -10987,7 +11212,7 @@
       <c r="N47" s="30"/>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B48" s="60"/>
+      <c r="B48" s="77"/>
       <c r="C48" s="39" t="s">
         <v>186</v>
       </c>
@@ -11004,7 +11229,7 @@
       <c r="N48" s="30"/>
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B49" s="60"/>
+      <c r="B49" s="77"/>
       <c r="C49" s="39" t="s">
         <v>187</v>
       </c>
@@ -11021,7 +11246,7 @@
       <c r="N49" s="30"/>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B50" s="60"/>
+      <c r="B50" s="77"/>
       <c r="C50" s="39" t="s">
         <v>188</v>
       </c>
@@ -11038,7 +11263,7 @@
       <c r="N50" s="30"/>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B51" s="60"/>
+      <c r="B51" s="77"/>
       <c r="C51" s="39" t="s">
         <v>189</v>
       </c>
@@ -11055,7 +11280,7 @@
       <c r="N51" s="30"/>
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B52" s="60"/>
+      <c r="B52" s="77"/>
       <c r="C52" s="39" t="s">
         <v>190</v>
       </c>
@@ -11072,7 +11297,7 @@
       <c r="N52" s="30"/>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B53" s="60"/>
+      <c r="B53" s="77"/>
       <c r="C53" s="39" t="s">
         <v>191</v>
       </c>
@@ -11089,7 +11314,7 @@
       <c r="N53" s="30"/>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B54" s="60"/>
+      <c r="B54" s="77"/>
       <c r="C54" s="39" t="s">
         <v>192</v>
       </c>
@@ -11106,7 +11331,7 @@
       <c r="N54" s="30"/>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B55" s="60"/>
+      <c r="B55" s="77"/>
       <c r="C55" s="39" t="s">
         <v>193</v>
       </c>
@@ -11123,7 +11348,7 @@
       <c r="N55" s="30"/>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B56" s="60"/>
+      <c r="B56" s="77"/>
       <c r="C56" s="39" t="s">
         <v>194</v>
       </c>
@@ -11140,7 +11365,7 @@
       <c r="N56" s="30"/>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B57" s="60"/>
+      <c r="B57" s="77"/>
       <c r="C57" s="39" t="s">
         <v>195</v>
       </c>
@@ -11157,7 +11382,7 @@
       <c r="N57" s="30"/>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B58" s="60"/>
+      <c r="B58" s="77"/>
       <c r="C58" s="39" t="s">
         <v>196</v>
       </c>
@@ -11174,7 +11399,7 @@
       <c r="N58" s="30"/>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B59" s="60"/>
+      <c r="B59" s="77"/>
       <c r="C59" s="39" t="s">
         <v>197</v>
       </c>
@@ -11191,7 +11416,7 @@
       <c r="N59" s="30"/>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B60" s="60"/>
+      <c r="B60" s="77"/>
       <c r="C60" s="39" t="s">
         <v>198</v>
       </c>
@@ -11208,7 +11433,7 @@
       <c r="N60" s="30"/>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B61" s="60"/>
+      <c r="B61" s="77"/>
       <c r="C61" s="39" t="s">
         <v>198</v>
       </c>
@@ -11225,7 +11450,7 @@
       <c r="N61" s="30"/>
     </row>
     <row r="62" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B62" s="61"/>
+      <c r="B62" s="78"/>
       <c r="C62" s="40" t="s">
         <v>198</v>
       </c>
@@ -11242,7 +11467,7 @@
       <c r="N62" s="31"/>
     </row>
     <row r="63" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B63" s="59" t="s">
+      <c r="B63" s="76" t="s">
         <v>157</v>
       </c>
       <c r="C63" s="39" t="s">
@@ -11261,7 +11486,7 @@
       <c r="N63" s="30"/>
     </row>
     <row r="64" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B64" s="60"/>
+      <c r="B64" s="77"/>
       <c r="C64" s="39" t="s">
         <v>174</v>
       </c>
@@ -11278,7 +11503,7 @@
       <c r="N64" s="30"/>
     </row>
     <row r="65" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B65" s="60"/>
+      <c r="B65" s="77"/>
       <c r="C65" s="39" t="s">
         <v>175</v>
       </c>
@@ -11295,7 +11520,7 @@
       <c r="N65" s="30"/>
     </row>
     <row r="66" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B66" s="60"/>
+      <c r="B66" s="77"/>
       <c r="C66" s="39" t="s">
         <v>176</v>
       </c>
@@ -11312,7 +11537,7 @@
       <c r="N66" s="30"/>
     </row>
     <row r="67" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B67" s="60"/>
+      <c r="B67" s="77"/>
       <c r="C67" s="39" t="s">
         <v>177</v>
       </c>
@@ -11329,7 +11554,7 @@
       <c r="N67" s="30"/>
     </row>
     <row r="68" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B68" s="60"/>
+      <c r="B68" s="77"/>
       <c r="C68" s="39" t="s">
         <v>178</v>
       </c>
@@ -11346,7 +11571,7 @@
       <c r="N68" s="30"/>
     </row>
     <row r="69" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B69" s="60"/>
+      <c r="B69" s="77"/>
       <c r="C69" s="39" t="s">
         <v>179</v>
       </c>
@@ -11363,7 +11588,7 @@
       <c r="N69" s="30"/>
     </row>
     <row r="70" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B70" s="60"/>
+      <c r="B70" s="77"/>
       <c r="C70" s="39" t="s">
         <v>180</v>
       </c>
@@ -11380,7 +11605,7 @@
       <c r="N70" s="30"/>
     </row>
     <row r="71" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B71" s="60"/>
+      <c r="B71" s="77"/>
       <c r="C71" s="39" t="s">
         <v>181</v>
       </c>
@@ -11397,7 +11622,7 @@
       <c r="N71" s="30"/>
     </row>
     <row r="72" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B72" s="60"/>
+      <c r="B72" s="77"/>
       <c r="C72" s="39" t="s">
         <v>182</v>
       </c>
@@ -11414,7 +11639,7 @@
       <c r="N72" s="30"/>
     </row>
     <row r="73" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B73" s="60"/>
+      <c r="B73" s="77"/>
       <c r="C73" s="39" t="s">
         <v>183</v>
       </c>
@@ -11431,7 +11656,7 @@
       <c r="N73" s="30"/>
     </row>
     <row r="74" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B74" s="60"/>
+      <c r="B74" s="77"/>
       <c r="C74" s="39" t="s">
         <v>184</v>
       </c>
@@ -11448,7 +11673,7 @@
       <c r="N74" s="30"/>
     </row>
     <row r="75" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B75" s="60"/>
+      <c r="B75" s="77"/>
       <c r="C75" s="39" t="s">
         <v>185</v>
       </c>
@@ -11465,7 +11690,7 @@
       <c r="N75" s="30"/>
     </row>
     <row r="76" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B76" s="60"/>
+      <c r="B76" s="77"/>
       <c r="C76" s="39" t="s">
         <v>186</v>
       </c>
@@ -11482,7 +11707,7 @@
       <c r="N76" s="30"/>
     </row>
     <row r="77" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B77" s="60"/>
+      <c r="B77" s="77"/>
       <c r="C77" s="39" t="s">
         <v>187</v>
       </c>
@@ -11499,7 +11724,7 @@
       <c r="N77" s="30"/>
     </row>
     <row r="78" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B78" s="60"/>
+      <c r="B78" s="77"/>
       <c r="C78" s="39" t="s">
         <v>188</v>
       </c>
@@ -11516,7 +11741,7 @@
       <c r="N78" s="30"/>
     </row>
     <row r="79" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B79" s="60"/>
+      <c r="B79" s="77"/>
       <c r="C79" s="39" t="s">
         <v>189</v>
       </c>
@@ -11533,7 +11758,7 @@
       <c r="N79" s="30"/>
     </row>
     <row r="80" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B80" s="60"/>
+      <c r="B80" s="77"/>
       <c r="C80" s="39" t="s">
         <v>190</v>
       </c>
@@ -11550,7 +11775,7 @@
       <c r="N80" s="30"/>
     </row>
     <row r="81" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B81" s="60"/>
+      <c r="B81" s="77"/>
       <c r="C81" s="39" t="s">
         <v>191</v>
       </c>
@@ -11567,7 +11792,7 @@
       <c r="N81" s="30"/>
     </row>
     <row r="82" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B82" s="60"/>
+      <c r="B82" s="77"/>
       <c r="C82" s="39" t="s">
         <v>192</v>
       </c>
@@ -11584,7 +11809,7 @@
       <c r="N82" s="30"/>
     </row>
     <row r="83" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B83" s="60"/>
+      <c r="B83" s="77"/>
       <c r="C83" s="39" t="s">
         <v>193</v>
       </c>
@@ -11601,7 +11826,7 @@
       <c r="N83" s="30"/>
     </row>
     <row r="84" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B84" s="60"/>
+      <c r="B84" s="77"/>
       <c r="C84" s="39" t="s">
         <v>194</v>
       </c>
@@ -11618,7 +11843,7 @@
       <c r="N84" s="30"/>
     </row>
     <row r="85" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B85" s="60"/>
+      <c r="B85" s="77"/>
       <c r="C85" s="39" t="s">
         <v>195</v>
       </c>
@@ -11635,7 +11860,7 @@
       <c r="N85" s="30"/>
     </row>
     <row r="86" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B86" s="60"/>
+      <c r="B86" s="77"/>
       <c r="C86" s="39" t="s">
         <v>196</v>
       </c>
@@ -11652,7 +11877,7 @@
       <c r="N86" s="30"/>
     </row>
     <row r="87" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B87" s="60"/>
+      <c r="B87" s="77"/>
       <c r="C87" s="39" t="s">
         <v>197</v>
       </c>
@@ -11669,7 +11894,7 @@
       <c r="N87" s="30"/>
     </row>
     <row r="88" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B88" s="60"/>
+      <c r="B88" s="77"/>
       <c r="C88" s="39" t="s">
         <v>198</v>
       </c>
@@ -11686,7 +11911,7 @@
       <c r="N88" s="30"/>
     </row>
     <row r="89" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B89" s="60"/>
+      <c r="B89" s="77"/>
       <c r="C89" s="39" t="s">
         <v>198</v>
       </c>
@@ -11703,7 +11928,7 @@
       <c r="N89" s="30"/>
     </row>
     <row r="90" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B90" s="61"/>
+      <c r="B90" s="78"/>
       <c r="C90" s="40" t="s">
         <v>198</v>
       </c>
@@ -11720,7 +11945,7 @@
       <c r="N90" s="31"/>
     </row>
     <row r="91" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B91" s="59" t="s">
+      <c r="B91" s="76" t="s">
         <v>158</v>
       </c>
       <c r="C91" s="39" t="s">
@@ -11739,7 +11964,7 @@
       <c r="N91" s="30"/>
     </row>
     <row r="92" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B92" s="60"/>
+      <c r="B92" s="77"/>
       <c r="C92" s="39" t="s">
         <v>174</v>
       </c>
@@ -11756,7 +11981,7 @@
       <c r="N92" s="30"/>
     </row>
     <row r="93" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B93" s="60"/>
+      <c r="B93" s="77"/>
       <c r="C93" s="39" t="s">
         <v>175</v>
       </c>
@@ -11773,7 +11998,7 @@
       <c r="N93" s="30"/>
     </row>
     <row r="94" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B94" s="60"/>
+      <c r="B94" s="77"/>
       <c r="C94" s="39" t="s">
         <v>176</v>
       </c>
@@ -11790,7 +12015,7 @@
       <c r="N94" s="30"/>
     </row>
     <row r="95" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B95" s="60"/>
+      <c r="B95" s="77"/>
       <c r="C95" s="39" t="s">
         <v>177</v>
       </c>
@@ -11807,7 +12032,7 @@
       <c r="N95" s="30"/>
     </row>
     <row r="96" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B96" s="60"/>
+      <c r="B96" s="77"/>
       <c r="C96" s="39" t="s">
         <v>178</v>
       </c>
@@ -11824,7 +12049,7 @@
       <c r="N96" s="30"/>
     </row>
     <row r="97" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B97" s="60"/>
+      <c r="B97" s="77"/>
       <c r="C97" s="39" t="s">
         <v>179</v>
       </c>
@@ -11841,7 +12066,7 @@
       <c r="N97" s="30"/>
     </row>
     <row r="98" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B98" s="60"/>
+      <c r="B98" s="77"/>
       <c r="C98" s="39" t="s">
         <v>180</v>
       </c>
@@ -11858,7 +12083,7 @@
       <c r="N98" s="30"/>
     </row>
     <row r="99" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B99" s="60"/>
+      <c r="B99" s="77"/>
       <c r="C99" s="39" t="s">
         <v>181</v>
       </c>
@@ -11875,7 +12100,7 @@
       <c r="N99" s="30"/>
     </row>
     <row r="100" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B100" s="60"/>
+      <c r="B100" s="77"/>
       <c r="C100" s="39" t="s">
         <v>182</v>
       </c>
@@ -11892,7 +12117,7 @@
       <c r="N100" s="30"/>
     </row>
     <row r="101" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B101" s="60"/>
+      <c r="B101" s="77"/>
       <c r="C101" s="39" t="s">
         <v>183</v>
       </c>
@@ -11909,7 +12134,7 @@
       <c r="N101" s="30"/>
     </row>
     <row r="102" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B102" s="60"/>
+      <c r="B102" s="77"/>
       <c r="C102" s="39" t="s">
         <v>184</v>
       </c>
@@ -11926,7 +12151,7 @@
       <c r="N102" s="30"/>
     </row>
     <row r="103" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B103" s="60"/>
+      <c r="B103" s="77"/>
       <c r="C103" s="39" t="s">
         <v>185</v>
       </c>
@@ -11943,7 +12168,7 @@
       <c r="N103" s="30"/>
     </row>
     <row r="104" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B104" s="60"/>
+      <c r="B104" s="77"/>
       <c r="C104" s="39" t="s">
         <v>186</v>
       </c>
@@ -11960,7 +12185,7 @@
       <c r="N104" s="30"/>
     </row>
     <row r="105" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B105" s="60"/>
+      <c r="B105" s="77"/>
       <c r="C105" s="39" t="s">
         <v>187</v>
       </c>
@@ -11977,7 +12202,7 @@
       <c r="N105" s="30"/>
     </row>
     <row r="106" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B106" s="60"/>
+      <c r="B106" s="77"/>
       <c r="C106" s="39" t="s">
         <v>188</v>
       </c>
@@ -11994,7 +12219,7 @@
       <c r="N106" s="30"/>
     </row>
     <row r="107" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B107" s="60"/>
+      <c r="B107" s="77"/>
       <c r="C107" s="39" t="s">
         <v>189</v>
       </c>
@@ -12011,7 +12236,7 @@
       <c r="N107" s="30"/>
     </row>
     <row r="108" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B108" s="60"/>
+      <c r="B108" s="77"/>
       <c r="C108" s="39" t="s">
         <v>190</v>
       </c>
@@ -12028,7 +12253,7 @@
       <c r="N108" s="30"/>
     </row>
     <row r="109" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B109" s="60"/>
+      <c r="B109" s="77"/>
       <c r="C109" s="39" t="s">
         <v>191</v>
       </c>
@@ -12045,7 +12270,7 @@
       <c r="N109" s="30"/>
     </row>
     <row r="110" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B110" s="60"/>
+      <c r="B110" s="77"/>
       <c r="C110" s="39" t="s">
         <v>192</v>
       </c>
@@ -12062,7 +12287,7 @@
       <c r="N110" s="30"/>
     </row>
     <row r="111" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B111" s="60"/>
+      <c r="B111" s="77"/>
       <c r="C111" s="39" t="s">
         <v>193</v>
       </c>
@@ -12079,7 +12304,7 @@
       <c r="N111" s="30"/>
     </row>
     <row r="112" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B112" s="60"/>
+      <c r="B112" s="77"/>
       <c r="C112" s="39" t="s">
         <v>194</v>
       </c>
@@ -12096,7 +12321,7 @@
       <c r="N112" s="30"/>
     </row>
     <row r="113" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B113" s="60"/>
+      <c r="B113" s="77"/>
       <c r="C113" s="39" t="s">
         <v>195</v>
       </c>
@@ -12113,7 +12338,7 @@
       <c r="N113" s="30"/>
     </row>
     <row r="114" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B114" s="60"/>
+      <c r="B114" s="77"/>
       <c r="C114" s="39" t="s">
         <v>196</v>
       </c>
@@ -12130,7 +12355,7 @@
       <c r="N114" s="30"/>
     </row>
     <row r="115" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B115" s="60"/>
+      <c r="B115" s="77"/>
       <c r="C115" s="39" t="s">
         <v>197</v>
       </c>
@@ -12147,7 +12372,7 @@
       <c r="N115" s="30"/>
     </row>
     <row r="116" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B116" s="60"/>
+      <c r="B116" s="77"/>
       <c r="C116" s="39" t="s">
         <v>198</v>
       </c>
@@ -12164,7 +12389,7 @@
       <c r="N116" s="30"/>
     </row>
     <row r="117" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B117" s="60"/>
+      <c r="B117" s="77"/>
       <c r="C117" s="39" t="s">
         <v>198</v>
       </c>
@@ -12181,7 +12406,7 @@
       <c r="N117" s="30"/>
     </row>
     <row r="118" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B118" s="61"/>
+      <c r="B118" s="78"/>
       <c r="C118" s="40" t="s">
         <v>198</v>
       </c>
@@ -12198,7 +12423,7 @@
       <c r="N118" s="31"/>
     </row>
     <row r="119" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B119" s="59" t="s">
+      <c r="B119" s="76" t="s">
         <v>159</v>
       </c>
       <c r="C119" s="39" t="s">
@@ -12217,7 +12442,7 @@
       <c r="N119" s="30"/>
     </row>
     <row r="120" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B120" s="60"/>
+      <c r="B120" s="77"/>
       <c r="C120" s="39" t="s">
         <v>174</v>
       </c>
@@ -12234,7 +12459,7 @@
       <c r="N120" s="30"/>
     </row>
     <row r="121" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B121" s="60"/>
+      <c r="B121" s="77"/>
       <c r="C121" s="39" t="s">
         <v>175</v>
       </c>
@@ -12251,7 +12476,7 @@
       <c r="N121" s="30"/>
     </row>
     <row r="122" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B122" s="60"/>
+      <c r="B122" s="77"/>
       <c r="C122" s="39" t="s">
         <v>176</v>
       </c>
@@ -12268,7 +12493,7 @@
       <c r="N122" s="30"/>
     </row>
     <row r="123" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B123" s="60"/>
+      <c r="B123" s="77"/>
       <c r="C123" s="39" t="s">
         <v>177</v>
       </c>
@@ -12285,7 +12510,7 @@
       <c r="N123" s="30"/>
     </row>
     <row r="124" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B124" s="60"/>
+      <c r="B124" s="77"/>
       <c r="C124" s="39" t="s">
         <v>178</v>
       </c>
@@ -12302,7 +12527,7 @@
       <c r="N124" s="30"/>
     </row>
     <row r="125" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B125" s="60"/>
+      <c r="B125" s="77"/>
       <c r="C125" s="39" t="s">
         <v>179</v>
       </c>
@@ -12319,7 +12544,7 @@
       <c r="N125" s="30"/>
     </row>
     <row r="126" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B126" s="60"/>
+      <c r="B126" s="77"/>
       <c r="C126" s="39" t="s">
         <v>180</v>
       </c>
@@ -12336,7 +12561,7 @@
       <c r="N126" s="30"/>
     </row>
     <row r="127" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B127" s="60"/>
+      <c r="B127" s="77"/>
       <c r="C127" s="39" t="s">
         <v>181</v>
       </c>
@@ -12353,7 +12578,7 @@
       <c r="N127" s="30"/>
     </row>
     <row r="128" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B128" s="60"/>
+      <c r="B128" s="77"/>
       <c r="C128" s="39" t="s">
         <v>182</v>
       </c>
@@ -12370,7 +12595,7 @@
       <c r="N128" s="30"/>
     </row>
     <row r="129" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B129" s="60"/>
+      <c r="B129" s="77"/>
       <c r="C129" s="39" t="s">
         <v>183</v>
       </c>
@@ -12387,7 +12612,7 @@
       <c r="N129" s="30"/>
     </row>
     <row r="130" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B130" s="60"/>
+      <c r="B130" s="77"/>
       <c r="C130" s="39" t="s">
         <v>184</v>
       </c>
@@ -12404,7 +12629,7 @@
       <c r="N130" s="30"/>
     </row>
     <row r="131" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B131" s="60"/>
+      <c r="B131" s="77"/>
       <c r="C131" s="39" t="s">
         <v>185</v>
       </c>
@@ -12421,7 +12646,7 @@
       <c r="N131" s="30"/>
     </row>
     <row r="132" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B132" s="60"/>
+      <c r="B132" s="77"/>
       <c r="C132" s="39" t="s">
         <v>186</v>
       </c>
@@ -12438,7 +12663,7 @@
       <c r="N132" s="30"/>
     </row>
     <row r="133" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B133" s="60"/>
+      <c r="B133" s="77"/>
       <c r="C133" s="39" t="s">
         <v>187</v>
       </c>
@@ -12455,7 +12680,7 @@
       <c r="N133" s="30"/>
     </row>
     <row r="134" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B134" s="60"/>
+      <c r="B134" s="77"/>
       <c r="C134" s="39" t="s">
         <v>188</v>
       </c>
@@ -12472,7 +12697,7 @@
       <c r="N134" s="30"/>
     </row>
     <row r="135" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B135" s="60"/>
+      <c r="B135" s="77"/>
       <c r="C135" s="39" t="s">
         <v>189</v>
       </c>
@@ -12489,7 +12714,7 @@
       <c r="N135" s="30"/>
     </row>
     <row r="136" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B136" s="60"/>
+      <c r="B136" s="77"/>
       <c r="C136" s="39" t="s">
         <v>190</v>
       </c>
@@ -12506,7 +12731,7 @@
       <c r="N136" s="30"/>
     </row>
     <row r="137" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B137" s="60"/>
+      <c r="B137" s="77"/>
       <c r="C137" s="39" t="s">
         <v>191</v>
       </c>
@@ -12523,7 +12748,7 @@
       <c r="N137" s="30"/>
     </row>
     <row r="138" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B138" s="60"/>
+      <c r="B138" s="77"/>
       <c r="C138" s="39" t="s">
         <v>192</v>
       </c>
@@ -12540,7 +12765,7 @@
       <c r="N138" s="30"/>
     </row>
     <row r="139" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B139" s="60"/>
+      <c r="B139" s="77"/>
       <c r="C139" s="39" t="s">
         <v>193</v>
       </c>
@@ -12557,7 +12782,7 @@
       <c r="N139" s="30"/>
     </row>
     <row r="140" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B140" s="60"/>
+      <c r="B140" s="77"/>
       <c r="C140" s="39" t="s">
         <v>194</v>
       </c>
@@ -12574,7 +12799,7 @@
       <c r="N140" s="30"/>
     </row>
     <row r="141" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B141" s="60"/>
+      <c r="B141" s="77"/>
       <c r="C141" s="39" t="s">
         <v>195</v>
       </c>
@@ -12591,7 +12816,7 @@
       <c r="N141" s="30"/>
     </row>
     <row r="142" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B142" s="60"/>
+      <c r="B142" s="77"/>
       <c r="C142" s="39" t="s">
         <v>196</v>
       </c>
@@ -12608,7 +12833,7 @@
       <c r="N142" s="30"/>
     </row>
     <row r="143" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B143" s="60"/>
+      <c r="B143" s="77"/>
       <c r="C143" s="39" t="s">
         <v>197</v>
       </c>
@@ -12625,7 +12850,7 @@
       <c r="N143" s="30"/>
     </row>
     <row r="144" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B144" s="60"/>
+      <c r="B144" s="77"/>
       <c r="C144" s="39" t="s">
         <v>198</v>
       </c>
@@ -12642,7 +12867,7 @@
       <c r="N144" s="30"/>
     </row>
     <row r="145" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B145" s="60"/>
+      <c r="B145" s="77"/>
       <c r="C145" s="39" t="s">
         <v>198</v>
       </c>
@@ -12659,7 +12884,7 @@
       <c r="N145" s="30"/>
     </row>
     <row r="146" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B146" s="61"/>
+      <c r="B146" s="78"/>
       <c r="C146" s="40" t="s">
         <v>198</v>
       </c>
@@ -12676,7 +12901,7 @@
       <c r="N146" s="31"/>
     </row>
     <row r="147" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B147" s="59" t="s">
+      <c r="B147" s="76" t="s">
         <v>160</v>
       </c>
       <c r="C147" s="39" t="s">
@@ -12695,7 +12920,7 @@
       <c r="N147" s="30"/>
     </row>
     <row r="148" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B148" s="60"/>
+      <c r="B148" s="77"/>
       <c r="C148" s="39" t="s">
         <v>174</v>
       </c>
@@ -12712,7 +12937,7 @@
       <c r="N148" s="30"/>
     </row>
     <row r="149" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B149" s="60"/>
+      <c r="B149" s="77"/>
       <c r="C149" s="39" t="s">
         <v>175</v>
       </c>
@@ -12729,7 +12954,7 @@
       <c r="N149" s="30"/>
     </row>
     <row r="150" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B150" s="60"/>
+      <c r="B150" s="77"/>
       <c r="C150" s="39" t="s">
         <v>176</v>
       </c>
@@ -12746,7 +12971,7 @@
       <c r="N150" s="30"/>
     </row>
     <row r="151" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B151" s="60"/>
+      <c r="B151" s="77"/>
       <c r="C151" s="39" t="s">
         <v>177</v>
       </c>
@@ -12763,7 +12988,7 @@
       <c r="N151" s="30"/>
     </row>
     <row r="152" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B152" s="60"/>
+      <c r="B152" s="77"/>
       <c r="C152" s="39" t="s">
         <v>178</v>
       </c>
@@ -12780,7 +13005,7 @@
       <c r="N152" s="30"/>
     </row>
     <row r="153" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B153" s="60"/>
+      <c r="B153" s="77"/>
       <c r="C153" s="39" t="s">
         <v>179</v>
       </c>
@@ -12797,7 +13022,7 @@
       <c r="N153" s="30"/>
     </row>
     <row r="154" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B154" s="60"/>
+      <c r="B154" s="77"/>
       <c r="C154" s="39" t="s">
         <v>180</v>
       </c>
@@ -12814,7 +13039,7 @@
       <c r="N154" s="30"/>
     </row>
     <row r="155" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B155" s="60"/>
+      <c r="B155" s="77"/>
       <c r="C155" s="39" t="s">
         <v>181</v>
       </c>
@@ -12831,7 +13056,7 @@
       <c r="N155" s="30"/>
     </row>
     <row r="156" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B156" s="60"/>
+      <c r="B156" s="77"/>
       <c r="C156" s="39" t="s">
         <v>182</v>
       </c>
@@ -12848,7 +13073,7 @@
       <c r="N156" s="30"/>
     </row>
     <row r="157" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B157" s="60"/>
+      <c r="B157" s="77"/>
       <c r="C157" s="39" t="s">
         <v>183</v>
       </c>
@@ -12865,7 +13090,7 @@
       <c r="N157" s="30"/>
     </row>
     <row r="158" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B158" s="60"/>
+      <c r="B158" s="77"/>
       <c r="C158" s="39" t="s">
         <v>184</v>
       </c>
@@ -12882,7 +13107,7 @@
       <c r="N158" s="30"/>
     </row>
     <row r="159" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B159" s="60"/>
+      <c r="B159" s="77"/>
       <c r="C159" s="39" t="s">
         <v>185</v>
       </c>
@@ -12899,7 +13124,7 @@
       <c r="N159" s="30"/>
     </row>
     <row r="160" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B160" s="60"/>
+      <c r="B160" s="77"/>
       <c r="C160" s="39" t="s">
         <v>186</v>
       </c>
@@ -12916,7 +13141,7 @@
       <c r="N160" s="30"/>
     </row>
     <row r="161" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B161" s="60"/>
+      <c r="B161" s="77"/>
       <c r="C161" s="39" t="s">
         <v>187</v>
       </c>
@@ -12933,7 +13158,7 @@
       <c r="N161" s="30"/>
     </row>
     <row r="162" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B162" s="60"/>
+      <c r="B162" s="77"/>
       <c r="C162" s="39" t="s">
         <v>188</v>
       </c>
@@ -12950,7 +13175,7 @@
       <c r="N162" s="30"/>
     </row>
     <row r="163" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B163" s="60"/>
+      <c r="B163" s="77"/>
       <c r="C163" s="39" t="s">
         <v>189</v>
       </c>
@@ -12967,7 +13192,7 @@
       <c r="N163" s="30"/>
     </row>
     <row r="164" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B164" s="60"/>
+      <c r="B164" s="77"/>
       <c r="C164" s="39" t="s">
         <v>190</v>
       </c>
@@ -12984,7 +13209,7 @@
       <c r="N164" s="30"/>
     </row>
     <row r="165" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B165" s="60"/>
+      <c r="B165" s="77"/>
       <c r="C165" s="39" t="s">
         <v>191</v>
       </c>
@@ -13001,7 +13226,7 @@
       <c r="N165" s="30"/>
     </row>
     <row r="166" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B166" s="60"/>
+      <c r="B166" s="77"/>
       <c r="C166" s="39" t="s">
         <v>192</v>
       </c>
@@ -13018,7 +13243,7 @@
       <c r="N166" s="30"/>
     </row>
     <row r="167" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B167" s="60"/>
+      <c r="B167" s="77"/>
       <c r="C167" s="39" t="s">
         <v>193</v>
       </c>
@@ -13035,7 +13260,7 @@
       <c r="N167" s="30"/>
     </row>
     <row r="168" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B168" s="60"/>
+      <c r="B168" s="77"/>
       <c r="C168" s="39" t="s">
         <v>194</v>
       </c>
@@ -13052,7 +13277,7 @@
       <c r="N168" s="30"/>
     </row>
     <row r="169" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B169" s="60"/>
+      <c r="B169" s="77"/>
       <c r="C169" s="39" t="s">
         <v>195</v>
       </c>
@@ -13069,7 +13294,7 @@
       <c r="N169" s="30"/>
     </row>
     <row r="170" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B170" s="60"/>
+      <c r="B170" s="77"/>
       <c r="C170" s="39" t="s">
         <v>196</v>
       </c>
@@ -13086,7 +13311,7 @@
       <c r="N170" s="30"/>
     </row>
     <row r="171" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B171" s="60"/>
+      <c r="B171" s="77"/>
       <c r="C171" s="39" t="s">
         <v>197</v>
       </c>
@@ -13103,7 +13328,7 @@
       <c r="N171" s="30"/>
     </row>
     <row r="172" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B172" s="60"/>
+      <c r="B172" s="77"/>
       <c r="C172" s="39" t="s">
         <v>198</v>
       </c>
@@ -13120,7 +13345,7 @@
       <c r="N172" s="30"/>
     </row>
     <row r="173" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B173" s="60"/>
+      <c r="B173" s="77"/>
       <c r="C173" s="39" t="s">
         <v>198</v>
       </c>
@@ -13137,7 +13362,7 @@
       <c r="N173" s="30"/>
     </row>
     <row r="174" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B174" s="62"/>
+      <c r="B174" s="79"/>
       <c r="C174" s="41" t="s">
         <v>198</v>
       </c>
@@ -13306,16 +13531,16 @@
       <c r="I3"/>
     </row>
     <row r="4" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="69" t="s">
+      <c r="C4" s="86" t="s">
         <v>199</v>
       </c>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="69"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
     </row>
     <row r="5" spans="1:10" ht="104.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="20" t="s">

</xml_diff>

<commit_message>
Run and add GridSearch results and 1st Submission
</commit_message>
<xml_diff>
--- a/ML_Excel_ReportResults.xlsx
+++ b/ML_Excel_ReportResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveeduisegiunl-my.sharepoint.com/personal/20240502_novaims_unl_pt/Documents/MDSAA-DS_1ºAno/1º Semestre/2_Machine Learning_[ML]/[ML]_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2250" documentId="8_{617E8CF7-4F71-4121-97E1-8CD89EF3D5D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BE85228-BE92-4218-ABA5-5140CBF57262}"/>
+  <xr:revisionPtr revIDLastSave="2262" documentId="8_{617E8CF7-4F71-4121-97E1-8CD89EF3D5D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C912384-2484-4E01-ABAF-D80C50DAB6D8}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{B50C4AD8-7853-4F6B-84A1-47D583CD2B87}"/>
   </bookViews>
@@ -102,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1331" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1345" uniqueCount="345">
   <si>
     <t>Wrapper Methods | RFE</t>
   </si>
@@ -1774,12 +1774,6 @@
     <t xml:space="preserve"> This analysis aimed to see how these techniques influence the feature selection and model performance. The coefficients were rounded to 1 decimal place.</t>
   </si>
   <si>
-    <t>The team members applied various models on their own set of features and reported the results below.</t>
-  </si>
-  <si>
-    <t>Final Decision (11.11.2024)</t>
-  </si>
-  <si>
     <t>Final Decision*</t>
   </si>
   <si>
@@ -1796,6 +1790,54 @@
       </rPr>
       <t>Until 11.11.2024, these were the variables chosen based on the table at the end of 2nd notebook</t>
     </r>
+  </si>
+  <si>
+    <t>The team members applied various models on their own set of features and reported the results below,</t>
+  </si>
+  <si>
+    <t>Final Decision (11,11,2024)</t>
+  </si>
+  <si>
+    <t>33,28 +/-0,23</t>
+  </si>
+  <si>
+    <t>26,71 +/-0,25</t>
+  </si>
+  <si>
+    <t>30,14 +/-0,08</t>
+  </si>
+  <si>
+    <t>30,05 +/-0,07</t>
+  </si>
+  <si>
+    <t>48,49 +/-0,29</t>
+  </si>
+  <si>
+    <t>1,11 +/-0,01</t>
+  </si>
+  <si>
+    <t>2,44 +/-0,01</t>
+  </si>
+  <si>
+    <t>0,44 +/-0,0</t>
+  </si>
+  <si>
+    <t>0,83 +/-0,0</t>
+  </si>
+  <si>
+    <t>0,21 +/-0,0</t>
+  </si>
+  <si>
+    <t>0,16 +/-0,0</t>
+  </si>
+  <si>
+    <t>0,17 +/-0,0</t>
+  </si>
+  <si>
+    <t>0,23 +/-0,0</t>
+  </si>
+  <si>
+    <t>0,33 +/-0,0</t>
   </si>
 </sst>
 </file>
@@ -2848,18 +2890,6 @@
     <xf numFmtId="0" fontId="18" fillId="9" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2876,6 +2906,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2920,13 +2956,10 @@
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2941,11 +2974,32 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="17" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2998,9 +3052,6 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -3010,23 +3061,14 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="27">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -3054,6 +3096,26 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3766,12 +3828,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4281BA12-2AB6-4402-9C8A-B97791AE3613}" name="Sheet1__6" displayName="Sheet1__6" ref="A1:G31" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:G31" xr:uid="{4281BA12-2AB6-4402-9C8A-B97791AE3613}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{1E410214-D17A-4C6A-936C-E9960C4A04F9}" uniqueName="1" name="features" queryTableFieldId="1" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{AD5A5509-557B-4D77-82E7-61F7BBAF1AC6}" uniqueName="2" name="lasso" queryTableFieldId="2" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{1E410214-D17A-4C6A-936C-E9960C4A04F9}" uniqueName="1" name="features" queryTableFieldId="1" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{AD5A5509-557B-4D77-82E7-61F7BBAF1AC6}" uniqueName="2" name="lasso" queryTableFieldId="2" dataDxfId="25"/>
     <tableColumn id="3" xr3:uid="{C3755214-5E9D-4104-9F76-4C89B243E0C8}" uniqueName="3" name="num1" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{92C60055-6DCA-4ABA-8C93-8215973B353E}" uniqueName="4" name="ridge" queryTableFieldId="4" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{92C60055-6DCA-4ABA-8C93-8215973B353E}" uniqueName="4" name="ridge" queryTableFieldId="4" dataDxfId="24"/>
     <tableColumn id="5" xr3:uid="{D2D8E92F-67FF-451F-AACB-1C8D333C779A}" uniqueName="5" name="num2" queryTableFieldId="5"/>
-    <tableColumn id="6" xr3:uid="{EEB25EE1-2CF1-4BBB-8571-07BC55213599}" uniqueName="6" name="method" queryTableFieldId="6" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{EEB25EE1-2CF1-4BBB-8571-07BC55213599}" uniqueName="6" name="method" queryTableFieldId="6" dataDxfId="23"/>
     <tableColumn id="7" xr3:uid="{C996D4D0-777E-4CF3-B876-32524B63EBB6}" uniqueName="7" name="selection" queryTableFieldId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3782,12 +3844,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AE5E4999-D2C9-4039-851C-A2E5A9935AFF}" name="Sheet1__4" displayName="Sheet1__4" ref="A1:G31" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:G31" xr:uid="{AE5E4999-D2C9-4039-851C-A2E5A9935AFF}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{F9CAD7A5-EAB8-4AD7-B34E-84CB404A5093}" uniqueName="1" name="features" queryTableFieldId="1" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{9B56B4D4-BBB1-42BD-A291-0BB3760A0CE6}" uniqueName="2" name="lasso" queryTableFieldId="2" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{F9CAD7A5-EAB8-4AD7-B34E-84CB404A5093}" uniqueName="1" name="features" queryTableFieldId="1" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{9B56B4D4-BBB1-42BD-A291-0BB3760A0CE6}" uniqueName="2" name="lasso" queryTableFieldId="2" dataDxfId="21"/>
     <tableColumn id="3" xr3:uid="{EF18F783-366A-49C7-A66C-6D2EC1E644DD}" uniqueName="3" name="num1" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{09BF3A29-5803-46E1-8176-ECC0FE5716B6}" uniqueName="4" name="ridge" queryTableFieldId="4" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{09BF3A29-5803-46E1-8176-ECC0FE5716B6}" uniqueName="4" name="ridge" queryTableFieldId="4" dataDxfId="20"/>
     <tableColumn id="5" xr3:uid="{5FCC126A-E409-438E-8825-B622EB0F070F}" uniqueName="5" name="num2" queryTableFieldId="5"/>
-    <tableColumn id="6" xr3:uid="{09F24BC2-F194-4B81-8251-0BB034BC8967}" uniqueName="6" name="method" queryTableFieldId="6" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{09F24BC2-F194-4B81-8251-0BB034BC8967}" uniqueName="6" name="method" queryTableFieldId="6" dataDxfId="19"/>
     <tableColumn id="7" xr3:uid="{F777D099-CBEE-4F28-AEEE-B2E16618203A}" uniqueName="7" name="selection" queryTableFieldId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3798,12 +3860,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{24C0E013-82E5-4CFE-B43C-766D23522FAF}" name="Sheet1__3" displayName="Sheet1__3" ref="A1:G124" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:G124" xr:uid="{24C0E013-82E5-4CFE-B43C-766D23522FAF}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{44A245CE-A0F5-4450-B017-A3A5E9E9CAE5}" uniqueName="1" name="features" queryTableFieldId="1" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{1527B258-DB70-4F36-8C5C-0D96BC6A24EF}" uniqueName="2" name="lasso" queryTableFieldId="2" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{44A245CE-A0F5-4450-B017-A3A5E9E9CAE5}" uniqueName="1" name="features" queryTableFieldId="1" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{1527B258-DB70-4F36-8C5C-0D96BC6A24EF}" uniqueName="2" name="lasso" queryTableFieldId="2" dataDxfId="17"/>
     <tableColumn id="3" xr3:uid="{E4C6FB47-E882-4FAD-B736-991DBF721E5D}" uniqueName="3" name="num1" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{CECBE909-A71D-4994-AE0D-08E6D081EE22}" uniqueName="4" name="ridge" queryTableFieldId="4" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{CECBE909-A71D-4994-AE0D-08E6D081EE22}" uniqueName="4" name="ridge" queryTableFieldId="4" dataDxfId="16"/>
     <tableColumn id="5" xr3:uid="{6D52BEBB-6286-422A-80B6-AA44B939067D}" uniqueName="5" name="num2" queryTableFieldId="5"/>
-    <tableColumn id="6" xr3:uid="{34473513-FA19-45A8-B748-F61E9D3A85F5}" uniqueName="6" name="method" queryTableFieldId="6" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{34473513-FA19-45A8-B748-F61E9D3A85F5}" uniqueName="6" name="method" queryTableFieldId="6" dataDxfId="15"/>
     <tableColumn id="7" xr3:uid="{735F41F4-717C-4910-98CC-AB94C917AE25}" uniqueName="7" name="selection" queryTableFieldId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3814,12 +3876,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C35BF9C7-9564-4DA5-9D57-3530814F9E46}" name="Sheet1__7" displayName="Sheet1__7" ref="A1:G124" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:G124" xr:uid="{C35BF9C7-9564-4DA5-9D57-3530814F9E46}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{F8C4ED62-AB84-4728-A317-69931DBFCEBA}" uniqueName="1" name="features" queryTableFieldId="1" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{A8AFAE2B-BE28-48A8-AFCA-2D6D5C89D1F6}" uniqueName="2" name="lasso" queryTableFieldId="2" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{F8C4ED62-AB84-4728-A317-69931DBFCEBA}" uniqueName="1" name="features" queryTableFieldId="1" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{A8AFAE2B-BE28-48A8-AFCA-2D6D5C89D1F6}" uniqueName="2" name="lasso" queryTableFieldId="2" dataDxfId="13"/>
     <tableColumn id="3" xr3:uid="{B4984FB6-96AF-41F6-922C-1069F40069DF}" uniqueName="3" name="num1" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{D58AE284-97A9-4BCE-B134-2ABB1C3912F5}" uniqueName="4" name="ridge" queryTableFieldId="4" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{D58AE284-97A9-4BCE-B134-2ABB1C3912F5}" uniqueName="4" name="ridge" queryTableFieldId="4" dataDxfId="12"/>
     <tableColumn id="5" xr3:uid="{E8EA3B7A-FE2B-4079-9059-C668D49AF0DE}" uniqueName="5" name="num2" queryTableFieldId="5"/>
-    <tableColumn id="6" xr3:uid="{5AAD9C3F-BC5C-47B1-A60C-C934118C5F4F}" uniqueName="6" name="method" queryTableFieldId="6" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{5AAD9C3F-BC5C-47B1-A60C-C934118C5F4F}" uniqueName="6" name="method" queryTableFieldId="6" dataDxfId="11"/>
     <tableColumn id="7" xr3:uid="{59E56AC7-2A4F-42C0-8271-2175D0266004}" uniqueName="7" name="selection" queryTableFieldId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4759,10 +4821,10 @@
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <conditionalFormatting sqref="C10:F39">
-    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="10" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="9" priority="2" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4803,181 +4865,181 @@
   <sheetData>
     <row r="1" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:22" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="95" t="s">
+      <c r="B2" s="91" t="s">
         <v>316</v>
       </c>
-      <c r="C2" s="96"/>
-      <c r="D2" s="101" t="s">
+      <c r="C2" s="92"/>
+      <c r="D2" s="99" t="s">
         <v>324</v>
       </c>
-      <c r="E2" s="102"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
-      <c r="J2" s="102"/>
-      <c r="K2" s="102"/>
-      <c r="L2" s="102"/>
-      <c r="M2" s="102"/>
-      <c r="N2" s="102"/>
-      <c r="O2" s="102"/>
-      <c r="P2" s="102"/>
-      <c r="Q2" s="103"/>
-      <c r="S2" s="113" t="s">
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="100"/>
+      <c r="M2" s="100"/>
+      <c r="N2" s="100"/>
+      <c r="O2" s="100"/>
+      <c r="P2" s="100"/>
+      <c r="Q2" s="101"/>
+      <c r="S2" s="111" t="s">
         <v>317</v>
       </c>
-      <c r="T2" s="114"/>
-      <c r="U2" s="114"/>
-      <c r="V2" s="114"/>
+      <c r="T2" s="112"/>
+      <c r="U2" s="112"/>
+      <c r="V2" s="112"/>
     </row>
     <row r="3" spans="2:22" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="97"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="104" t="s">
+      <c r="B3" s="93"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="102" t="s">
         <v>326</v>
       </c>
-      <c r="E3" s="105"/>
-      <c r="F3" s="105"/>
-      <c r="G3" s="105"/>
-      <c r="H3" s="105"/>
-      <c r="I3" s="105"/>
-      <c r="J3" s="105"/>
-      <c r="K3" s="105"/>
-      <c r="L3" s="105"/>
-      <c r="M3" s="105"/>
-      <c r="N3" s="105"/>
-      <c r="O3" s="105"/>
-      <c r="P3" s="105"/>
-      <c r="Q3" s="106"/>
+      <c r="E3" s="103"/>
+      <c r="F3" s="103"/>
+      <c r="G3" s="103"/>
+      <c r="H3" s="103"/>
+      <c r="I3" s="103"/>
+      <c r="J3" s="103"/>
+      <c r="K3" s="103"/>
+      <c r="L3" s="103"/>
+      <c r="M3" s="103"/>
+      <c r="N3" s="103"/>
+      <c r="O3" s="103"/>
+      <c r="P3" s="103"/>
+      <c r="Q3" s="104"/>
       <c r="S3" s="72">
         <v>0</v>
       </c>
-      <c r="T3" s="107" t="s">
+      <c r="T3" s="105" t="s">
         <v>318</v>
       </c>
-      <c r="U3" s="107"/>
-      <c r="V3" s="108"/>
+      <c r="U3" s="105"/>
+      <c r="V3" s="106"/>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.35">
       <c r="S4" s="73">
         <v>1</v>
       </c>
-      <c r="T4" s="109" t="s">
+      <c r="T4" s="107" t="s">
         <v>319</v>
       </c>
-      <c r="U4" s="109"/>
-      <c r="V4" s="110"/>
+      <c r="U4" s="107"/>
+      <c r="V4" s="108"/>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.35">
       <c r="S5" s="73">
         <v>2</v>
       </c>
-      <c r="T5" s="109" t="s">
+      <c r="T5" s="107" t="s">
         <v>320</v>
       </c>
-      <c r="U5" s="109"/>
-      <c r="V5" s="110"/>
+      <c r="U5" s="107"/>
+      <c r="V5" s="108"/>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.35">
       <c r="S6" s="74">
         <v>3</v>
       </c>
-      <c r="T6" s="111" t="s">
+      <c r="T6" s="109" t="s">
         <v>321</v>
       </c>
-      <c r="U6" s="111"/>
-      <c r="V6" s="112"/>
+      <c r="U6" s="109"/>
+      <c r="V6" s="110"/>
     </row>
     <row r="8" spans="2:22" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="91" t="s">
+      <c r="B8" s="113" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="91"/>
-      <c r="D8" s="91"/>
-      <c r="E8" s="91"/>
-      <c r="F8" s="91"/>
-      <c r="G8" s="91"/>
+      <c r="C8" s="113"/>
+      <c r="D8" s="113"/>
+      <c r="E8" s="113"/>
+      <c r="F8" s="113"/>
+      <c r="G8" s="113"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="99" t="s">
+      <c r="J8" s="95" t="s">
         <v>38</v>
       </c>
-      <c r="K8" s="99"/>
-      <c r="L8" s="99"/>
-      <c r="M8" s="99"/>
-      <c r="N8" s="99"/>
-      <c r="O8" s="99"/>
-      <c r="Q8" s="99" t="s">
+      <c r="K8" s="95"/>
+      <c r="L8" s="95"/>
+      <c r="M8" s="95"/>
+      <c r="N8" s="95"/>
+      <c r="O8" s="95"/>
+      <c r="Q8" s="95" t="s">
         <v>39</v>
       </c>
-      <c r="R8" s="99"/>
-      <c r="S8" s="99"/>
-      <c r="T8" s="99"/>
-      <c r="U8" s="99"/>
-      <c r="V8" s="99"/>
+      <c r="R8" s="95"/>
+      <c r="S8" s="95"/>
+      <c r="T8" s="95"/>
+      <c r="U8" s="95"/>
+      <c r="V8" s="95"/>
     </row>
     <row r="9" spans="2:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="92"/>
-      <c r="C9" s="92"/>
-      <c r="D9" s="92"/>
-      <c r="E9" s="92"/>
-      <c r="F9" s="92"/>
-      <c r="G9" s="92"/>
+      <c r="B9" s="114"/>
+      <c r="C9" s="114"/>
+      <c r="D9" s="114"/>
+      <c r="E9" s="114"/>
+      <c r="F9" s="114"/>
+      <c r="G9" s="114"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="100"/>
-      <c r="K9" s="100"/>
-      <c r="L9" s="100"/>
-      <c r="M9" s="100"/>
-      <c r="N9" s="100"/>
-      <c r="O9" s="100"/>
-      <c r="Q9" s="100"/>
-      <c r="R9" s="100"/>
-      <c r="S9" s="100"/>
-      <c r="T9" s="100"/>
-      <c r="U9" s="100"/>
-      <c r="V9" s="100"/>
+      <c r="J9" s="96"/>
+      <c r="K9" s="96"/>
+      <c r="L9" s="96"/>
+      <c r="M9" s="96"/>
+      <c r="N9" s="96"/>
+      <c r="O9" s="96"/>
+      <c r="Q9" s="96"/>
+      <c r="R9" s="96"/>
+      <c r="S9" s="96"/>
+      <c r="T9" s="96"/>
+      <c r="U9" s="96"/>
+      <c r="V9" s="96"/>
     </row>
     <row r="10" spans="2:22" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="93" t="s">
+      <c r="C10" s="97" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="94"/>
-      <c r="E10" s="93" t="s">
+      <c r="D10" s="98"/>
+      <c r="E10" s="97" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="94"/>
+      <c r="F10" s="98"/>
       <c r="G10" s="35" t="s">
         <v>42</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="K10" s="93" t="s">
+      <c r="K10" s="97" t="s">
         <v>40</v>
       </c>
-      <c r="L10" s="94"/>
-      <c r="M10" s="93" t="s">
+      <c r="L10" s="98"/>
+      <c r="M10" s="97" t="s">
         <v>41</v>
       </c>
-      <c r="N10" s="94"/>
+      <c r="N10" s="98"/>
       <c r="O10" s="3" t="s">
         <v>42</v>
       </c>
       <c r="Q10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="R10" s="93" t="s">
+      <c r="R10" s="97" t="s">
         <v>40</v>
       </c>
-      <c r="S10" s="94"/>
-      <c r="T10" s="93" t="s">
+      <c r="S10" s="98"/>
+      <c r="T10" s="97" t="s">
         <v>41</v>
       </c>
-      <c r="U10" s="94"/>
+      <c r="U10" s="98"/>
       <c r="V10" s="3" t="s">
         <v>42</v>
       </c>
@@ -6748,14 +6810,14 @@
       </c>
     </row>
     <row r="43" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B43" s="91" t="s">
+      <c r="B43" s="113" t="s">
         <v>76</v>
       </c>
-      <c r="C43" s="91"/>
-      <c r="D43" s="91"/>
-      <c r="E43" s="91"/>
-      <c r="F43" s="91"/>
-      <c r="G43" s="91"/>
+      <c r="C43" s="113"/>
+      <c r="D43" s="113"/>
+      <c r="E43" s="113"/>
+      <c r="F43" s="113"/>
+      <c r="G43" s="113"/>
       <c r="J43" t="s">
         <v>64</v>
       </c>
@@ -6794,12 +6856,12 @@
       </c>
     </row>
     <row r="44" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="92"/>
-      <c r="C44" s="92"/>
-      <c r="D44" s="92"/>
-      <c r="E44" s="92"/>
-      <c r="F44" s="92"/>
-      <c r="G44" s="92"/>
+      <c r="B44" s="114"/>
+      <c r="C44" s="114"/>
+      <c r="D44" s="114"/>
+      <c r="E44" s="114"/>
+      <c r="F44" s="114"/>
+      <c r="G44" s="114"/>
       <c r="J44" t="s">
         <v>18</v>
       </c>
@@ -6841,14 +6903,14 @@
       <c r="B45" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="93" t="s">
+      <c r="C45" s="97" t="s">
         <v>40</v>
       </c>
-      <c r="D45" s="94"/>
-      <c r="E45" s="93" t="s">
+      <c r="D45" s="98"/>
+      <c r="E45" s="97" t="s">
         <v>41</v>
       </c>
-      <c r="F45" s="94"/>
+      <c r="F45" s="98"/>
       <c r="G45" s="35" t="s">
         <v>42</v>
       </c>
@@ -10778,6 +10840,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B43:G44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="B8:G9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
     <mergeCell ref="B2:C3"/>
     <mergeCell ref="Q8:V9"/>
     <mergeCell ref="R10:S10"/>
@@ -10792,12 +10860,6 @@
     <mergeCell ref="T5:V5"/>
     <mergeCell ref="T6:V6"/>
     <mergeCell ref="S2:V2"/>
-    <mergeCell ref="B43:G44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="B8:G9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -16244,10 +16306,10 @@
   <sheetData>
     <row r="1" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:23" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="145" t="s">
+      <c r="B2" s="122" t="s">
         <v>313</v>
       </c>
-      <c r="C2" s="146"/>
+      <c r="C2" s="123"/>
       <c r="D2" s="87" t="s">
         <v>325</v>
       </c>
@@ -16258,8 +16320,8 @@
       <c r="I2" s="88"/>
     </row>
     <row r="3" spans="2:23" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="147"/>
-      <c r="C3" s="148"/>
+      <c r="B3" s="124"/>
+      <c r="C3" s="125"/>
       <c r="D3" s="89"/>
       <c r="E3" s="89"/>
       <c r="F3" s="89"/>
@@ -16268,62 +16330,62 @@
       <c r="I3" s="90"/>
     </row>
     <row r="5" spans="2:23" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="C5" s="116" t="s">
+      <c r="C5" s="126" t="s">
         <v>156</v>
       </c>
-      <c r="D5" s="116"/>
-      <c r="E5" s="116"/>
-      <c r="F5" s="116"/>
-      <c r="G5" s="116"/>
-      <c r="H5" s="116"/>
-      <c r="I5" s="116"/>
-      <c r="L5" s="116" t="s">
+      <c r="D5" s="126"/>
+      <c r="E5" s="126"/>
+      <c r="F5" s="126"/>
+      <c r="G5" s="126"/>
+      <c r="H5" s="126"/>
+      <c r="I5" s="126"/>
+      <c r="L5" s="126" t="s">
         <v>157</v>
       </c>
-      <c r="M5" s="116"/>
-      <c r="N5" s="116"/>
-      <c r="O5" s="116"/>
-      <c r="P5" s="116"/>
-      <c r="Q5" s="116"/>
-      <c r="R5" s="116"/>
-      <c r="S5" s="116"/>
-      <c r="T5" s="116"/>
-      <c r="U5" s="116"/>
-      <c r="V5" s="116"/>
-      <c r="W5" s="116"/>
+      <c r="M5" s="126"/>
+      <c r="N5" s="126"/>
+      <c r="O5" s="126"/>
+      <c r="P5" s="126"/>
+      <c r="Q5" s="126"/>
+      <c r="R5" s="126"/>
+      <c r="S5" s="126"/>
+      <c r="T5" s="126"/>
+      <c r="U5" s="126"/>
+      <c r="V5" s="126"/>
+      <c r="W5" s="126"/>
     </row>
     <row r="6" spans="2:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C6" s="117"/>
-      <c r="D6" s="117"/>
-      <c r="E6" s="117"/>
-      <c r="F6" s="117"/>
-      <c r="G6" s="117"/>
-      <c r="H6" s="117"/>
-      <c r="I6" s="117"/>
-      <c r="L6" s="121" t="s">
+      <c r="C6" s="127"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="127"/>
+      <c r="F6" s="127"/>
+      <c r="G6" s="127"/>
+      <c r="H6" s="127"/>
+      <c r="I6" s="127"/>
+      <c r="L6" s="118" t="s">
         <v>158</v>
       </c>
-      <c r="M6" s="115"/>
-      <c r="N6" s="115" t="s">
+      <c r="M6" s="119"/>
+      <c r="N6" s="119" t="s">
         <v>159</v>
       </c>
-      <c r="O6" s="115"/>
-      <c r="P6" s="115" t="s">
+      <c r="O6" s="119"/>
+      <c r="P6" s="119" t="s">
         <v>160</v>
       </c>
-      <c r="Q6" s="115"/>
-      <c r="R6" s="115" t="s">
+      <c r="Q6" s="119"/>
+      <c r="R6" s="119" t="s">
         <v>161</v>
       </c>
-      <c r="S6" s="115"/>
-      <c r="T6" s="115" t="s">
+      <c r="S6" s="119"/>
+      <c r="T6" s="119" t="s">
         <v>162</v>
       </c>
-      <c r="U6" s="115"/>
-      <c r="V6" s="115" t="s">
+      <c r="U6" s="119"/>
+      <c r="V6" s="119" t="s">
         <v>163</v>
       </c>
-      <c r="W6" s="115"/>
+      <c r="W6" s="119"/>
     </row>
     <row r="7" spans="2:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="13"/>
@@ -16346,7 +16408,7 @@
         <v>163</v>
       </c>
       <c r="I7" s="50" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="L7" s="69" t="s">
         <v>164</v>
@@ -16411,35 +16473,35 @@
       <c r="L8" s="10">
         <v>1</v>
       </c>
-      <c r="M8" s="122" t="s">
+      <c r="M8" s="120" t="s">
         <v>296</v>
       </c>
       <c r="N8" s="10">
         <v>0</v>
       </c>
-      <c r="O8" s="118" t="s">
+      <c r="O8" s="115" t="s">
         <v>315</v>
       </c>
       <c r="P8" s="10">
         <v>0</v>
       </c>
-      <c r="Q8" s="118" t="s">
+      <c r="Q8" s="115" t="s">
         <v>315</v>
       </c>
       <c r="R8" s="10">
         <v>0</v>
       </c>
-      <c r="S8" s="118" t="s">
+      <c r="S8" s="115" t="s">
         <v>315</v>
       </c>
       <c r="T8" s="45"/>
-      <c r="U8" s="118" t="s">
+      <c r="U8" s="115" t="s">
         <v>315</v>
       </c>
       <c r="V8" s="47">
         <v>0</v>
       </c>
-      <c r="W8" s="118" t="s">
+      <c r="W8" s="115" t="s">
         <v>315</v>
       </c>
     </row>
@@ -16469,25 +16531,25 @@
       <c r="L9" s="10">
         <v>1</v>
       </c>
-      <c r="M9" s="122"/>
+      <c r="M9" s="120"/>
       <c r="N9" s="10">
         <v>0</v>
       </c>
-      <c r="O9" s="118"/>
+      <c r="O9" s="115"/>
       <c r="P9" s="10">
         <v>0</v>
       </c>
-      <c r="Q9" s="118"/>
+      <c r="Q9" s="115"/>
       <c r="R9" s="10">
         <v>0</v>
       </c>
-      <c r="S9" s="118"/>
+      <c r="S9" s="115"/>
       <c r="T9" s="46"/>
-      <c r="U9" s="118"/>
+      <c r="U9" s="115"/>
       <c r="V9" s="48">
         <v>0</v>
       </c>
-      <c r="W9" s="118"/>
+      <c r="W9" s="115"/>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B10" s="14" t="s">
@@ -16515,25 +16577,25 @@
       <c r="L10" s="10">
         <v>1</v>
       </c>
-      <c r="M10" s="122"/>
+      <c r="M10" s="120"/>
       <c r="N10" s="10">
         <v>0</v>
       </c>
-      <c r="O10" s="118"/>
+      <c r="O10" s="115"/>
       <c r="P10" s="10">
         <v>0</v>
       </c>
-      <c r="Q10" s="118"/>
+      <c r="Q10" s="115"/>
       <c r="R10" s="10">
         <v>0</v>
       </c>
-      <c r="S10" s="118"/>
+      <c r="S10" s="115"/>
       <c r="T10" s="46"/>
-      <c r="U10" s="118"/>
+      <c r="U10" s="115"/>
       <c r="V10" s="48">
         <v>0</v>
       </c>
-      <c r="W10" s="118"/>
+      <c r="W10" s="115"/>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B11" s="14" t="s">
@@ -16561,25 +16623,25 @@
       <c r="L11" s="10">
         <v>1</v>
       </c>
-      <c r="M11" s="122"/>
+      <c r="M11" s="120"/>
       <c r="N11" s="10">
         <v>1</v>
       </c>
-      <c r="O11" s="118"/>
+      <c r="O11" s="115"/>
       <c r="P11" s="10">
         <v>0</v>
       </c>
-      <c r="Q11" s="118"/>
+      <c r="Q11" s="115"/>
       <c r="R11" s="10">
         <v>1</v>
       </c>
-      <c r="S11" s="118"/>
+      <c r="S11" s="115"/>
       <c r="T11" s="46"/>
-      <c r="U11" s="118"/>
+      <c r="U11" s="115"/>
       <c r="V11" s="48">
         <v>0</v>
       </c>
-      <c r="W11" s="118"/>
+      <c r="W11" s="115"/>
     </row>
     <row r="12" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B12" s="14" t="s">
@@ -16607,25 +16669,25 @@
       <c r="L12" s="10">
         <v>1</v>
       </c>
-      <c r="M12" s="122"/>
+      <c r="M12" s="120"/>
       <c r="N12" s="10">
         <v>0</v>
       </c>
-      <c r="O12" s="118"/>
+      <c r="O12" s="115"/>
       <c r="P12" s="10">
         <v>0</v>
       </c>
-      <c r="Q12" s="118"/>
+      <c r="Q12" s="115"/>
       <c r="R12" s="10">
         <v>0</v>
       </c>
-      <c r="S12" s="118"/>
+      <c r="S12" s="115"/>
       <c r="T12" s="46"/>
-      <c r="U12" s="118"/>
+      <c r="U12" s="115"/>
       <c r="V12" s="48">
         <v>1</v>
       </c>
-      <c r="W12" s="118"/>
+      <c r="W12" s="115"/>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B13" s="14" t="s">
@@ -16653,25 +16715,25 @@
       <c r="L13" s="10">
         <v>1</v>
       </c>
-      <c r="M13" s="122"/>
+      <c r="M13" s="120"/>
       <c r="N13" s="10">
         <v>1</v>
       </c>
-      <c r="O13" s="118"/>
+      <c r="O13" s="115"/>
       <c r="P13" s="10">
         <v>0</v>
       </c>
-      <c r="Q13" s="118"/>
+      <c r="Q13" s="115"/>
       <c r="R13" s="10">
         <v>1</v>
       </c>
-      <c r="S13" s="118"/>
+      <c r="S13" s="115"/>
       <c r="T13" s="46"/>
-      <c r="U13" s="118"/>
+      <c r="U13" s="115"/>
       <c r="V13" s="48">
         <v>0</v>
       </c>
-      <c r="W13" s="118"/>
+      <c r="W13" s="115"/>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B14" s="14" t="s">
@@ -16699,25 +16761,25 @@
       <c r="L14" s="10">
         <v>1</v>
       </c>
-      <c r="M14" s="122"/>
+      <c r="M14" s="120"/>
       <c r="N14" s="10">
         <v>0</v>
       </c>
-      <c r="O14" s="118"/>
+      <c r="O14" s="115"/>
       <c r="P14" s="10">
         <v>0</v>
       </c>
-      <c r="Q14" s="118"/>
+      <c r="Q14" s="115"/>
       <c r="R14" s="10">
         <v>0</v>
       </c>
-      <c r="S14" s="118"/>
+      <c r="S14" s="115"/>
       <c r="T14" s="46"/>
-      <c r="U14" s="118"/>
+      <c r="U14" s="115"/>
       <c r="V14" s="48">
         <v>0</v>
       </c>
-      <c r="W14" s="118"/>
+      <c r="W14" s="115"/>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B15" s="14" t="s">
@@ -16745,25 +16807,25 @@
       <c r="L15" s="10">
         <v>1</v>
       </c>
-      <c r="M15" s="122"/>
+      <c r="M15" s="120"/>
       <c r="N15" s="10">
         <v>0</v>
       </c>
-      <c r="O15" s="118"/>
+      <c r="O15" s="115"/>
       <c r="P15" s="10">
         <v>0</v>
       </c>
-      <c r="Q15" s="118"/>
+      <c r="Q15" s="115"/>
       <c r="R15" s="10">
         <v>0</v>
       </c>
-      <c r="S15" s="118"/>
+      <c r="S15" s="115"/>
       <c r="T15" s="46"/>
-      <c r="U15" s="118"/>
+      <c r="U15" s="115"/>
       <c r="V15" s="48">
         <v>0</v>
       </c>
-      <c r="W15" s="118"/>
+      <c r="W15" s="115"/>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B16" s="14" t="s">
@@ -16791,25 +16853,25 @@
       <c r="L16" s="10">
         <v>1</v>
       </c>
-      <c r="M16" s="122"/>
+      <c r="M16" s="120"/>
       <c r="N16" s="10">
         <v>0</v>
       </c>
-      <c r="O16" s="118"/>
+      <c r="O16" s="115"/>
       <c r="P16" s="10">
         <v>0</v>
       </c>
-      <c r="Q16" s="118"/>
+      <c r="Q16" s="115"/>
       <c r="R16" s="10">
         <v>0</v>
       </c>
-      <c r="S16" s="118"/>
+      <c r="S16" s="115"/>
       <c r="T16" s="46"/>
-      <c r="U16" s="118"/>
+      <c r="U16" s="115"/>
       <c r="V16" s="48">
         <v>0</v>
       </c>
-      <c r="W16" s="118"/>
+      <c r="W16" s="115"/>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B17" s="14" t="s">
@@ -16837,25 +16899,25 @@
       <c r="L17" s="10">
         <v>1</v>
       </c>
-      <c r="M17" s="122"/>
+      <c r="M17" s="120"/>
       <c r="N17" s="10">
         <v>0</v>
       </c>
-      <c r="O17" s="118"/>
+      <c r="O17" s="115"/>
       <c r="P17" s="10">
         <v>0</v>
       </c>
-      <c r="Q17" s="118"/>
+      <c r="Q17" s="115"/>
       <c r="R17" s="10">
         <v>0</v>
       </c>
-      <c r="S17" s="118"/>
+      <c r="S17" s="115"/>
       <c r="T17" s="46"/>
-      <c r="U17" s="118"/>
+      <c r="U17" s="115"/>
       <c r="V17" s="48">
         <v>0</v>
       </c>
-      <c r="W17" s="118"/>
+      <c r="W17" s="115"/>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B18" s="14" t="s">
@@ -16883,25 +16945,25 @@
       <c r="L18" s="10">
         <v>1</v>
       </c>
-      <c r="M18" s="122"/>
+      <c r="M18" s="120"/>
       <c r="N18" s="10">
         <v>0</v>
       </c>
-      <c r="O18" s="118"/>
+      <c r="O18" s="115"/>
       <c r="P18" s="10">
         <v>1</v>
       </c>
-      <c r="Q18" s="118"/>
+      <c r="Q18" s="115"/>
       <c r="R18" s="10">
         <v>1</v>
       </c>
-      <c r="S18" s="118"/>
+      <c r="S18" s="115"/>
       <c r="T18" s="46"/>
-      <c r="U18" s="118"/>
+      <c r="U18" s="115"/>
       <c r="V18" s="48">
         <v>1</v>
       </c>
-      <c r="W18" s="118"/>
+      <c r="W18" s="115"/>
     </row>
     <row r="19" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B19" s="14" t="s">
@@ -16929,25 +16991,25 @@
       <c r="L19" s="10">
         <v>1</v>
       </c>
-      <c r="M19" s="122"/>
+      <c r="M19" s="120"/>
       <c r="N19" s="10">
         <v>0</v>
       </c>
-      <c r="O19" s="118"/>
+      <c r="O19" s="115"/>
       <c r="P19" s="10">
         <v>0</v>
       </c>
-      <c r="Q19" s="118"/>
+      <c r="Q19" s="115"/>
       <c r="R19" s="10">
         <v>0</v>
       </c>
-      <c r="S19" s="118"/>
+      <c r="S19" s="115"/>
       <c r="T19" s="46"/>
-      <c r="U19" s="118"/>
+      <c r="U19" s="115"/>
       <c r="V19" s="48">
         <v>0</v>
       </c>
-      <c r="W19" s="118"/>
+      <c r="W19" s="115"/>
     </row>
     <row r="20" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B20" s="14" t="s">
@@ -16975,25 +17037,25 @@
       <c r="L20" s="10">
         <v>1</v>
       </c>
-      <c r="M20" s="122"/>
+      <c r="M20" s="120"/>
       <c r="N20" s="10">
         <v>0</v>
       </c>
-      <c r="O20" s="118"/>
+      <c r="O20" s="115"/>
       <c r="P20" s="10">
         <v>0</v>
       </c>
-      <c r="Q20" s="118"/>
+      <c r="Q20" s="115"/>
       <c r="R20" s="10">
         <v>0</v>
       </c>
-      <c r="S20" s="118"/>
+      <c r="S20" s="115"/>
       <c r="T20" s="46"/>
-      <c r="U20" s="118"/>
+      <c r="U20" s="115"/>
       <c r="V20" s="48">
         <v>0</v>
       </c>
-      <c r="W20" s="118"/>
+      <c r="W20" s="115"/>
     </row>
     <row r="21" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B21" s="14" t="s">
@@ -17021,25 +17083,25 @@
       <c r="L21" s="10">
         <v>1</v>
       </c>
-      <c r="M21" s="122"/>
+      <c r="M21" s="120"/>
       <c r="N21" s="10">
         <v>0</v>
       </c>
-      <c r="O21" s="118"/>
+      <c r="O21" s="115"/>
       <c r="P21" s="10">
         <v>0</v>
       </c>
-      <c r="Q21" s="118"/>
+      <c r="Q21" s="115"/>
       <c r="R21" s="10">
         <v>0</v>
       </c>
-      <c r="S21" s="118"/>
+      <c r="S21" s="115"/>
       <c r="T21" s="46"/>
-      <c r="U21" s="118"/>
+      <c r="U21" s="115"/>
       <c r="V21" s="48">
         <v>0</v>
       </c>
-      <c r="W21" s="118"/>
+      <c r="W21" s="115"/>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B22" s="14" t="s">
@@ -17067,25 +17129,25 @@
       <c r="L22" s="10">
         <v>1</v>
       </c>
-      <c r="M22" s="122"/>
+      <c r="M22" s="120"/>
       <c r="N22" s="10">
         <v>0</v>
       </c>
-      <c r="O22" s="118"/>
+      <c r="O22" s="115"/>
       <c r="P22" s="10">
         <v>0</v>
       </c>
-      <c r="Q22" s="118"/>
+      <c r="Q22" s="115"/>
       <c r="R22" s="10">
         <v>1</v>
       </c>
-      <c r="S22" s="118"/>
+      <c r="S22" s="115"/>
       <c r="T22" s="46"/>
-      <c r="U22" s="118"/>
+      <c r="U22" s="115"/>
       <c r="V22" s="48">
         <v>0</v>
       </c>
-      <c r="W22" s="118"/>
+      <c r="W22" s="115"/>
     </row>
     <row r="23" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B23" s="14" t="s">
@@ -17113,25 +17175,25 @@
       <c r="L23" s="10">
         <v>1</v>
       </c>
-      <c r="M23" s="122"/>
+      <c r="M23" s="120"/>
       <c r="N23" s="10">
         <v>0</v>
       </c>
-      <c r="O23" s="118"/>
+      <c r="O23" s="115"/>
       <c r="P23" s="10">
         <v>1</v>
       </c>
-      <c r="Q23" s="118"/>
+      <c r="Q23" s="115"/>
       <c r="R23" s="10">
         <v>0</v>
       </c>
-      <c r="S23" s="118"/>
+      <c r="S23" s="115"/>
       <c r="T23" s="46"/>
-      <c r="U23" s="118"/>
+      <c r="U23" s="115"/>
       <c r="V23" s="48">
         <v>1</v>
       </c>
-      <c r="W23" s="118"/>
+      <c r="W23" s="115"/>
     </row>
     <row r="24" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B24" s="14" t="s">
@@ -17159,25 +17221,25 @@
       <c r="L24" s="10">
         <v>1</v>
       </c>
-      <c r="M24" s="122"/>
+      <c r="M24" s="120"/>
       <c r="N24" s="10">
         <v>0</v>
       </c>
-      <c r="O24" s="118"/>
+      <c r="O24" s="115"/>
       <c r="P24" s="10">
         <v>0</v>
       </c>
-      <c r="Q24" s="118"/>
+      <c r="Q24" s="115"/>
       <c r="R24" s="10">
         <v>1</v>
       </c>
-      <c r="S24" s="118"/>
+      <c r="S24" s="115"/>
       <c r="T24" s="46"/>
-      <c r="U24" s="118"/>
+      <c r="U24" s="115"/>
       <c r="V24" s="48">
         <v>0</v>
       </c>
-      <c r="W24" s="118"/>
+      <c r="W24" s="115"/>
     </row>
     <row r="25" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B25" s="14" t="s">
@@ -17205,25 +17267,25 @@
       <c r="L25" s="10">
         <v>1</v>
       </c>
-      <c r="M25" s="122"/>
+      <c r="M25" s="120"/>
       <c r="N25" s="10">
         <v>0</v>
       </c>
-      <c r="O25" s="118"/>
+      <c r="O25" s="115"/>
       <c r="P25" s="10">
         <v>0</v>
       </c>
-      <c r="Q25" s="118"/>
+      <c r="Q25" s="115"/>
       <c r="R25" s="10">
         <v>1</v>
       </c>
-      <c r="S25" s="118"/>
+      <c r="S25" s="115"/>
       <c r="T25" s="46"/>
-      <c r="U25" s="118"/>
+      <c r="U25" s="115"/>
       <c r="V25" s="48">
         <v>0</v>
       </c>
-      <c r="W25" s="118"/>
+      <c r="W25" s="115"/>
     </row>
     <row r="26" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B26" s="14" t="s">
@@ -17251,25 +17313,25 @@
       <c r="L26" s="10">
         <v>1</v>
       </c>
-      <c r="M26" s="122"/>
+      <c r="M26" s="120"/>
       <c r="N26" s="10">
         <v>1</v>
       </c>
-      <c r="O26" s="118"/>
+      <c r="O26" s="115"/>
       <c r="P26" s="10">
         <v>0</v>
       </c>
-      <c r="Q26" s="118"/>
+      <c r="Q26" s="115"/>
       <c r="R26" s="10">
         <v>1</v>
       </c>
-      <c r="S26" s="118"/>
+      <c r="S26" s="115"/>
       <c r="T26" s="46"/>
-      <c r="U26" s="118"/>
+      <c r="U26" s="115"/>
       <c r="V26" s="48">
         <v>0</v>
       </c>
-      <c r="W26" s="118"/>
+      <c r="W26" s="115"/>
     </row>
     <row r="27" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B27" s="14" t="s">
@@ -17297,25 +17359,25 @@
       <c r="L27" s="10">
         <v>1</v>
       </c>
-      <c r="M27" s="122"/>
+      <c r="M27" s="120"/>
       <c r="N27" s="10">
         <v>0</v>
       </c>
-      <c r="O27" s="118"/>
+      <c r="O27" s="115"/>
       <c r="P27" s="10">
         <v>0</v>
       </c>
-      <c r="Q27" s="118"/>
+      <c r="Q27" s="115"/>
       <c r="R27" s="10">
         <v>1</v>
       </c>
-      <c r="S27" s="118"/>
+      <c r="S27" s="115"/>
       <c r="T27" s="46"/>
-      <c r="U27" s="118"/>
+      <c r="U27" s="115"/>
       <c r="V27" s="48">
         <v>0</v>
       </c>
-      <c r="W27" s="118"/>
+      <c r="W27" s="115"/>
     </row>
     <row r="28" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B28" s="14" t="s">
@@ -17343,25 +17405,25 @@
       <c r="L28" s="10">
         <v>1</v>
       </c>
-      <c r="M28" s="122"/>
+      <c r="M28" s="120"/>
       <c r="N28" s="10">
         <v>1</v>
       </c>
-      <c r="O28" s="118"/>
+      <c r="O28" s="115"/>
       <c r="P28" s="10">
         <v>1</v>
       </c>
-      <c r="Q28" s="118"/>
+      <c r="Q28" s="115"/>
       <c r="R28" s="10">
         <v>1</v>
       </c>
-      <c r="S28" s="118"/>
+      <c r="S28" s="115"/>
       <c r="T28" s="46"/>
-      <c r="U28" s="118"/>
+      <c r="U28" s="115"/>
       <c r="V28" s="48">
         <v>1</v>
       </c>
-      <c r="W28" s="118"/>
+      <c r="W28" s="115"/>
     </row>
     <row r="29" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B29" s="14" t="s">
@@ -17389,25 +17451,25 @@
       <c r="L29" s="10">
         <v>1</v>
       </c>
-      <c r="M29" s="122"/>
+      <c r="M29" s="120"/>
       <c r="N29" s="10">
         <v>0</v>
       </c>
-      <c r="O29" s="118"/>
+      <c r="O29" s="115"/>
       <c r="P29" s="10">
         <v>0</v>
       </c>
-      <c r="Q29" s="118"/>
+      <c r="Q29" s="115"/>
       <c r="R29" s="10">
         <v>1</v>
       </c>
-      <c r="S29" s="118"/>
+      <c r="S29" s="115"/>
       <c r="T29" s="46"/>
-      <c r="U29" s="118"/>
+      <c r="U29" s="115"/>
       <c r="V29" s="48">
         <v>0</v>
       </c>
-      <c r="W29" s="118"/>
+      <c r="W29" s="115"/>
     </row>
     <row r="30" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B30" s="14" t="s">
@@ -17435,25 +17497,25 @@
       <c r="L30" s="10">
         <v>1</v>
       </c>
-      <c r="M30" s="122"/>
+      <c r="M30" s="120"/>
       <c r="N30" s="10">
         <v>1</v>
       </c>
-      <c r="O30" s="118"/>
+      <c r="O30" s="115"/>
       <c r="P30" s="10">
         <v>1</v>
       </c>
-      <c r="Q30" s="118"/>
+      <c r="Q30" s="115"/>
       <c r="R30" s="10">
         <v>1</v>
       </c>
-      <c r="S30" s="118"/>
+      <c r="S30" s="115"/>
       <c r="T30" s="46"/>
-      <c r="U30" s="118"/>
+      <c r="U30" s="115"/>
       <c r="V30" s="48">
         <v>1</v>
       </c>
-      <c r="W30" s="118"/>
+      <c r="W30" s="115"/>
     </row>
     <row r="31" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B31" s="14" t="s">
@@ -17481,25 +17543,25 @@
       <c r="L31" s="10">
         <v>1</v>
       </c>
-      <c r="M31" s="122"/>
+      <c r="M31" s="120"/>
       <c r="N31" s="10">
         <v>0</v>
       </c>
-      <c r="O31" s="118"/>
+      <c r="O31" s="115"/>
       <c r="P31" s="10">
         <v>0</v>
       </c>
-      <c r="Q31" s="118"/>
+      <c r="Q31" s="115"/>
       <c r="R31" s="10">
         <v>1</v>
       </c>
-      <c r="S31" s="118"/>
+      <c r="S31" s="115"/>
       <c r="T31" s="46"/>
-      <c r="U31" s="118"/>
+      <c r="U31" s="115"/>
       <c r="V31" s="48">
         <v>0</v>
       </c>
-      <c r="W31" s="118"/>
+      <c r="W31" s="115"/>
     </row>
     <row r="32" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B32" s="14" t="s">
@@ -17527,25 +17589,25 @@
       <c r="L32" s="10">
         <v>1</v>
       </c>
-      <c r="M32" s="122"/>
+      <c r="M32" s="120"/>
       <c r="N32" s="10">
         <v>1</v>
       </c>
-      <c r="O32" s="118"/>
+      <c r="O32" s="115"/>
       <c r="P32" s="10">
         <v>0</v>
       </c>
-      <c r="Q32" s="118"/>
+      <c r="Q32" s="115"/>
       <c r="R32" s="10">
         <v>1</v>
       </c>
-      <c r="S32" s="118"/>
+      <c r="S32" s="115"/>
       <c r="T32" s="46"/>
-      <c r="U32" s="118"/>
+      <c r="U32" s="115"/>
       <c r="V32" s="48">
         <v>0</v>
       </c>
-      <c r="W32" s="118"/>
+      <c r="W32" s="115"/>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B33" s="14" t="s">
@@ -17573,25 +17635,25 @@
       <c r="L33" s="10">
         <v>1</v>
       </c>
-      <c r="M33" s="122"/>
+      <c r="M33" s="120"/>
       <c r="N33" s="10">
         <v>0</v>
       </c>
-      <c r="O33" s="118"/>
+      <c r="O33" s="115"/>
       <c r="P33" s="10">
         <v>0</v>
       </c>
-      <c r="Q33" s="118"/>
+      <c r="Q33" s="115"/>
       <c r="R33" s="10">
         <v>0</v>
       </c>
-      <c r="S33" s="118"/>
+      <c r="S33" s="115"/>
       <c r="T33" s="46"/>
-      <c r="U33" s="118"/>
+      <c r="U33" s="115"/>
       <c r="V33" s="48">
         <v>0</v>
       </c>
-      <c r="W33" s="118"/>
+      <c r="W33" s="115"/>
     </row>
     <row r="34" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B34" s="14" t="s">
@@ -17619,25 +17681,25 @@
       <c r="L34" s="10">
         <v>1</v>
       </c>
-      <c r="M34" s="122"/>
+      <c r="M34" s="120"/>
       <c r="N34" s="10">
         <v>1</v>
       </c>
-      <c r="O34" s="118"/>
+      <c r="O34" s="115"/>
       <c r="P34" s="10">
         <v>0</v>
       </c>
-      <c r="Q34" s="118"/>
+      <c r="Q34" s="115"/>
       <c r="R34" s="10">
         <v>1</v>
       </c>
-      <c r="S34" s="118"/>
+      <c r="S34" s="115"/>
       <c r="T34" s="46"/>
-      <c r="U34" s="118"/>
+      <c r="U34" s="115"/>
       <c r="V34" s="48">
         <v>1</v>
       </c>
-      <c r="W34" s="118"/>
+      <c r="W34" s="115"/>
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B35" s="14" t="s">
@@ -17665,25 +17727,25 @@
       <c r="L35" s="10">
         <v>1</v>
       </c>
-      <c r="M35" s="122"/>
+      <c r="M35" s="120"/>
       <c r="N35" s="10">
         <v>0</v>
       </c>
-      <c r="O35" s="118"/>
+      <c r="O35" s="115"/>
       <c r="P35" s="10">
         <v>0</v>
       </c>
-      <c r="Q35" s="118"/>
+      <c r="Q35" s="115"/>
       <c r="R35" s="10">
         <v>1</v>
       </c>
-      <c r="S35" s="118"/>
+      <c r="S35" s="115"/>
       <c r="T35" s="46"/>
-      <c r="U35" s="118"/>
+      <c r="U35" s="115"/>
       <c r="V35" s="48">
         <v>0</v>
       </c>
-      <c r="W35" s="118"/>
+      <c r="W35" s="115"/>
     </row>
     <row r="36" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B36" s="14" t="s">
@@ -17711,25 +17773,25 @@
       <c r="L36" s="10">
         <v>1</v>
       </c>
-      <c r="M36" s="122"/>
+      <c r="M36" s="120"/>
       <c r="N36" s="10">
         <v>1</v>
       </c>
-      <c r="O36" s="118"/>
+      <c r="O36" s="115"/>
       <c r="P36" s="10">
         <v>0</v>
       </c>
-      <c r="Q36" s="118"/>
+      <c r="Q36" s="115"/>
       <c r="R36" s="10">
         <v>1</v>
       </c>
-      <c r="S36" s="118"/>
+      <c r="S36" s="115"/>
       <c r="T36" s="46"/>
-      <c r="U36" s="118"/>
+      <c r="U36" s="115"/>
       <c r="V36" s="48">
         <v>1</v>
       </c>
-      <c r="W36" s="118"/>
+      <c r="W36" s="115"/>
     </row>
     <row r="37" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B37" s="14" t="s">
@@ -17757,39 +17819,39 @@
       <c r="L37" s="11">
         <v>1</v>
       </c>
-      <c r="M37" s="123"/>
+      <c r="M37" s="121"/>
       <c r="N37" s="11">
         <v>1</v>
       </c>
-      <c r="O37" s="119"/>
+      <c r="O37" s="116"/>
       <c r="P37" s="11">
         <v>1</v>
       </c>
-      <c r="Q37" s="119"/>
+      <c r="Q37" s="116"/>
       <c r="R37" s="11">
         <v>1</v>
       </c>
-      <c r="S37" s="119"/>
+      <c r="S37" s="116"/>
       <c r="T37" s="12"/>
-      <c r="U37" s="119"/>
+      <c r="U37" s="116"/>
       <c r="V37" s="49">
         <v>1</v>
       </c>
-      <c r="W37" s="119"/>
+      <c r="W37" s="116"/>
     </row>
     <row r="38" spans="2:23" x14ac:dyDescent="0.35">
-      <c r="C38" s="120" t="s">
+      <c r="C38" s="117" t="s">
         <v>166</v>
       </c>
-      <c r="D38" s="120"/>
-      <c r="E38" s="120"/>
-      <c r="F38" s="120"/>
-      <c r="G38" s="120"/>
-      <c r="H38" s="120"/>
+      <c r="D38" s="117"/>
+      <c r="E38" s="117"/>
+      <c r="F38" s="117"/>
+      <c r="G38" s="117"/>
+      <c r="H38" s="117"/>
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.35">
       <c r="I39" s="40" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="40" spans="2:23" x14ac:dyDescent="0.35">
@@ -17812,6 +17874,12 @@
     <sortCondition ref="B8:B37"/>
   </sortState>
   <mergeCells count="17">
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="D2:I3"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="L5:W5"/>
+    <mergeCell ref="C5:I6"/>
+    <mergeCell ref="T6:U6"/>
     <mergeCell ref="U8:U37"/>
     <mergeCell ref="W8:W37"/>
     <mergeCell ref="C38:H38"/>
@@ -17823,12 +17891,6 @@
     <mergeCell ref="O8:O37"/>
     <mergeCell ref="S8:S37"/>
     <mergeCell ref="Q8:Q37"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="D2:I3"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="L5:W5"/>
-    <mergeCell ref="C5:I6"/>
-    <mergeCell ref="T6:U6"/>
   </mergeCells>
   <conditionalFormatting sqref="C8:C37 F8:G37">
     <cfRule type="iconSet" priority="18">
@@ -17929,8 +17991,19 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V8:V37">
-    <cfRule type="iconSet" priority="9">
+  <conditionalFormatting sqref="P8:P36">
+    <cfRule type="iconSet" priority="1">
+      <iconSet iconSet="5Quarters">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="20"/>
+        <cfvo type="percent" val="40"/>
+        <cfvo type="percent" val="60"/>
+        <cfvo type="percent" val="80"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P37">
+    <cfRule type="iconSet" priority="2">
       <iconSet iconSet="5Quarters">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="20"/>
@@ -17951,19 +18024,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P37">
-    <cfRule type="iconSet" priority="2">
-      <iconSet iconSet="5Quarters">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="20"/>
-        <cfvo type="percent" val="40"/>
-        <cfvo type="percent" val="60"/>
-        <cfvo type="percent" val="80"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P8:P36">
-    <cfRule type="iconSet" priority="1">
+  <conditionalFormatting sqref="V8:V37">
+    <cfRule type="iconSet" priority="9">
       <iconSet iconSet="5Quarters">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="20"/>
@@ -17984,8 +18046,8 @@
   </sheetPr>
   <dimension ref="B1:O225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17997,12 +18059,12 @@
   <sheetData>
     <row r="1" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="124" t="s">
+      <c r="B2" s="128" t="s">
         <v>167</v>
       </c>
-      <c r="C2" s="125"/>
+      <c r="C2" s="129"/>
       <c r="D2" s="87" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="E2" s="87"/>
       <c r="F2" s="87"/>
@@ -18016,8 +18078,8 @@
       <c r="N2" s="88"/>
     </row>
     <row r="3" spans="2:14" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="126"/>
-      <c r="C3" s="127"/>
+      <c r="B3" s="130"/>
+      <c r="C3" s="131"/>
       <c r="D3" s="89"/>
       <c r="E3" s="89"/>
       <c r="F3" s="89"/>
@@ -18031,53 +18093,53 @@
       <c r="N3" s="90"/>
     </row>
     <row r="6" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="134" t="s">
+      <c r="B6" s="138" t="s">
         <v>167</v>
       </c>
-      <c r="C6" s="134"/>
-      <c r="D6" s="134"/>
-      <c r="E6" s="134"/>
-      <c r="F6" s="134"/>
-      <c r="G6" s="134"/>
-      <c r="H6" s="134"/>
-      <c r="I6" s="134"/>
-      <c r="J6" s="134"/>
-      <c r="K6" s="134"/>
-      <c r="L6" s="134"/>
-      <c r="M6" s="134"/>
-      <c r="N6" s="134"/>
+      <c r="C6" s="138"/>
+      <c r="D6" s="138"/>
+      <c r="E6" s="138"/>
+      <c r="F6" s="138"/>
+      <c r="G6" s="138"/>
+      <c r="H6" s="138"/>
+      <c r="I6" s="138"/>
+      <c r="J6" s="138"/>
+      <c r="K6" s="138"/>
+      <c r="L6" s="138"/>
+      <c r="M6" s="138"/>
+      <c r="N6" s="138"/>
     </row>
     <row r="7" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="135"/>
-      <c r="C7" s="135"/>
-      <c r="D7" s="135"/>
-      <c r="E7" s="135"/>
-      <c r="F7" s="135"/>
-      <c r="G7" s="135"/>
-      <c r="H7" s="135"/>
-      <c r="I7" s="135"/>
-      <c r="J7" s="135"/>
-      <c r="K7" s="135"/>
-      <c r="L7" s="135"/>
-      <c r="M7" s="135"/>
-      <c r="N7" s="135"/>
+      <c r="B7" s="139"/>
+      <c r="C7" s="139"/>
+      <c r="D7" s="139"/>
+      <c r="E7" s="139"/>
+      <c r="F7" s="139"/>
+      <c r="G7" s="139"/>
+      <c r="H7" s="139"/>
+      <c r="I7" s="139"/>
+      <c r="J7" s="139"/>
+      <c r="K7" s="139"/>
+      <c r="L7" s="139"/>
+      <c r="M7" s="139"/>
+      <c r="N7" s="139"/>
     </row>
     <row r="8" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D8" s="136" t="s">
+      <c r="D8" s="140" t="s">
         <v>168</v>
       </c>
-      <c r="E8" s="137"/>
-      <c r="F8" s="137"/>
-      <c r="G8" s="137"/>
-      <c r="H8" s="137"/>
-      <c r="I8" s="138"/>
-      <c r="J8" s="139" t="s">
+      <c r="E8" s="141"/>
+      <c r="F8" s="141"/>
+      <c r="G8" s="141"/>
+      <c r="H8" s="141"/>
+      <c r="I8" s="142"/>
+      <c r="J8" s="143" t="s">
         <v>169</v>
       </c>
-      <c r="K8" s="139"/>
-      <c r="L8" s="139"/>
-      <c r="M8" s="139"/>
-      <c r="N8" s="139"/>
+      <c r="K8" s="143"/>
+      <c r="L8" s="143"/>
+      <c r="M8" s="143"/>
+      <c r="N8" s="143"/>
     </row>
     <row r="9" spans="2:14" s="24" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C9" s="31" t="s">
@@ -18118,247 +18180,555 @@
       </c>
     </row>
     <row r="10" spans="2:14" s="24" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="142" t="s">
-        <v>328</v>
+      <c r="B10" s="145" t="s">
+        <v>330</v>
       </c>
       <c r="C10" s="42" t="s">
         <v>177</v>
       </c>
-      <c r="D10" s="27"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="29"/>
+      <c r="D10" s="27" t="s">
+        <v>331</v>
+      </c>
+      <c r="E10" s="25">
+        <v>0.59</v>
+      </c>
+      <c r="F10" s="25">
+        <v>0.44</v>
+      </c>
+      <c r="G10" s="25">
+        <v>0.17</v>
+      </c>
+      <c r="H10" s="25">
+        <v>0.16</v>
+      </c>
+      <c r="I10" s="29">
+        <v>0.69</v>
+      </c>
+      <c r="J10" s="25">
+        <v>0.59</v>
+      </c>
+      <c r="K10" s="25">
+        <v>0.44</v>
+      </c>
+      <c r="L10" s="25">
+        <v>0.17</v>
+      </c>
+      <c r="M10" s="25">
+        <v>0.16</v>
+      </c>
+      <c r="N10" s="29">
+        <v>0.68</v>
+      </c>
     </row>
     <row r="11" spans="2:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="143"/>
+      <c r="B11" s="146"/>
       <c r="C11" s="42" t="s">
         <v>178</v>
       </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="29"/>
+      <c r="D11" s="27" t="s">
+        <v>332</v>
+      </c>
+      <c r="E11" s="25">
+        <v>0.75</v>
+      </c>
+      <c r="F11" s="25">
+        <v>0.47</v>
+      </c>
+      <c r="G11" s="25">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H11" s="25">
+        <v>0.3</v>
+      </c>
+      <c r="I11" s="29">
+        <v>0.89</v>
+      </c>
+      <c r="J11" s="25">
+        <v>0.75</v>
+      </c>
+      <c r="K11" s="25">
+        <v>0.49</v>
+      </c>
+      <c r="L11" s="25">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M11" s="25">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="N11" s="29">
+        <v>0.89</v>
+      </c>
     </row>
     <row r="12" spans="2:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="143"/>
+      <c r="B12" s="146"/>
       <c r="C12" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="D12" s="27"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="29"/>
+      <c r="D12" s="27" t="s">
+        <v>333</v>
+      </c>
+      <c r="E12" s="25">
+        <v>0.75</v>
+      </c>
+      <c r="F12" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="G12" s="25">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H12" s="25">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="I12" s="29">
+        <v>0.89</v>
+      </c>
+      <c r="J12" s="25">
+        <v>0.75</v>
+      </c>
+      <c r="K12" s="25">
+        <v>0.6</v>
+      </c>
+      <c r="L12" s="25">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M12" s="25">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="N12" s="29">
+        <v>0.89</v>
+      </c>
     </row>
     <row r="13" spans="2:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="143"/>
+      <c r="B13" s="146"/>
       <c r="C13" s="42" t="s">
         <v>180</v>
       </c>
-      <c r="D13" s="27"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="29"/>
+      <c r="D13" s="27" t="s">
+        <v>334</v>
+      </c>
+      <c r="E13" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="F13" s="25">
+        <v>0.44</v>
+      </c>
+      <c r="G13" s="25">
+        <v>0.13</v>
+      </c>
+      <c r="H13" s="25">
+        <v>0.09</v>
+      </c>
+      <c r="I13" s="29">
+        <v>0.65</v>
+      </c>
+      <c r="J13" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="K13" s="25">
+        <v>0.27</v>
+      </c>
+      <c r="L13" s="25">
+        <v>0.13</v>
+      </c>
+      <c r="M13" s="25">
+        <v>0.09</v>
+      </c>
+      <c r="N13" s="29">
+        <v>0.66</v>
+      </c>
     </row>
     <row r="14" spans="2:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="143"/>
+      <c r="B14" s="146"/>
       <c r="C14" s="42" t="s">
         <v>181</v>
       </c>
-      <c r="D14" s="27"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="29"/>
+      <c r="D14" s="27" t="s">
+        <v>335</v>
+      </c>
+      <c r="E14" s="25">
+        <v>0.67</v>
+      </c>
+      <c r="F14" s="25">
+        <v>0.38</v>
+      </c>
+      <c r="G14" s="25">
+        <v>0.22</v>
+      </c>
+      <c r="H14" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="I14" s="29">
+        <v>0.73</v>
+      </c>
+      <c r="J14" s="25">
+        <v>0.67</v>
+      </c>
+      <c r="K14" s="25">
+        <v>0.37</v>
+      </c>
+      <c r="L14" s="25">
+        <v>0.22</v>
+      </c>
+      <c r="M14" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="N14" s="29">
+        <v>0.73</v>
+      </c>
     </row>
     <row r="15" spans="2:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="143"/>
+      <c r="B15" s="146"/>
       <c r="C15" s="42" t="s">
         <v>182</v>
       </c>
-      <c r="D15" s="27"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
-      <c r="N15" s="29"/>
+      <c r="D15" s="27" t="s">
+        <v>336</v>
+      </c>
+      <c r="E15" s="25">
+        <v>0.71</v>
+      </c>
+      <c r="F15" s="25">
+        <v>0.44</v>
+      </c>
+      <c r="G15" s="25">
+        <v>0.35</v>
+      </c>
+      <c r="H15" s="25">
+        <v>0.34</v>
+      </c>
+      <c r="I15" s="29">
+        <v>0.9</v>
+      </c>
+      <c r="J15" s="25">
+        <v>0.71</v>
+      </c>
+      <c r="K15" s="25">
+        <v>0.39</v>
+      </c>
+      <c r="L15" s="25">
+        <v>0.35</v>
+      </c>
+      <c r="M15" s="25">
+        <v>0.34</v>
+      </c>
+      <c r="N15" s="29">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="16" spans="2:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="143"/>
+      <c r="B16" s="146"/>
       <c r="C16" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="D16" s="27"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="25"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="29"/>
+      <c r="D16" s="27" t="s">
+        <v>337</v>
+      </c>
+      <c r="E16" s="25">
+        <v>0.71</v>
+      </c>
+      <c r="F16" s="25">
+        <v>0.44</v>
+      </c>
+      <c r="G16" s="25">
+        <v>0.32</v>
+      </c>
+      <c r="H16" s="25">
+        <v>0.33</v>
+      </c>
+      <c r="I16" s="29">
+        <v>0.9</v>
+      </c>
+      <c r="J16" s="25">
+        <v>0.71</v>
+      </c>
+      <c r="K16" s="25">
+        <v>0.41</v>
+      </c>
+      <c r="L16" s="25">
+        <v>0.32</v>
+      </c>
+      <c r="M16" s="25">
+        <v>0.32</v>
+      </c>
+      <c r="N16" s="29">
+        <v>0.89</v>
+      </c>
     </row>
     <row r="17" spans="2:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="143"/>
+      <c r="B17" s="146"/>
       <c r="C17" s="42" t="s">
         <v>184</v>
       </c>
-      <c r="D17" s="27"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="29"/>
+      <c r="D17" s="27" t="s">
+        <v>338</v>
+      </c>
+      <c r="E17" s="25">
+        <v>0.64</v>
+      </c>
+      <c r="F17" s="25">
+        <v>0.33</v>
+      </c>
+      <c r="G17" s="25">
+        <v>0.39</v>
+      </c>
+      <c r="H17" s="25">
+        <v>0.33</v>
+      </c>
+      <c r="I17" s="29">
+        <v>0.89</v>
+      </c>
+      <c r="J17" s="25">
+        <v>0.65</v>
+      </c>
+      <c r="K17" s="25">
+        <v>0.33</v>
+      </c>
+      <c r="L17" s="25">
+        <v>0.39</v>
+      </c>
+      <c r="M17" s="25">
+        <v>0.33</v>
+      </c>
+      <c r="N17" s="29">
+        <v>0.89</v>
+      </c>
     </row>
     <row r="18" spans="2:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="143"/>
+      <c r="B18" s="146"/>
       <c r="C18" s="42" t="s">
         <v>185</v>
       </c>
-      <c r="D18" s="27"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="29"/>
+      <c r="D18" s="27" t="s">
+        <v>339</v>
+      </c>
+      <c r="E18" s="25">
+        <v>0.65</v>
+      </c>
+      <c r="F18" s="25">
+        <v>0.32</v>
+      </c>
+      <c r="G18" s="25">
+        <v>0.52</v>
+      </c>
+      <c r="H18" s="25">
+        <v>0.32</v>
+      </c>
+      <c r="I18" s="29">
+        <v>0.89</v>
+      </c>
+      <c r="J18" s="25">
+        <v>0.65</v>
+      </c>
+      <c r="K18" s="25">
+        <v>0.32</v>
+      </c>
+      <c r="L18" s="25">
+        <v>0.54</v>
+      </c>
+      <c r="M18" s="25">
+        <v>0.33</v>
+      </c>
+      <c r="N18" s="29">
+        <v>0.89</v>
+      </c>
     </row>
     <row r="19" spans="2:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="143"/>
+      <c r="B19" s="146"/>
       <c r="C19" s="42" t="s">
         <v>186</v>
       </c>
-      <c r="D19" s="27"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="29"/>
+      <c r="D19" s="27" t="s">
+        <v>340</v>
+      </c>
+      <c r="E19" s="25">
+        <v>0.78</v>
+      </c>
+      <c r="F19" s="25">
+        <v>0.63</v>
+      </c>
+      <c r="G19" s="25">
+        <v>0.37</v>
+      </c>
+      <c r="H19" s="25">
+        <v>0.4</v>
+      </c>
+      <c r="I19" s="29">
+        <v>0.88</v>
+      </c>
+      <c r="J19" s="25">
+        <v>0.73</v>
+      </c>
+      <c r="K19" s="25">
+        <v>0.46</v>
+      </c>
+      <c r="L19" s="25">
+        <v>0.32</v>
+      </c>
+      <c r="M19" s="25">
+        <v>0.33</v>
+      </c>
+      <c r="N19" s="29">
+        <v>0.73</v>
+      </c>
     </row>
     <row r="20" spans="2:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="143"/>
+      <c r="B20" s="146"/>
       <c r="C20" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="D20" s="27"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="25"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="29"/>
+      <c r="D20" s="27" t="s">
+        <v>341</v>
+      </c>
+      <c r="E20" s="25">
+        <v>0.78</v>
+      </c>
+      <c r="F20" s="25">
+        <v>0.63</v>
+      </c>
+      <c r="G20" s="25">
+        <v>0.39</v>
+      </c>
+      <c r="H20" s="25">
+        <v>0.42</v>
+      </c>
+      <c r="I20" s="29">
+        <v>0.88</v>
+      </c>
+      <c r="J20" s="25">
+        <v>0.74</v>
+      </c>
+      <c r="K20" s="25">
+        <v>0.42</v>
+      </c>
+      <c r="L20" s="25">
+        <v>0.34</v>
+      </c>
+      <c r="M20" s="25">
+        <v>0.36</v>
+      </c>
+      <c r="N20" s="29">
+        <v>0.74</v>
+      </c>
     </row>
     <row r="21" spans="2:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="143"/>
+      <c r="B21" s="146"/>
       <c r="C21" s="42" t="s">
         <v>188</v>
       </c>
-      <c r="D21" s="27"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="25"/>
-      <c r="M21" s="25"/>
-      <c r="N21" s="29"/>
+      <c r="D21" s="27" t="s">
+        <v>342</v>
+      </c>
+      <c r="E21" s="25">
+        <v>0.78</v>
+      </c>
+      <c r="F21" s="25">
+        <v>0.64</v>
+      </c>
+      <c r="G21" s="25">
+        <v>0.39</v>
+      </c>
+      <c r="H21" s="25">
+        <v>0.43</v>
+      </c>
+      <c r="I21" s="29">
+        <v>0.88</v>
+      </c>
+      <c r="J21" s="25">
+        <v>0.74</v>
+      </c>
+      <c r="K21" s="25">
+        <v>0.42</v>
+      </c>
+      <c r="L21" s="25">
+        <v>0.34</v>
+      </c>
+      <c r="M21" s="25">
+        <v>0.36</v>
+      </c>
+      <c r="N21" s="29">
+        <v>0.74</v>
+      </c>
     </row>
     <row r="22" spans="2:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="143"/>
+      <c r="B22" s="146"/>
       <c r="C22" s="42" t="s">
         <v>189</v>
       </c>
-      <c r="D22" s="27"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
-      <c r="M22" s="25"/>
-      <c r="N22" s="29"/>
+      <c r="D22" s="27" t="s">
+        <v>343</v>
+      </c>
+      <c r="E22" s="25">
+        <v>0.48</v>
+      </c>
+      <c r="F22" s="25">
+        <v>0.36</v>
+      </c>
+      <c r="G22" s="25">
+        <v>0.19</v>
+      </c>
+      <c r="H22" s="25">
+        <v>0.19</v>
+      </c>
+      <c r="I22" s="29">
+        <v>0.62</v>
+      </c>
+      <c r="J22" s="25">
+        <v>0.46</v>
+      </c>
+      <c r="K22" s="25">
+        <v>0.26</v>
+      </c>
+      <c r="L22" s="25">
+        <v>0.17</v>
+      </c>
+      <c r="M22" s="25">
+        <v>0.17</v>
+      </c>
+      <c r="N22" s="29">
+        <v>0.56999999999999995</v>
+      </c>
     </row>
     <row r="23" spans="2:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="143"/>
+      <c r="B23" s="146"/>
       <c r="C23" s="42" t="s">
         <v>190</v>
       </c>
-      <c r="D23" s="27"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="29"/>
+      <c r="D23" s="27" t="s">
+        <v>344</v>
+      </c>
+      <c r="E23" s="25">
+        <v>0.78</v>
+      </c>
+      <c r="F23" s="25">
+        <v>0.63</v>
+      </c>
+      <c r="G23" s="25">
+        <v>0.39</v>
+      </c>
+      <c r="H23" s="25">
+        <v>0.42</v>
+      </c>
+      <c r="I23" s="29">
+        <v>0.88</v>
+      </c>
+      <c r="J23" s="25">
+        <v>0.74</v>
+      </c>
+      <c r="K23" s="25">
+        <v>0.42</v>
+      </c>
+      <c r="L23" s="25">
+        <v>0.34</v>
+      </c>
+      <c r="M23" s="25">
+        <v>0.36</v>
+      </c>
+      <c r="N23" s="29">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="24" spans="2:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="143"/>
+      <c r="B24" s="146"/>
       <c r="C24" s="42" t="s">
         <v>191</v>
       </c>
@@ -18375,7 +18745,7 @@
       <c r="N24" s="29"/>
     </row>
     <row r="25" spans="2:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="143"/>
+      <c r="B25" s="146"/>
       <c r="C25" s="42" t="s">
         <v>192</v>
       </c>
@@ -18392,7 +18762,7 @@
       <c r="N25" s="29"/>
     </row>
     <row r="26" spans="2:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="143"/>
+      <c r="B26" s="146"/>
       <c r="C26" s="42" t="s">
         <v>193</v>
       </c>
@@ -18409,7 +18779,7 @@
       <c r="N26" s="29"/>
     </row>
     <row r="27" spans="2:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="143"/>
+      <c r="B27" s="146"/>
       <c r="C27" s="42" t="s">
         <v>194</v>
       </c>
@@ -18426,7 +18796,7 @@
       <c r="N27" s="29"/>
     </row>
     <row r="28" spans="2:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="143"/>
+      <c r="B28" s="146"/>
       <c r="C28" s="42" t="s">
         <v>195</v>
       </c>
@@ -18443,7 +18813,7 @@
       <c r="N28" s="29"/>
     </row>
     <row r="29" spans="2:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="143"/>
+      <c r="B29" s="146"/>
       <c r="C29" s="42" t="s">
         <v>196</v>
       </c>
@@ -18460,7 +18830,7 @@
       <c r="N29" s="29"/>
     </row>
     <row r="30" spans="2:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="143"/>
+      <c r="B30" s="146"/>
       <c r="C30" s="42" t="s">
         <v>197</v>
       </c>
@@ -18477,7 +18847,7 @@
       <c r="N30" s="29"/>
     </row>
     <row r="31" spans="2:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="143"/>
+      <c r="B31" s="146"/>
       <c r="C31" s="42" t="s">
         <v>198</v>
       </c>
@@ -18494,7 +18864,7 @@
       <c r="N31" s="29"/>
     </row>
     <row r="32" spans="2:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="143"/>
+      <c r="B32" s="146"/>
       <c r="C32" s="42" t="s">
         <v>199</v>
       </c>
@@ -18511,7 +18881,7 @@
       <c r="N32" s="29"/>
     </row>
     <row r="33" spans="2:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="143"/>
+      <c r="B33" s="146"/>
       <c r="C33" s="42" t="s">
         <v>200</v>
       </c>
@@ -18528,7 +18898,7 @@
       <c r="N33" s="29"/>
     </row>
     <row r="34" spans="2:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="143"/>
+      <c r="B34" s="146"/>
       <c r="C34" s="42" t="s">
         <v>230</v>
       </c>
@@ -18545,7 +18915,7 @@
       <c r="N34" s="29"/>
     </row>
     <row r="35" spans="2:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="143"/>
+      <c r="B35" s="146"/>
       <c r="C35" s="42" t="s">
         <v>201</v>
       </c>
@@ -18562,7 +18932,7 @@
       <c r="N35" s="29"/>
     </row>
     <row r="36" spans="2:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="143"/>
+      <c r="B36" s="146"/>
       <c r="C36" s="42" t="s">
         <v>201</v>
       </c>
@@ -18579,7 +18949,7 @@
       <c r="N36" s="29"/>
     </row>
     <row r="37" spans="2:14" s="24" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="144"/>
+      <c r="B37" s="147"/>
       <c r="C37" s="34" t="s">
         <v>201</v>
       </c>
@@ -18596,7 +18966,7 @@
       <c r="N37" s="30"/>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B38" s="140" t="s">
+      <c r="B38" s="144" t="s">
         <v>158</v>
       </c>
       <c r="C38" s="42" t="s">
@@ -18637,7 +19007,7 @@
       </c>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B39" s="132"/>
+      <c r="B39" s="136"/>
       <c r="C39" s="42" t="s">
         <v>178</v>
       </c>
@@ -18676,7 +19046,7 @@
       </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B40" s="132"/>
+      <c r="B40" s="136"/>
       <c r="C40" s="42" t="s">
         <v>179</v>
       </c>
@@ -18715,7 +19085,7 @@
       </c>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B41" s="132"/>
+      <c r="B41" s="136"/>
       <c r="C41" s="42" t="s">
         <v>180</v>
       </c>
@@ -18754,7 +19124,7 @@
       </c>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B42" s="132"/>
+      <c r="B42" s="136"/>
       <c r="C42" s="42" t="s">
         <v>181</v>
       </c>
@@ -18793,7 +19163,7 @@
       </c>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B43" s="132"/>
+      <c r="B43" s="136"/>
       <c r="C43" s="42" t="s">
         <v>182</v>
       </c>
@@ -18832,7 +19202,7 @@
       </c>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B44" s="132"/>
+      <c r="B44" s="136"/>
       <c r="C44" s="42" t="s">
         <v>183</v>
       </c>
@@ -18871,7 +19241,7 @@
       </c>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B45" s="132"/>
+      <c r="B45" s="136"/>
       <c r="C45" s="42" t="s">
         <v>184</v>
       </c>
@@ -18910,7 +19280,7 @@
       </c>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B46" s="132"/>
+      <c r="B46" s="136"/>
       <c r="C46" s="42" t="s">
         <v>185</v>
       </c>
@@ -18949,7 +19319,7 @@
       </c>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B47" s="132"/>
+      <c r="B47" s="136"/>
       <c r="C47" s="42" t="s">
         <v>186</v>
       </c>
@@ -18966,7 +19336,7 @@
       <c r="N47" s="29"/>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B48" s="132"/>
+      <c r="B48" s="136"/>
       <c r="C48" s="42" t="s">
         <v>187</v>
       </c>
@@ -18983,7 +19353,7 @@
       <c r="N48" s="29"/>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B49" s="132"/>
+      <c r="B49" s="136"/>
       <c r="C49" s="42" t="s">
         <v>188</v>
       </c>
@@ -19000,7 +19370,7 @@
       <c r="N49" s="29"/>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B50" s="132"/>
+      <c r="B50" s="136"/>
       <c r="C50" s="42" t="s">
         <v>189</v>
       </c>
@@ -19017,7 +19387,7 @@
       <c r="N50" s="29"/>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B51" s="132"/>
+      <c r="B51" s="136"/>
       <c r="C51" s="42" t="s">
         <v>190</v>
       </c>
@@ -19034,7 +19404,7 @@
       <c r="N51" s="29"/>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B52" s="132"/>
+      <c r="B52" s="136"/>
       <c r="C52" s="42" t="s">
         <v>191</v>
       </c>
@@ -19051,7 +19421,7 @@
       <c r="N52" s="65"/>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B53" s="132"/>
+      <c r="B53" s="136"/>
       <c r="C53" s="42" t="s">
         <v>192</v>
       </c>
@@ -19068,7 +19438,7 @@
       <c r="N53" s="65"/>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B54" s="132"/>
+      <c r="B54" s="136"/>
       <c r="C54" s="42" t="s">
         <v>193</v>
       </c>
@@ -19085,7 +19455,7 @@
       <c r="N54" s="65"/>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B55" s="132"/>
+      <c r="B55" s="136"/>
       <c r="C55" s="42" t="s">
         <v>194</v>
       </c>
@@ -19102,7 +19472,7 @@
       <c r="N55" s="65"/>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B56" s="132"/>
+      <c r="B56" s="136"/>
       <c r="C56" s="42" t="s">
         <v>195</v>
       </c>
@@ -19122,7 +19492,7 @@
       </c>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B57" s="132"/>
+      <c r="B57" s="136"/>
       <c r="C57" s="42" t="s">
         <v>196</v>
       </c>
@@ -19139,7 +19509,7 @@
       <c r="N57" s="65"/>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B58" s="132"/>
+      <c r="B58" s="136"/>
       <c r="C58" s="42" t="s">
         <v>197</v>
       </c>
@@ -19156,7 +19526,7 @@
       <c r="N58" s="65"/>
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B59" s="132"/>
+      <c r="B59" s="136"/>
       <c r="C59" s="42" t="s">
         <v>198</v>
       </c>
@@ -19173,7 +19543,7 @@
       <c r="N59" s="65"/>
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B60" s="132"/>
+      <c r="B60" s="136"/>
       <c r="C60" s="42" t="s">
         <v>199</v>
       </c>
@@ -19190,7 +19560,7 @@
       <c r="N60" s="65"/>
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B61" s="132"/>
+      <c r="B61" s="136"/>
       <c r="C61" s="42" t="s">
         <v>200</v>
       </c>
@@ -19210,7 +19580,7 @@
       </c>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B62" s="132"/>
+      <c r="B62" s="136"/>
       <c r="C62" s="42" t="s">
         <v>201</v>
       </c>
@@ -19227,7 +19597,7 @@
       <c r="N62" s="29"/>
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B63" s="132"/>
+      <c r="B63" s="136"/>
       <c r="C63" s="42" t="s">
         <v>201</v>
       </c>
@@ -19244,7 +19614,7 @@
       <c r="N63" s="29"/>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B64" s="132"/>
+      <c r="B64" s="136"/>
       <c r="C64" s="42" t="s">
         <v>201</v>
       </c>
@@ -19261,7 +19631,7 @@
       <c r="N64" s="29"/>
     </row>
     <row r="65" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B65" s="133"/>
+      <c r="B65" s="137"/>
       <c r="C65" s="34" t="s">
         <v>201</v>
       </c>
@@ -19278,7 +19648,7 @@
       <c r="N65" s="30"/>
     </row>
     <row r="66" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B66" s="131" t="s">
+      <c r="B66" s="135" t="s">
         <v>159</v>
       </c>
       <c r="C66" s="42" t="s">
@@ -19319,7 +19689,7 @@
       </c>
     </row>
     <row r="67" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B67" s="132"/>
+      <c r="B67" s="136"/>
       <c r="C67" s="42" t="s">
         <v>178</v>
       </c>
@@ -19358,7 +19728,7 @@
       </c>
     </row>
     <row r="68" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B68" s="132"/>
+      <c r="B68" s="136"/>
       <c r="C68" s="42" t="s">
         <v>179</v>
       </c>
@@ -19397,7 +19767,7 @@
       </c>
     </row>
     <row r="69" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B69" s="132"/>
+      <c r="B69" s="136"/>
       <c r="C69" s="42" t="s">
         <v>180</v>
       </c>
@@ -19436,7 +19806,7 @@
       </c>
     </row>
     <row r="70" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B70" s="132"/>
+      <c r="B70" s="136"/>
       <c r="C70" s="42" t="s">
         <v>181</v>
       </c>
@@ -19475,7 +19845,7 @@
       </c>
     </row>
     <row r="71" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B71" s="132"/>
+      <c r="B71" s="136"/>
       <c r="C71" s="42" t="s">
         <v>182</v>
       </c>
@@ -19514,7 +19884,7 @@
       </c>
     </row>
     <row r="72" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B72" s="132"/>
+      <c r="B72" s="136"/>
       <c r="C72" s="42" t="s">
         <v>183</v>
       </c>
@@ -19553,7 +19923,7 @@
       </c>
     </row>
     <row r="73" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B73" s="132"/>
+      <c r="B73" s="136"/>
       <c r="C73" s="42" t="s">
         <v>184</v>
       </c>
@@ -19592,7 +19962,7 @@
       </c>
     </row>
     <row r="74" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B74" s="132"/>
+      <c r="B74" s="136"/>
       <c r="C74" s="42" t="s">
         <v>185</v>
       </c>
@@ -19631,7 +20001,7 @@
       </c>
     </row>
     <row r="75" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B75" s="132"/>
+      <c r="B75" s="136"/>
       <c r="C75" s="42" t="s">
         <v>186</v>
       </c>
@@ -19670,7 +20040,7 @@
       </c>
     </row>
     <row r="76" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B76" s="132"/>
+      <c r="B76" s="136"/>
       <c r="C76" s="42" t="s">
         <v>187</v>
       </c>
@@ -19709,7 +20079,7 @@
       </c>
     </row>
     <row r="77" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B77" s="132"/>
+      <c r="B77" s="136"/>
       <c r="C77" s="42" t="s">
         <v>188</v>
       </c>
@@ -19748,7 +20118,7 @@
       </c>
     </row>
     <row r="78" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B78" s="132"/>
+      <c r="B78" s="136"/>
       <c r="C78" s="42" t="s">
         <v>189</v>
       </c>
@@ -19787,7 +20157,7 @@
       </c>
     </row>
     <row r="79" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B79" s="132"/>
+      <c r="B79" s="136"/>
       <c r="C79" s="42" t="s">
         <v>190</v>
       </c>
@@ -19826,7 +20196,7 @@
       </c>
     </row>
     <row r="80" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B80" s="132"/>
+      <c r="B80" s="136"/>
       <c r="C80" s="42" t="s">
         <v>191</v>
       </c>
@@ -19865,7 +20235,7 @@
       </c>
     </row>
     <row r="81" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B81" s="132"/>
+      <c r="B81" s="136"/>
       <c r="C81" s="42" t="s">
         <v>192</v>
       </c>
@@ -19904,7 +20274,7 @@
       </c>
     </row>
     <row r="82" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B82" s="132"/>
+      <c r="B82" s="136"/>
       <c r="C82" s="42" t="s">
         <v>193</v>
       </c>
@@ -19943,7 +20313,7 @@
       </c>
     </row>
     <row r="83" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B83" s="132"/>
+      <c r="B83" s="136"/>
       <c r="C83" s="42" t="s">
         <v>194</v>
       </c>
@@ -19982,7 +20352,7 @@
       </c>
     </row>
     <row r="84" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B84" s="132"/>
+      <c r="B84" s="136"/>
       <c r="C84" s="42" t="s">
         <v>195</v>
       </c>
@@ -20021,7 +20391,7 @@
       </c>
     </row>
     <row r="85" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B85" s="132"/>
+      <c r="B85" s="136"/>
       <c r="C85" s="42" t="s">
         <v>196</v>
       </c>
@@ -20060,7 +20430,7 @@
       </c>
     </row>
     <row r="86" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B86" s="132"/>
+      <c r="B86" s="136"/>
       <c r="C86" s="42" t="s">
         <v>197</v>
       </c>
@@ -20099,7 +20469,7 @@
       </c>
     </row>
     <row r="87" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B87" s="132"/>
+      <c r="B87" s="136"/>
       <c r="C87" s="42" t="s">
         <v>198</v>
       </c>
@@ -20138,7 +20508,7 @@
       </c>
     </row>
     <row r="88" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B88" s="132"/>
+      <c r="B88" s="136"/>
       <c r="C88" s="42" t="s">
         <v>199</v>
       </c>
@@ -20177,7 +20547,7 @@
       </c>
     </row>
     <row r="89" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B89" s="132"/>
+      <c r="B89" s="136"/>
       <c r="C89" s="42" t="s">
         <v>200</v>
       </c>
@@ -20216,7 +20586,7 @@
       </c>
     </row>
     <row r="90" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B90" s="132"/>
+      <c r="B90" s="136"/>
       <c r="C90" s="42" t="s">
         <v>201</v>
       </c>
@@ -20233,7 +20603,7 @@
       <c r="N90" s="29"/>
     </row>
     <row r="91" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B91" s="132"/>
+      <c r="B91" s="136"/>
       <c r="C91" s="42" t="s">
         <v>201</v>
       </c>
@@ -20250,7 +20620,7 @@
       <c r="N91" s="29"/>
     </row>
     <row r="92" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B92" s="132"/>
+      <c r="B92" s="136"/>
       <c r="C92" s="42" t="s">
         <v>201</v>
       </c>
@@ -20267,7 +20637,7 @@
       <c r="N92" s="29"/>
     </row>
     <row r="93" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B93" s="133"/>
+      <c r="B93" s="137"/>
       <c r="C93" s="34" t="s">
         <v>201</v>
       </c>
@@ -20284,7 +20654,7 @@
       <c r="N93" s="30"/>
     </row>
     <row r="94" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B94" s="131" t="s">
+      <c r="B94" s="135" t="s">
         <v>160</v>
       </c>
       <c r="C94" s="42" t="s">
@@ -20303,7 +20673,7 @@
       <c r="N94" s="29"/>
     </row>
     <row r="95" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B95" s="132"/>
+      <c r="B95" s="136"/>
       <c r="C95" s="42" t="s">
         <v>178</v>
       </c>
@@ -20320,7 +20690,7 @@
       <c r="N95" s="29"/>
     </row>
     <row r="96" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B96" s="132"/>
+      <c r="B96" s="136"/>
       <c r="C96" s="42" t="s">
         <v>179</v>
       </c>
@@ -20359,7 +20729,7 @@
       </c>
     </row>
     <row r="97" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B97" s="132"/>
+      <c r="B97" s="136"/>
       <c r="C97" s="42" t="s">
         <v>180</v>
       </c>
@@ -20380,7 +20750,7 @@
       <c r="N97" s="29"/>
     </row>
     <row r="98" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B98" s="132"/>
+      <c r="B98" s="136"/>
       <c r="C98" s="42" t="s">
         <v>181</v>
       </c>
@@ -20401,7 +20771,7 @@
       <c r="N98" s="29"/>
     </row>
     <row r="99" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B99" s="132"/>
+      <c r="B99" s="136"/>
       <c r="C99" s="42" t="s">
         <v>182</v>
       </c>
@@ -20440,7 +20810,7 @@
       </c>
     </row>
     <row r="100" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B100" s="132"/>
+      <c r="B100" s="136"/>
       <c r="C100" s="42" t="s">
         <v>183</v>
       </c>
@@ -20461,7 +20831,7 @@
       <c r="N100" s="29"/>
     </row>
     <row r="101" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B101" s="132"/>
+      <c r="B101" s="136"/>
       <c r="C101" s="42" t="s">
         <v>184</v>
       </c>
@@ -20500,7 +20870,7 @@
       </c>
     </row>
     <row r="102" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B102" s="132"/>
+      <c r="B102" s="136"/>
       <c r="C102" s="42" t="s">
         <v>185</v>
       </c>
@@ -20521,7 +20891,7 @@
       <c r="N102" s="29"/>
     </row>
     <row r="103" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B103" s="132"/>
+      <c r="B103" s="136"/>
       <c r="C103" s="42" t="s">
         <v>186</v>
       </c>
@@ -20542,7 +20912,7 @@
       <c r="N103" s="29"/>
     </row>
     <row r="104" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B104" s="132"/>
+      <c r="B104" s="136"/>
       <c r="C104" s="42" t="s">
         <v>187</v>
       </c>
@@ -20563,7 +20933,7 @@
       <c r="N104" s="29"/>
     </row>
     <row r="105" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B105" s="132"/>
+      <c r="B105" s="136"/>
       <c r="C105" s="42" t="s">
         <v>188</v>
       </c>
@@ -20584,7 +20954,7 @@
       <c r="N105" s="29"/>
     </row>
     <row r="106" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B106" s="132"/>
+      <c r="B106" s="136"/>
       <c r="C106" s="42" t="s">
         <v>189</v>
       </c>
@@ -20605,7 +20975,7 @@
       <c r="N106" s="29"/>
     </row>
     <row r="107" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B107" s="132"/>
+      <c r="B107" s="136"/>
       <c r="C107" s="42" t="s">
         <v>190</v>
       </c>
@@ -20626,7 +20996,7 @@
       <c r="N107" s="29"/>
     </row>
     <row r="108" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B108" s="132"/>
+      <c r="B108" s="136"/>
       <c r="C108" s="42" t="s">
         <v>191</v>
       </c>
@@ -20647,7 +21017,7 @@
       <c r="N108" s="29"/>
     </row>
     <row r="109" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B109" s="132"/>
+      <c r="B109" s="136"/>
       <c r="C109" s="42" t="s">
         <v>192</v>
       </c>
@@ -20668,7 +21038,7 @@
       <c r="N109" s="29"/>
     </row>
     <row r="110" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B110" s="132"/>
+      <c r="B110" s="136"/>
       <c r="C110" s="42" t="s">
         <v>193</v>
       </c>
@@ -20707,7 +21077,7 @@
       </c>
     </row>
     <row r="111" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B111" s="132"/>
+      <c r="B111" s="136"/>
       <c r="C111" s="42" t="s">
         <v>194</v>
       </c>
@@ -20728,7 +21098,7 @@
       <c r="N111" s="29"/>
     </row>
     <row r="112" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B112" s="132"/>
+      <c r="B112" s="136"/>
       <c r="C112" s="42" t="s">
         <v>195</v>
       </c>
@@ -20749,7 +21119,7 @@
       <c r="N112" s="29"/>
     </row>
     <row r="113" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B113" s="132"/>
+      <c r="B113" s="136"/>
       <c r="C113" s="42" t="s">
         <v>196</v>
       </c>
@@ -20770,7 +21140,7 @@
       <c r="N113" s="29"/>
     </row>
     <row r="114" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B114" s="132"/>
+      <c r="B114" s="136"/>
       <c r="C114" s="42" t="s">
         <v>197</v>
       </c>
@@ -20791,7 +21161,7 @@
       <c r="N114" s="29"/>
     </row>
     <row r="115" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B115" s="132"/>
+      <c r="B115" s="136"/>
       <c r="C115" s="42" t="s">
         <v>198</v>
       </c>
@@ -20830,7 +21200,7 @@
       </c>
     </row>
     <row r="116" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B116" s="132"/>
+      <c r="B116" s="136"/>
       <c r="C116" s="42" t="s">
         <v>199</v>
       </c>
@@ -20847,7 +21217,7 @@
       <c r="N116" s="29"/>
     </row>
     <row r="117" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B117" s="132"/>
+      <c r="B117" s="136"/>
       <c r="C117" s="42" t="s">
         <v>200</v>
       </c>
@@ -20864,7 +21234,7 @@
       <c r="N117" s="29"/>
     </row>
     <row r="118" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B118" s="132"/>
+      <c r="B118" s="136"/>
       <c r="C118" s="42" t="s">
         <v>201</v>
       </c>
@@ -20881,7 +21251,7 @@
       <c r="N118" s="29"/>
     </row>
     <row r="119" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B119" s="132"/>
+      <c r="B119" s="136"/>
       <c r="C119" s="42" t="s">
         <v>201</v>
       </c>
@@ -20898,7 +21268,7 @@
       <c r="N119" s="29"/>
     </row>
     <row r="120" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B120" s="132"/>
+      <c r="B120" s="136"/>
       <c r="C120" s="42" t="s">
         <v>201</v>
       </c>
@@ -20915,7 +21285,7 @@
       <c r="N120" s="29"/>
     </row>
     <row r="121" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B121" s="133"/>
+      <c r="B121" s="137"/>
       <c r="C121" s="34" t="s">
         <v>201</v>
       </c>
@@ -20932,7 +21302,7 @@
       <c r="N121" s="30"/>
     </row>
     <row r="122" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B122" s="131" t="s">
+      <c r="B122" s="135" t="s">
         <v>161</v>
       </c>
       <c r="C122" s="42" t="s">
@@ -20951,7 +21321,7 @@
       <c r="N122" s="29"/>
     </row>
     <row r="123" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B123" s="132"/>
+      <c r="B123" s="136"/>
       <c r="C123" s="67" t="s">
         <v>298</v>
       </c>
@@ -20980,7 +21350,7 @@
       </c>
     </row>
     <row r="124" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B124" s="132"/>
+      <c r="B124" s="136"/>
       <c r="C124" s="67" t="s">
         <v>299</v>
       </c>
@@ -21009,7 +21379,7 @@
       </c>
     </row>
     <row r="125" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B125" s="132"/>
+      <c r="B125" s="136"/>
       <c r="C125" s="67" t="s">
         <v>297</v>
       </c>
@@ -21038,7 +21408,7 @@
       </c>
     </row>
     <row r="126" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B126" s="132"/>
+      <c r="B126" s="136"/>
       <c r="C126" s="42" t="s">
         <v>181</v>
       </c>
@@ -21055,7 +21425,7 @@
       <c r="N126" s="29"/>
     </row>
     <row r="127" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B127" s="132"/>
+      <c r="B127" s="136"/>
       <c r="C127" s="42" t="s">
         <v>182</v>
       </c>
@@ -21072,7 +21442,7 @@
       <c r="N127" s="29"/>
     </row>
     <row r="128" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B128" s="132"/>
+      <c r="B128" s="136"/>
       <c r="C128" s="42" t="s">
         <v>183</v>
       </c>
@@ -21089,7 +21459,7 @@
       <c r="N128" s="29"/>
     </row>
     <row r="129" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B129" s="132"/>
+      <c r="B129" s="136"/>
       <c r="C129" s="67" t="s">
         <v>300</v>
       </c>
@@ -21106,7 +21476,7 @@
       <c r="N129" s="29"/>
     </row>
     <row r="130" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B130" s="132"/>
+      <c r="B130" s="136"/>
       <c r="C130" s="68" t="s">
         <v>301</v>
       </c>
@@ -21135,7 +21505,7 @@
       </c>
     </row>
     <row r="131" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B131" s="132"/>
+      <c r="B131" s="136"/>
       <c r="C131" s="68" t="s">
         <v>302</v>
       </c>
@@ -21164,7 +21534,7 @@
       </c>
     </row>
     <row r="132" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B132" s="132"/>
+      <c r="B132" s="136"/>
       <c r="C132" s="67" t="s">
         <v>303</v>
       </c>
@@ -21193,7 +21563,7 @@
       </c>
     </row>
     <row r="133" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B133" s="132"/>
+      <c r="B133" s="136"/>
       <c r="C133" s="42" t="s">
         <v>186</v>
       </c>
@@ -21210,7 +21580,7 @@
       <c r="N133" s="29"/>
     </row>
     <row r="134" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B134" s="132"/>
+      <c r="B134" s="136"/>
       <c r="C134" s="67" t="s">
         <v>304</v>
       </c>
@@ -21227,7 +21597,7 @@
       <c r="N134" s="29"/>
     </row>
     <row r="135" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B135" s="132"/>
+      <c r="B135" s="136"/>
       <c r="C135" s="67" t="s">
         <v>305</v>
       </c>
@@ -21256,7 +21626,7 @@
       </c>
     </row>
     <row r="136" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B136" s="132"/>
+      <c r="B136" s="136"/>
       <c r="C136" s="67" t="s">
         <v>306</v>
       </c>
@@ -21273,7 +21643,7 @@
       <c r="N136" s="29"/>
     </row>
     <row r="137" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B137" s="132"/>
+      <c r="B137" s="136"/>
       <c r="C137" s="42" t="s">
         <v>190</v>
       </c>
@@ -21290,7 +21660,7 @@
       <c r="N137" s="29"/>
     </row>
     <row r="138" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B138" s="132"/>
+      <c r="B138" s="136"/>
       <c r="C138" s="42" t="s">
         <v>191</v>
       </c>
@@ -21307,7 +21677,7 @@
       <c r="N138" s="29"/>
     </row>
     <row r="139" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B139" s="132"/>
+      <c r="B139" s="136"/>
       <c r="C139" s="67" t="s">
         <v>307</v>
       </c>
@@ -21324,7 +21694,7 @@
       <c r="N139" s="29"/>
     </row>
     <row r="140" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B140" s="132"/>
+      <c r="B140" s="136"/>
       <c r="C140" s="67" t="s">
         <v>308</v>
       </c>
@@ -21341,7 +21711,7 @@
       <c r="N140" s="29"/>
     </row>
     <row r="141" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B141" s="132"/>
+      <c r="B141" s="136"/>
       <c r="C141" s="67" t="s">
         <v>309</v>
       </c>
@@ -21358,7 +21728,7 @@
       <c r="N141" s="29"/>
     </row>
     <row r="142" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B142" s="132"/>
+      <c r="B142" s="136"/>
       <c r="C142" s="42" t="s">
         <v>195</v>
       </c>
@@ -21375,7 +21745,7 @@
       <c r="N142" s="29"/>
     </row>
     <row r="143" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B143" s="132"/>
+      <c r="B143" s="136"/>
       <c r="C143" s="42" t="s">
         <v>196</v>
       </c>
@@ -21392,7 +21762,7 @@
       <c r="N143" s="29"/>
     </row>
     <row r="144" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B144" s="132"/>
+      <c r="B144" s="136"/>
       <c r="C144" s="42" t="s">
         <v>197</v>
       </c>
@@ -21409,7 +21779,7 @@
       <c r="N144" s="29"/>
     </row>
     <row r="145" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B145" s="132"/>
+      <c r="B145" s="136"/>
       <c r="C145" s="42" t="s">
         <v>198</v>
       </c>
@@ -21426,7 +21796,7 @@
       <c r="N145" s="29"/>
     </row>
     <row r="146" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B146" s="132"/>
+      <c r="B146" s="136"/>
       <c r="C146" s="42" t="s">
         <v>199</v>
       </c>
@@ -21443,7 +21813,7 @@
       <c r="N146" s="29"/>
     </row>
     <row r="147" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B147" s="132"/>
+      <c r="B147" s="136"/>
       <c r="C147" s="42" t="s">
         <v>200</v>
       </c>
@@ -21460,7 +21830,7 @@
       <c r="N147" s="29"/>
     </row>
     <row r="148" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B148" s="132"/>
+      <c r="B148" s="136"/>
       <c r="C148" s="42" t="s">
         <v>201</v>
       </c>
@@ -21477,7 +21847,7 @@
       <c r="N148" s="29"/>
     </row>
     <row r="149" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B149" s="132"/>
+      <c r="B149" s="136"/>
       <c r="C149" s="42" t="s">
         <v>310</v>
       </c>
@@ -21494,7 +21864,7 @@
       <c r="N149" s="29"/>
     </row>
     <row r="150" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B150" s="132"/>
+      <c r="B150" s="136"/>
       <c r="C150" s="42" t="s">
         <v>201</v>
       </c>
@@ -21511,7 +21881,7 @@
       <c r="N150" s="29"/>
     </row>
     <row r="151" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B151" s="133"/>
+      <c r="B151" s="137"/>
       <c r="C151" s="34" t="s">
         <v>201</v>
       </c>
@@ -21528,7 +21898,7 @@
       <c r="N151" s="30"/>
     </row>
     <row r="152" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B152" s="131" t="s">
+      <c r="B152" s="135" t="s">
         <v>162</v>
       </c>
       <c r="C152" s="42" t="s">
@@ -21547,7 +21917,7 @@
       <c r="N152" s="29"/>
     </row>
     <row r="153" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B153" s="132"/>
+      <c r="B153" s="136"/>
       <c r="C153" s="42" t="s">
         <v>178</v>
       </c>
@@ -21564,7 +21934,7 @@
       <c r="N153" s="29"/>
     </row>
     <row r="154" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B154" s="132"/>
+      <c r="B154" s="136"/>
       <c r="C154" s="42" t="s">
         <v>179</v>
       </c>
@@ -21581,7 +21951,7 @@
       <c r="N154" s="29"/>
     </row>
     <row r="155" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B155" s="132"/>
+      <c r="B155" s="136"/>
       <c r="C155" s="42" t="s">
         <v>180</v>
       </c>
@@ -21598,7 +21968,7 @@
       <c r="N155" s="29"/>
     </row>
     <row r="156" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B156" s="132"/>
+      <c r="B156" s="136"/>
       <c r="C156" s="42" t="s">
         <v>181</v>
       </c>
@@ -21615,7 +21985,7 @@
       <c r="N156" s="29"/>
     </row>
     <row r="157" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B157" s="132"/>
+      <c r="B157" s="136"/>
       <c r="C157" s="42" t="s">
         <v>182</v>
       </c>
@@ -21632,7 +22002,7 @@
       <c r="N157" s="29"/>
     </row>
     <row r="158" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B158" s="132"/>
+      <c r="B158" s="136"/>
       <c r="C158" s="42" t="s">
         <v>183</v>
       </c>
@@ -21649,7 +22019,7 @@
       <c r="N158" s="29"/>
     </row>
     <row r="159" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B159" s="132"/>
+      <c r="B159" s="136"/>
       <c r="C159" s="42" t="s">
         <v>184</v>
       </c>
@@ -21666,7 +22036,7 @@
       <c r="N159" s="29"/>
     </row>
     <row r="160" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B160" s="132"/>
+      <c r="B160" s="136"/>
       <c r="C160" s="42" t="s">
         <v>185</v>
       </c>
@@ -21683,7 +22053,7 @@
       <c r="N160" s="29"/>
     </row>
     <row r="161" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B161" s="132"/>
+      <c r="B161" s="136"/>
       <c r="C161" s="42" t="s">
         <v>186</v>
       </c>
@@ -21700,7 +22070,7 @@
       <c r="N161" s="29"/>
     </row>
     <row r="162" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B162" s="132"/>
+      <c r="B162" s="136"/>
       <c r="C162" s="42" t="s">
         <v>187</v>
       </c>
@@ -21717,7 +22087,7 @@
       <c r="N162" s="29"/>
     </row>
     <row r="163" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B163" s="132"/>
+      <c r="B163" s="136"/>
       <c r="C163" s="42" t="s">
         <v>188</v>
       </c>
@@ -21734,7 +22104,7 @@
       <c r="N163" s="29"/>
     </row>
     <row r="164" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B164" s="132"/>
+      <c r="B164" s="136"/>
       <c r="C164" s="42" t="s">
         <v>189</v>
       </c>
@@ -21751,7 +22121,7 @@
       <c r="N164" s="29"/>
     </row>
     <row r="165" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B165" s="132"/>
+      <c r="B165" s="136"/>
       <c r="C165" s="42" t="s">
         <v>190</v>
       </c>
@@ -21768,7 +22138,7 @@
       <c r="N165" s="29"/>
     </row>
     <row r="166" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B166" s="132"/>
+      <c r="B166" s="136"/>
       <c r="C166" s="42" t="s">
         <v>191</v>
       </c>
@@ -21785,7 +22155,7 @@
       <c r="N166" s="29"/>
     </row>
     <row r="167" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B167" s="132"/>
+      <c r="B167" s="136"/>
       <c r="C167" s="42" t="s">
         <v>192</v>
       </c>
@@ -21802,7 +22172,7 @@
       <c r="N167" s="29"/>
     </row>
     <row r="168" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B168" s="132"/>
+      <c r="B168" s="136"/>
       <c r="C168" s="42" t="s">
         <v>193</v>
       </c>
@@ -21819,7 +22189,7 @@
       <c r="N168" s="29"/>
     </row>
     <row r="169" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B169" s="132"/>
+      <c r="B169" s="136"/>
       <c r="C169" s="42" t="s">
         <v>194</v>
       </c>
@@ -21836,7 +22206,7 @@
       <c r="N169" s="29"/>
     </row>
     <row r="170" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B170" s="132"/>
+      <c r="B170" s="136"/>
       <c r="C170" s="42" t="s">
         <v>195</v>
       </c>
@@ -21853,7 +22223,7 @@
       <c r="N170" s="29"/>
     </row>
     <row r="171" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B171" s="132"/>
+      <c r="B171" s="136"/>
       <c r="C171" s="42" t="s">
         <v>196</v>
       </c>
@@ -21870,7 +22240,7 @@
       <c r="N171" s="29"/>
     </row>
     <row r="172" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B172" s="132"/>
+      <c r="B172" s="136"/>
       <c r="C172" s="42" t="s">
         <v>197</v>
       </c>
@@ -21887,7 +22257,7 @@
       <c r="N172" s="29"/>
     </row>
     <row r="173" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B173" s="132"/>
+      <c r="B173" s="136"/>
       <c r="C173" s="42" t="s">
         <v>198</v>
       </c>
@@ -21904,7 +22274,7 @@
       <c r="N173" s="29"/>
     </row>
     <row r="174" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B174" s="132"/>
+      <c r="B174" s="136"/>
       <c r="C174" s="42" t="s">
         <v>199</v>
       </c>
@@ -21921,7 +22291,7 @@
       <c r="N174" s="29"/>
     </row>
     <row r="175" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B175" s="132"/>
+      <c r="B175" s="136"/>
       <c r="C175" s="42" t="s">
         <v>200</v>
       </c>
@@ -21938,7 +22308,7 @@
       <c r="N175" s="29"/>
     </row>
     <row r="176" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B176" s="132"/>
+      <c r="B176" s="136"/>
       <c r="C176" s="42" t="s">
         <v>230</v>
       </c>
@@ -21955,7 +22325,7 @@
       <c r="N176" s="29"/>
     </row>
     <row r="177" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B177" s="132"/>
+      <c r="B177" s="136"/>
       <c r="C177" s="42" t="s">
         <v>201</v>
       </c>
@@ -21972,7 +22342,7 @@
       <c r="N177" s="29"/>
     </row>
     <row r="178" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B178" s="132"/>
+      <c r="B178" s="136"/>
       <c r="C178" s="42" t="s">
         <v>201</v>
       </c>
@@ -21989,7 +22359,7 @@
       <c r="N178" s="29"/>
     </row>
     <row r="179" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B179" s="133"/>
+      <c r="B179" s="137"/>
       <c r="C179" s="34" t="s">
         <v>201</v>
       </c>
@@ -22006,7 +22376,7 @@
       <c r="N179" s="30"/>
     </row>
     <row r="180" spans="2:14" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B180" s="128" t="s">
+      <c r="B180" s="132" t="s">
         <v>163</v>
       </c>
       <c r="C180" s="42" t="s">
@@ -22047,7 +22417,7 @@
       </c>
     </row>
     <row r="181" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B181" s="129"/>
+      <c r="B181" s="133"/>
       <c r="C181" s="42" t="s">
         <v>178</v>
       </c>
@@ -22086,7 +22456,7 @@
       </c>
     </row>
     <row r="182" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B182" s="129"/>
+      <c r="B182" s="133"/>
       <c r="C182" s="42" t="s">
         <v>179</v>
       </c>
@@ -22125,7 +22495,7 @@
       </c>
     </row>
     <row r="183" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B183" s="129"/>
+      <c r="B183" s="133"/>
       <c r="C183" s="42" t="s">
         <v>180</v>
       </c>
@@ -22164,7 +22534,7 @@
       </c>
     </row>
     <row r="184" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B184" s="129"/>
+      <c r="B184" s="133"/>
       <c r="C184" s="42" t="s">
         <v>181</v>
       </c>
@@ -22203,7 +22573,7 @@
       </c>
     </row>
     <row r="185" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B185" s="129"/>
+      <c r="B185" s="133"/>
       <c r="C185" s="42" t="s">
         <v>182</v>
       </c>
@@ -22242,7 +22612,7 @@
       </c>
     </row>
     <row r="186" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B186" s="129"/>
+      <c r="B186" s="133"/>
       <c r="C186" s="42" t="s">
         <v>183</v>
       </c>
@@ -22281,7 +22651,7 @@
       </c>
     </row>
     <row r="187" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B187" s="129"/>
+      <c r="B187" s="133"/>
       <c r="C187" s="42" t="s">
         <v>184</v>
       </c>
@@ -22320,7 +22690,7 @@
       </c>
     </row>
     <row r="188" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B188" s="129"/>
+      <c r="B188" s="133"/>
       <c r="C188" s="42" t="s">
         <v>185</v>
       </c>
@@ -22359,7 +22729,7 @@
       </c>
     </row>
     <row r="189" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B189" s="129"/>
+      <c r="B189" s="133"/>
       <c r="C189" s="42" t="s">
         <v>207</v>
       </c>
@@ -22398,7 +22768,7 @@
       </c>
     </row>
     <row r="190" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B190" s="129"/>
+      <c r="B190" s="133"/>
       <c r="C190" s="42" t="s">
         <v>208</v>
       </c>
@@ -22437,7 +22807,7 @@
       </c>
     </row>
     <row r="191" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B191" s="129"/>
+      <c r="B191" s="133"/>
       <c r="C191" s="42" t="s">
         <v>209</v>
       </c>
@@ -22476,7 +22846,7 @@
       </c>
     </row>
     <row r="192" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B192" s="129"/>
+      <c r="B192" s="133"/>
       <c r="C192" s="42" t="s">
         <v>210</v>
       </c>
@@ -22515,7 +22885,7 @@
       </c>
     </row>
     <row r="193" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B193" s="129"/>
+      <c r="B193" s="133"/>
       <c r="C193" s="42" t="s">
         <v>211</v>
       </c>
@@ -22554,7 +22924,7 @@
       </c>
     </row>
     <row r="194" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B194" s="129"/>
+      <c r="B194" s="133"/>
       <c r="C194" s="75" t="s">
         <v>212</v>
       </c>
@@ -22571,7 +22941,7 @@
       <c r="N194" s="43"/>
     </row>
     <row r="195" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B195" s="129"/>
+      <c r="B195" s="133"/>
       <c r="C195" s="76" t="s">
         <v>177</v>
       </c>
@@ -22610,7 +22980,7 @@
       </c>
     </row>
     <row r="196" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B196" s="129"/>
+      <c r="B196" s="133"/>
       <c r="C196" s="76" t="s">
         <v>178</v>
       </c>
@@ -22649,7 +23019,7 @@
       </c>
     </row>
     <row r="197" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B197" s="129"/>
+      <c r="B197" s="133"/>
       <c r="C197" s="76" t="s">
         <v>179</v>
       </c>
@@ -22688,7 +23058,7 @@
       </c>
     </row>
     <row r="198" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B198" s="129"/>
+      <c r="B198" s="133"/>
       <c r="C198" s="76" t="s">
         <v>180</v>
       </c>
@@ -22727,7 +23097,7 @@
       </c>
     </row>
     <row r="199" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B199" s="129"/>
+      <c r="B199" s="133"/>
       <c r="C199" s="76" t="s">
         <v>181</v>
       </c>
@@ -22766,7 +23136,7 @@
       </c>
     </row>
     <row r="200" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B200" s="129"/>
+      <c r="B200" s="133"/>
       <c r="C200" s="76" t="s">
         <v>182</v>
       </c>
@@ -22805,7 +23175,7 @@
       </c>
     </row>
     <row r="201" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B201" s="129"/>
+      <c r="B201" s="133"/>
       <c r="C201" s="76" t="s">
         <v>183</v>
       </c>
@@ -22844,7 +23214,7 @@
       </c>
     </row>
     <row r="202" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B202" s="129"/>
+      <c r="B202" s="133"/>
       <c r="C202" s="76" t="s">
         <v>184</v>
       </c>
@@ -22883,7 +23253,7 @@
       </c>
     </row>
     <row r="203" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B203" s="129"/>
+      <c r="B203" s="133"/>
       <c r="C203" s="76" t="s">
         <v>185</v>
       </c>
@@ -22922,7 +23292,7 @@
       </c>
     </row>
     <row r="204" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B204" s="129"/>
+      <c r="B204" s="133"/>
       <c r="C204" s="76" t="s">
         <v>186</v>
       </c>
@@ -22961,7 +23331,7 @@
       </c>
     </row>
     <row r="205" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B205" s="129"/>
+      <c r="B205" s="133"/>
       <c r="C205" s="76" t="s">
         <v>187</v>
       </c>
@@ -23000,7 +23370,7 @@
       </c>
     </row>
     <row r="206" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B206" s="129"/>
+      <c r="B206" s="133"/>
       <c r="C206" s="76" t="s">
         <v>188</v>
       </c>
@@ -23039,7 +23409,7 @@
       </c>
     </row>
     <row r="207" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B207" s="129"/>
+      <c r="B207" s="133"/>
       <c r="C207" s="76" t="s">
         <v>189</v>
       </c>
@@ -23078,7 +23448,7 @@
       </c>
     </row>
     <row r="208" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B208" s="129"/>
+      <c r="B208" s="133"/>
       <c r="C208" s="76" t="s">
         <v>190</v>
       </c>
@@ -23117,7 +23487,7 @@
       </c>
     </row>
     <row r="209" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B209" s="129"/>
+      <c r="B209" s="133"/>
       <c r="C209" s="77" t="s">
         <v>213</v>
       </c>
@@ -23134,7 +23504,7 @@
       <c r="N209" s="62"/>
     </row>
     <row r="210" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B210" s="129"/>
+      <c r="B210" s="133"/>
       <c r="C210" s="78" t="s">
         <v>177</v>
       </c>
@@ -23173,7 +23543,7 @@
       </c>
     </row>
     <row r="211" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B211" s="129"/>
+      <c r="B211" s="133"/>
       <c r="C211" s="42" t="s">
         <v>178</v>
       </c>
@@ -23212,7 +23582,7 @@
       </c>
     </row>
     <row r="212" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B212" s="129"/>
+      <c r="B212" s="133"/>
       <c r="C212" s="42" t="s">
         <v>179</v>
       </c>
@@ -23251,7 +23621,7 @@
       </c>
     </row>
     <row r="213" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B213" s="129"/>
+      <c r="B213" s="133"/>
       <c r="C213" s="42" t="s">
         <v>180</v>
       </c>
@@ -23290,7 +23660,7 @@
       </c>
     </row>
     <row r="214" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B214" s="129"/>
+      <c r="B214" s="133"/>
       <c r="C214" s="79" t="s">
         <v>214</v>
       </c>
@@ -23329,7 +23699,7 @@
       </c>
     </row>
     <row r="215" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B215" s="129"/>
+      <c r="B215" s="133"/>
       <c r="C215" s="79" t="s">
         <v>215</v>
       </c>
@@ -23368,7 +23738,7 @@
       </c>
     </row>
     <row r="216" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B216" s="129"/>
+      <c r="B216" s="133"/>
       <c r="C216" s="80" t="s">
         <v>216</v>
       </c>
@@ -23407,7 +23777,7 @@
       </c>
     </row>
     <row r="217" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B217" s="129"/>
+      <c r="B217" s="133"/>
       <c r="C217" s="42" t="s">
         <v>186</v>
       </c>
@@ -23446,7 +23816,7 @@
       </c>
     </row>
     <row r="218" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B218" s="129"/>
+      <c r="B218" s="133"/>
       <c r="C218" s="42" t="s">
         <v>187</v>
       </c>
@@ -23485,7 +23855,7 @@
       </c>
     </row>
     <row r="219" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B219" s="129"/>
+      <c r="B219" s="133"/>
       <c r="C219" s="42" t="s">
         <v>188</v>
       </c>
@@ -23524,7 +23894,7 @@
       </c>
     </row>
     <row r="220" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B220" s="129"/>
+      <c r="B220" s="133"/>
       <c r="C220" s="81" t="s">
         <v>189</v>
       </c>
@@ -23563,7 +23933,7 @@
       </c>
     </row>
     <row r="221" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B221" s="129"/>
+      <c r="B221" s="133"/>
       <c r="C221" s="82" t="s">
         <v>217</v>
       </c>
@@ -23580,7 +23950,7 @@
       <c r="N221" s="62"/>
     </row>
     <row r="222" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B222" s="129"/>
+      <c r="B222" s="133"/>
       <c r="C222" s="78" t="s">
         <v>177</v>
       </c>
@@ -23619,7 +23989,7 @@
       </c>
     </row>
     <row r="223" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B223" s="129"/>
+      <c r="B223" s="133"/>
       <c r="C223" s="42" t="s">
         <v>178</v>
       </c>
@@ -23658,7 +24028,7 @@
       </c>
     </row>
     <row r="224" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="B224" s="129"/>
+      <c r="B224" s="133"/>
       <c r="C224" s="42" t="s">
         <v>179</v>
       </c>
@@ -23697,7 +24067,7 @@
       </c>
     </row>
     <row r="225" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B225" s="130"/>
+      <c r="B225" s="134"/>
       <c r="C225" s="34" t="s">
         <v>180</v>
       </c>
@@ -23751,7 +24121,7 @@
     <mergeCell ref="B10:B37"/>
   </mergeCells>
   <conditionalFormatting sqref="M119:M225 M10:M95">
-    <cfRule type="top10" dxfId="2" priority="2" rank="10"/>
+    <cfRule type="top10" dxfId="2" priority="3" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="M10:M37">
     <cfRule type="top10" dxfId="0" priority="1" rank="1"/>
@@ -23806,16 +24176,16 @@
       <c r="I3"/>
     </row>
     <row r="4" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="141" t="s">
+      <c r="C4" s="148" t="s">
         <v>218</v>
       </c>
-      <c r="D4" s="141"/>
-      <c r="E4" s="141"/>
-      <c r="F4" s="141"/>
-      <c r="G4" s="141"/>
-      <c r="H4" s="141"/>
-      <c r="I4" s="141"/>
-      <c r="J4" s="141"/>
+      <c r="D4" s="148"/>
+      <c r="E4" s="148"/>
+      <c r="F4" s="148"/>
+      <c r="G4" s="148"/>
+      <c r="H4" s="148"/>
+      <c r="I4" s="148"/>
+      <c r="J4" s="148"/>
     </row>
     <row r="5" spans="1:10" ht="104.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="15" t="s">
@@ -24555,20 +24925,20 @@
     <mergeCell ref="C4:J4"/>
   </mergeCells>
   <conditionalFormatting sqref="I6:I55">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>$A6&lt;&gt;$I6</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="7" priority="4">
       <formula>$A6=$I6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6">
-    <cfRule type="expression" dxfId="4" priority="14">
+    <cfRule type="expression" dxfId="6" priority="14">
       <formula>$B8=$J6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7 J9:J55">
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>$B7=$J7</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>